<commit_message>
Fixed remote schematic - try 2
</commit_message>
<xml_diff>
--- a/hardware/Wheelchair Receiver BOM.xlsx
+++ b/hardware/Wheelchair Receiver BOM.xlsx
@@ -294,9 +294,6 @@
     <t>Mom-Off-Mom Rocker, Linear Actuators</t>
   </si>
   <si>
-    <t>Xmega128A1</t>
-  </si>
-  <si>
     <t>401-1298-ND</t>
   </si>
   <si>
@@ -1111,6 +1108,9 @@
   </si>
   <si>
     <t>425-1949-5-ND</t>
+  </si>
+  <si>
+    <t>Xmega64A1</t>
   </si>
 </sst>
 </file>
@@ -2436,8 +2436,8 @@
   </sheetPr>
   <dimension ref="A1:M105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="D100" sqref="D100"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2532,10 +2532,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="42" t="s">
         <v>167</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>168</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>40</v>
@@ -2547,7 +2547,7 @@
         <v>39</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H4" s="23">
         <v>0.03</v>
@@ -2567,10 +2567,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>65</v>
@@ -2582,7 +2582,7 @@
         <v>67</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="H5" s="23">
         <v>0.04</v>
@@ -2605,7 +2605,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>66</v>
@@ -2617,7 +2617,7 @@
         <v>68</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="H6" s="23">
         <v>0.06</v>
@@ -2640,19 +2640,19 @@
         <v>19</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="H7" s="23">
         <v>7.0000000000000007E-2</v>
@@ -2672,22 +2672,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="H8" s="23">
         <v>0.04</v>
@@ -2707,22 +2707,22 @@
         <v>6</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="H9" s="23">
         <v>0.04</v>
@@ -2745,19 +2745,19 @@
         <v>19</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="H10" s="23">
         <v>7.0000000000000007E-2</v>
@@ -2777,22 +2777,22 @@
         <v>8</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="H11" s="23">
         <v>0.04</v>
@@ -2812,22 +2812,22 @@
         <v>9</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="H12" s="23">
         <v>0.04</v>
@@ -2850,19 +2850,19 @@
         <v>19</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="H13" s="23">
         <v>7.0000000000000007E-2</v>
@@ -2882,19 +2882,19 @@
         <v>11</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="D14" s="19" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>134</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>135</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="23">
@@ -2915,22 +2915,22 @@
         <v>12</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D15" s="19" t="s">
+        <v>270</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>323</v>
+      </c>
+      <c r="G15" s="20" t="s">
         <v>271</v>
-      </c>
-      <c r="E15" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F15" s="19" t="s">
-        <v>324</v>
-      </c>
-      <c r="G15" s="20" t="s">
-        <v>272</v>
       </c>
       <c r="H15" s="23">
         <v>0.04</v>
@@ -2950,22 +2950,22 @@
         <v>13</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D16" s="19" t="s">
+        <v>272</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="G16" s="23" t="s">
         <v>273</v>
-      </c>
-      <c r="E16" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="19" t="s">
-        <v>326</v>
-      </c>
-      <c r="G16" s="23" t="s">
-        <v>274</v>
       </c>
       <c r="H16" s="23">
         <v>0.04</v>
@@ -3021,10 +3021,10 @@
         <v>11</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>20</v>
@@ -3058,10 +3058,10 @@
         <v>19</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>20</v>
@@ -3070,7 +3070,7 @@
         <v>30</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="H20" s="17">
         <v>0.21</v>
@@ -3095,7 +3095,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>42</v>
@@ -3130,7 +3130,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="42" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>44</v>
@@ -3165,7 +3165,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>47</v>
@@ -3200,7 +3200,7 @@
         <v>18</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>50</v>
@@ -3235,7 +3235,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>56</v>
@@ -3270,7 +3270,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>55</v>
@@ -3305,7 +3305,7 @@
         <v>18</v>
       </c>
       <c r="C27" s="42" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>59</v>
@@ -3340,7 +3340,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>63</v>
@@ -3372,22 +3372,22 @@
         <v>11</v>
       </c>
       <c r="B29" s="19" t="s">
+        <v>190</v>
+      </c>
+      <c r="C29" s="46" t="s">
         <v>191</v>
       </c>
-      <c r="C29" s="46" t="s">
-        <v>192</v>
-      </c>
       <c r="D29" s="31" t="s">
+        <v>124</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="31" t="s">
         <v>125</v>
       </c>
-      <c r="E29" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="31" t="s">
-        <v>126</v>
-      </c>
       <c r="G29" s="31" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="H29" s="32">
         <v>0.05</v>
@@ -3407,22 +3407,22 @@
         <v>12</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E30" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F30" s="31" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="H30" s="32">
         <v>0.3</v>
@@ -3442,22 +3442,22 @@
         <v>13</v>
       </c>
       <c r="B31" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="C31" s="45" t="s">
         <v>320</v>
       </c>
-      <c r="C31" s="45" t="s">
-        <v>321</v>
-      </c>
       <c r="D31" s="19" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="E31" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G31" s="19" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="H31" s="23">
         <v>0.56499999999999995</v>
@@ -3480,19 +3480,19 @@
         <v>18</v>
       </c>
       <c r="C32" s="45" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D32" s="19" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E32" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="G32" s="19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H32" s="23">
         <v>0.39</v>
@@ -3545,10 +3545,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="19" t="s">
+        <v>193</v>
+      </c>
+      <c r="C35" s="42" t="s">
         <v>194</v>
-      </c>
-      <c r="C35" s="42" t="s">
-        <v>195</v>
       </c>
       <c r="D35" s="21" t="s">
         <v>26</v>
@@ -3580,10 +3580,10 @@
         <v>2</v>
       </c>
       <c r="B36" s="19" t="s">
+        <v>198</v>
+      </c>
+      <c r="C36" s="42" t="s">
         <v>199</v>
-      </c>
-      <c r="C36" s="42" t="s">
-        <v>200</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>77</v>
@@ -3615,10 +3615,10 @@
         <v>3</v>
       </c>
       <c r="B37" s="19" t="s">
+        <v>196</v>
+      </c>
+      <c r="C37" s="46" t="s">
         <v>197</v>
-      </c>
-      <c r="C37" s="46" t="s">
-        <v>198</v>
       </c>
       <c r="D37" s="36" t="s">
         <v>82</v>
@@ -3630,7 +3630,7 @@
         <v>81</v>
       </c>
       <c r="G37" s="19" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="H37" s="32">
         <v>5.08</v>
@@ -3650,22 +3650,22 @@
         <v>4</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C38" s="42" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>89</v>
+        <v>361</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>85</v>
       </c>
       <c r="F38" s="31" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="G38" s="19" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="H38" s="32">
         <v>7.53</v>
@@ -3685,22 +3685,22 @@
         <v>5</v>
       </c>
       <c r="B39" s="19" t="s">
+        <v>285</v>
+      </c>
+      <c r="C39" s="42" t="s">
+        <v>287</v>
+      </c>
+      <c r="D39" s="19" t="s">
         <v>286</v>
       </c>
-      <c r="C39" s="42" t="s">
-        <v>288</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>287</v>
-      </c>
       <c r="E39" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G39" s="19" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H39" s="23">
         <v>5.63</v>
@@ -3753,13 +3753,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="15" t="s">
+        <v>201</v>
+      </c>
+      <c r="C42" s="43" t="s">
         <v>202</v>
       </c>
-      <c r="C42" s="43" t="s">
-        <v>203</v>
-      </c>
       <c r="D42" s="18" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>20</v>
@@ -3768,7 +3768,7 @@
         <v>21</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H42" s="17">
         <v>0.49</v>
@@ -3788,10 +3788,10 @@
         <v>2</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C43" s="49" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>23</v>
@@ -3803,7 +3803,7 @@
         <v>22</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H43" s="17">
         <v>0.74</v>
@@ -3823,13 +3823,13 @@
         <v>3</v>
       </c>
       <c r="B44" s="19" t="s">
+        <v>206</v>
+      </c>
+      <c r="C44" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="C44" s="44" t="s">
-        <v>208</v>
-      </c>
       <c r="D44" s="21" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E44" s="15" t="s">
         <v>20</v>
@@ -3858,13 +3858,13 @@
         <v>4</v>
       </c>
       <c r="B45" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="C45" s="44" t="s">
         <v>209</v>
       </c>
-      <c r="C45" s="44" t="s">
-        <v>210</v>
-      </c>
       <c r="D45" s="18" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E45" s="15" t="s">
         <v>20</v>
@@ -3873,7 +3873,7 @@
         <v>28</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="H45" s="17">
         <v>0.42</v>
@@ -3893,10 +3893,10 @@
         <v>5</v>
       </c>
       <c r="B46" s="19" t="s">
+        <v>210</v>
+      </c>
+      <c r="C46" s="48" t="s">
         <v>211</v>
-      </c>
-      <c r="C46" s="48" t="s">
-        <v>212</v>
       </c>
       <c r="D46" s="21" t="s">
         <v>37</v>
@@ -3928,22 +3928,22 @@
         <v>6</v>
       </c>
       <c r="B47" s="19" t="s">
+        <v>212</v>
+      </c>
+      <c r="C47" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="C47" s="45" t="s">
-        <v>214</v>
-      </c>
       <c r="D47" s="19" t="s">
+        <v>98</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="E47" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>100</v>
-      </c>
       <c r="G47" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="H47" s="23">
         <v>0.39</v>
@@ -3963,22 +3963,22 @@
         <v>7</v>
       </c>
       <c r="B48" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="C48" s="42" t="s">
         <v>215</v>
       </c>
-      <c r="C48" s="42" t="s">
-        <v>216</v>
-      </c>
       <c r="D48" s="19" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="E48" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G48" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="H48" s="23">
         <v>1.05</v>
@@ -3998,10 +3998,10 @@
         <v>8</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D49" s="19" t="s">
         <v>69</v>
@@ -4013,7 +4013,7 @@
         <v>70</v>
       </c>
       <c r="G49" s="19" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="H49" s="23">
         <v>0.05</v>
@@ -4033,10 +4033,10 @@
         <v>9</v>
       </c>
       <c r="B50" s="19" t="s">
+        <v>217</v>
+      </c>
+      <c r="C50" s="42" t="s">
         <v>218</v>
-      </c>
-      <c r="C50" s="42" t="s">
-        <v>219</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>71</v>
@@ -4048,7 +4048,7 @@
         <v>72</v>
       </c>
       <c r="G50" s="19" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="H50" s="23">
         <v>0.05</v>
@@ -4068,10 +4068,10 @@
         <v>10</v>
       </c>
       <c r="B51" s="19" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C51" s="42" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D51" s="19" t="s">
         <v>73</v>
@@ -4083,7 +4083,7 @@
         <v>74</v>
       </c>
       <c r="G51" s="19" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H51" s="23">
         <v>0.05</v>
@@ -4103,10 +4103,10 @@
         <v>11</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C52" s="45" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D52" s="19" t="s">
         <v>80</v>
@@ -4118,7 +4118,7 @@
         <v>79</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="H52" s="23">
         <v>2.36</v>
@@ -4138,19 +4138,19 @@
         <v>12</v>
       </c>
       <c r="B53" s="19" t="s">
+        <v>203</v>
+      </c>
+      <c r="C53" s="42" t="s">
         <v>204</v>
       </c>
-      <c r="C53" s="42" t="s">
-        <v>205</v>
-      </c>
       <c r="D53" s="19" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E53" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G53" s="19"/>
       <c r="H53" s="23">
@@ -4171,22 +4171,22 @@
         <v>13</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E54" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G54" s="19" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="H54" s="23">
         <v>0.49</v>
@@ -4206,22 +4206,22 @@
         <v>14</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C55" s="42" t="s">
+        <v>298</v>
+      </c>
+      <c r="D55" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="G55" s="19" t="s">
         <v>299</v>
-      </c>
-      <c r="D55" s="19" t="s">
-        <v>298</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F55" s="19" t="s">
-        <v>268</v>
-      </c>
-      <c r="G55" s="19" t="s">
-        <v>300</v>
       </c>
       <c r="H55" s="23">
         <v>1</v>
@@ -4241,22 +4241,22 @@
         <v>15</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C56" s="45" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="D56" s="19" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E56" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H56" s="23">
         <v>0.38</v>
@@ -4276,22 +4276,22 @@
         <v>16</v>
       </c>
       <c r="B57" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C57" s="42" t="s">
         <v>306</v>
       </c>
-      <c r="C57" s="42" t="s">
-        <v>307</v>
-      </c>
       <c r="D57" s="19" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E57" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="H57" s="23">
         <v>0.56999999999999995</v>
@@ -4311,22 +4311,22 @@
         <v>17</v>
       </c>
       <c r="B58" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="C58" s="45" t="s">
         <v>311</v>
       </c>
-      <c r="C58" s="45" t="s">
-        <v>312</v>
-      </c>
       <c r="D58" s="19" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E58" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G58" s="19" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="H58" s="23">
         <v>0.38</v>
@@ -4346,22 +4346,22 @@
         <v>18</v>
       </c>
       <c r="B59" s="19" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="C59" s="45" t="s">
+        <v>312</v>
+      </c>
+      <c r="D59" s="19" t="s">
         <v>313</v>
       </c>
-      <c r="D59" s="19" t="s">
-        <v>314</v>
-      </c>
       <c r="E59" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="G59" s="19" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="H59" s="23">
         <v>0.33</v>
@@ -4381,19 +4381,19 @@
         <v>19</v>
       </c>
       <c r="B60" s="31" t="s">
+        <v>338</v>
+      </c>
+      <c r="C60" s="46" t="s">
         <v>339</v>
       </c>
-      <c r="C60" s="46" t="s">
+      <c r="D60" s="31" t="s">
         <v>340</v>
       </c>
-      <c r="D60" s="31" t="s">
-        <v>341</v>
-      </c>
       <c r="E60" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F60" s="31" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="G60" s="31"/>
       <c r="H60" s="32">
@@ -4414,19 +4414,19 @@
         <v>20</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C61" s="46" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E61" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F61" s="31" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="G61" s="31"/>
       <c r="H61" s="32">
@@ -4481,19 +4481,19 @@
         <v>1</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C64" s="41" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D64" s="19" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E64" s="19" t="s">
         <v>85</v>
       </c>
       <c r="F64" s="19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G64" s="19"/>
       <c r="H64" s="23">
@@ -4514,7 +4514,7 @@
         <v>2</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C65" s="41" t="s">
         <v>86</v>
@@ -4547,10 +4547,10 @@
         <v>3</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C66" s="41" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="D66" s="31" t="s">
         <v>88</v>
@@ -4580,19 +4580,19 @@
         <v>4</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C67" s="41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D67" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E67" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F67" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G67" s="31"/>
       <c r="H67" s="32">
@@ -4613,19 +4613,19 @@
         <v>5</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C68" s="46" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="D68" s="31" t="s">
+        <v>91</v>
+      </c>
+      <c r="E68" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" s="31" t="s">
         <v>92</v>
-      </c>
-      <c r="E68" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F68" s="31" t="s">
-        <v>93</v>
       </c>
       <c r="G68" s="31"/>
       <c r="H68" s="32">
@@ -4646,19 +4646,19 @@
         <v>6</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C69" s="41" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E69" s="31" t="s">
         <v>85</v>
       </c>
       <c r="F69" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G69" s="31"/>
       <c r="H69" s="32">
@@ -4679,19 +4679,19 @@
         <v>7</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C70" s="41" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E70" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F70" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G70" s="31"/>
       <c r="H70" s="32">
@@ -4712,19 +4712,19 @@
         <v>8</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C71" s="41" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D71" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E71" s="31" t="s">
         <v>85</v>
       </c>
       <c r="F71" s="31" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="G71" s="31"/>
       <c r="H71" s="32">
@@ -4745,19 +4745,19 @@
         <v>9</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C72" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D72" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E72" s="31" t="s">
         <v>85</v>
       </c>
       <c r="F72" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G72" s="31"/>
       <c r="H72" s="32">
@@ -4778,19 +4778,19 @@
         <v>10</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C73" s="41" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D73" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E73" s="31" t="s">
         <v>85</v>
       </c>
       <c r="F73" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G73" s="31"/>
       <c r="H73" s="32">
@@ -4811,19 +4811,19 @@
         <v>11</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C74" s="41" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D74" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E74" s="31" t="s">
         <v>85</v>
       </c>
       <c r="F74" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G74" s="31"/>
       <c r="H74" s="32">
@@ -4844,19 +4844,19 @@
         <v>12</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C75" s="47" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="D75" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E75" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F75" s="31" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G75" s="31"/>
       <c r="H75" s="32">
@@ -4877,19 +4877,19 @@
         <v>13</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C76" s="47" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D76" s="19" t="s">
+        <v>160</v>
+      </c>
+      <c r="E76" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" s="31" t="s">
         <v>161</v>
-      </c>
-      <c r="E76" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F76" s="31" t="s">
-        <v>162</v>
       </c>
       <c r="G76" s="31"/>
       <c r="H76" s="32">
@@ -4910,19 +4910,19 @@
         <v>14</v>
       </c>
       <c r="B77" s="19" t="s">
+        <v>242</v>
+      </c>
+      <c r="C77" s="47" t="s">
         <v>243</v>
       </c>
-      <c r="C77" s="47" t="s">
-        <v>244</v>
-      </c>
       <c r="D77" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E77" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F77" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G77" s="31"/>
       <c r="H77" s="32">
@@ -4943,19 +4943,19 @@
         <v>15</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C78" s="41" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D78" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E78" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F78" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G78" s="31"/>
       <c r="H78" s="32">
@@ -4976,19 +4976,19 @@
         <v>16</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C79" s="46" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D79" s="31" t="s">
+        <v>118</v>
+      </c>
+      <c r="E79" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" s="31" t="s">
         <v>119</v>
-      </c>
-      <c r="E79" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F79" s="31" t="s">
-        <v>120</v>
       </c>
       <c r="G79" s="31"/>
       <c r="H79" s="32">
@@ -5009,19 +5009,19 @@
         <v>17</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C80" s="46" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D80" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E80" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F80" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G80" s="31"/>
       <c r="H80" s="32">
@@ -5042,19 +5042,19 @@
         <v>18</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C81" s="41" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D81" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E81" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F81" s="31" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G81" s="31"/>
       <c r="H81" s="32">
@@ -5078,16 +5078,16 @@
         <v>17</v>
       </c>
       <c r="C82" s="41" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="D82" s="31" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E82" s="19" t="s">
         <v>85</v>
       </c>
       <c r="F82" s="31" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="G82" s="31"/>
       <c r="H82" s="32">
@@ -5108,19 +5108,19 @@
         <v>20</v>
       </c>
       <c r="B83" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C83" s="41" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="D83" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E83" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G83" s="31"/>
       <c r="H83" s="32">
@@ -5141,19 +5141,19 @@
         <v>21</v>
       </c>
       <c r="B84" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C84" s="42" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="D84" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E84" s="19" t="s">
         <v>85</v>
       </c>
       <c r="F84" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G84" s="19"/>
       <c r="H84" s="23">
@@ -5174,19 +5174,19 @@
         <v>22</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C85" s="45" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D85" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E85" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G85" s="19"/>
       <c r="H85" s="23">
@@ -5207,19 +5207,19 @@
         <v>23</v>
       </c>
       <c r="B86" s="19" t="s">
+        <v>222</v>
+      </c>
+      <c r="C86" s="42" t="s">
         <v>223</v>
       </c>
-      <c r="C86" s="42" t="s">
-        <v>224</v>
-      </c>
       <c r="D86" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E86" s="19" t="s">
         <v>85</v>
       </c>
       <c r="F86" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G86" s="19"/>
       <c r="H86" s="23">
@@ -5241,16 +5241,16 @@
       </c>
       <c r="B87" s="31"/>
       <c r="C87" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D87" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E87" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F87" s="31" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G87" s="31"/>
       <c r="H87" s="32">
@@ -5265,7 +5265,7 @@
         <v>10.649999999999999</v>
       </c>
       <c r="K87" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="88" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5275,16 +5275,16 @@
       </c>
       <c r="B88" s="19"/>
       <c r="C88" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="E88" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G88" s="19"/>
       <c r="H88" s="32">
@@ -5299,7 +5299,7 @@
         <v>10.649999999999999</v>
       </c>
       <c r="K88" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="89" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5309,16 +5309,16 @@
       </c>
       <c r="B89" s="19"/>
       <c r="C89" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D89" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E89" s="19" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F89" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G89" s="19"/>
       <c r="H89" s="23">
@@ -5333,7 +5333,7 @@
         <v>11.435</v>
       </c>
       <c r="K89" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="90" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5343,16 +5343,16 @@
       </c>
       <c r="B90" s="19"/>
       <c r="C90" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D90" s="19" t="s">
+        <v>163</v>
+      </c>
+      <c r="E90" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F90" s="19" t="s">
         <v>164</v>
-      </c>
-      <c r="E90" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="F90" s="19" t="s">
-        <v>165</v>
       </c>
       <c r="G90" s="19"/>
       <c r="H90" s="23">
@@ -5367,7 +5367,7 @@
         <v>11.435</v>
       </c>
       <c r="K90" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="91" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5377,16 +5377,16 @@
       </c>
       <c r="B91" s="19"/>
       <c r="C91" s="19" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D91" s="19" t="s">
+        <v>349</v>
+      </c>
+      <c r="E91" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="F91" s="19" t="s">
         <v>350</v>
-      </c>
-      <c r="E91" s="19" t="s">
-        <v>150</v>
-      </c>
-      <c r="F91" s="19" t="s">
-        <v>351</v>
       </c>
       <c r="G91" s="19"/>
       <c r="H91" s="23">
@@ -5400,7 +5400,7 @@
         <v>11.434999999999999</v>
       </c>
       <c r="K91" s="21" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="92" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5409,19 +5409,19 @@
         <v>29</v>
       </c>
       <c r="B92" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C92" s="45" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D92" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="E92" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="G92" s="19"/>
       <c r="H92" s="23">
@@ -5446,19 +5446,19 @@
         <v>30</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C93" s="45" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D93" s="19" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="E93" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F93" s="19" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="G93" s="19"/>
       <c r="H93" s="23">
@@ -5472,7 +5472,7 @@
         <v>0.65</v>
       </c>
       <c r="K93" s="21" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="94" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5481,19 +5481,19 @@
         <v>31</v>
       </c>
       <c r="B94" s="19" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C94" s="45" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D94" s="19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="E94" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F94" s="19" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="G94" s="19"/>
       <c r="H94" s="23">
@@ -5507,7 +5507,7 @@
         <v>0.53</v>
       </c>
       <c r="K94" s="21" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
     </row>
     <row r="95" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5516,19 +5516,19 @@
         <v>32</v>
       </c>
       <c r="B95" s="19" t="s">
+        <v>330</v>
+      </c>
+      <c r="C95" s="45" t="s">
         <v>331</v>
       </c>
-      <c r="C95" s="45" t="s">
-        <v>332</v>
-      </c>
       <c r="D95" s="19" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="E95" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F95" s="19" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G95" s="19"/>
       <c r="H95" s="23">
@@ -5566,7 +5566,7 @@
       <c r="A99" s="1"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E99" s="3"/>
     </row>
@@ -5574,70 +5574,70 @@
       <c r="A100" s="1"/>
       <c r="C100" s="3"/>
       <c r="D100" t="s">
+        <v>353</v>
+      </c>
+      <c r="E100" t="s">
+        <v>20</v>
+      </c>
+      <c r="F100" t="s">
         <v>354</v>
-      </c>
-      <c r="E100" t="s">
-        <v>20</v>
-      </c>
-      <c r="F100" t="s">
-        <v>355</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="E101" t="s">
+        <v>20</v>
+      </c>
+      <c r="F101" t="s">
         <v>356</v>
-      </c>
-      <c r="E101" t="s">
-        <v>20</v>
-      </c>
-      <c r="F101" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D102" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E102" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F102" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D103" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F103" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D104" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F104" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D105" s="3" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F105" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor fixes in wheelchair schematic
</commit_message>
<xml_diff>
--- a/hardware/Wheelchair Receiver BOM.xlsx
+++ b/hardware/Wheelchair Receiver BOM.xlsx
@@ -252,9 +252,6 @@
     <t>712-1420-1-ND</t>
   </si>
   <si>
-    <t>Newark</t>
-  </si>
-  <si>
     <t>42M2397</t>
   </si>
   <si>
@@ -624,9 +621,6 @@
     <t>Nordic Semiconductor</t>
   </si>
   <si>
-    <t>NRF24L01G</t>
-  </si>
-  <si>
     <t>Atmel</t>
   </si>
   <si>
@@ -1111,6 +1105,12 @@
   </si>
   <si>
     <t>Xmega64A1</t>
+  </si>
+  <si>
+    <t>NRF24L01</t>
+  </si>
+  <si>
+    <t>Newark or Sparkfun or Mouser</t>
   </si>
 </sst>
 </file>
@@ -2446,7 +2446,7 @@
     <col min="2" max="2" width="21.7109375" customWidth="1"/>
     <col min="3" max="3" width="24.7109375" customWidth="1"/>
     <col min="4" max="4" width="36.140625" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24" customWidth="1"/>
     <col min="7" max="7" width="11.5703125" customWidth="1"/>
     <col min="8" max="8" width="10" bestFit="1" customWidth="1"/>
@@ -2469,7 +2469,7 @@
       </c>
       <c r="J1" s="29">
         <f>SUM(Table2[Sub Total])</f>
-        <v>398.82999999999993</v>
+        <v>398.79999999999995</v>
       </c>
       <c r="K1" s="5"/>
     </row>
@@ -2532,10 +2532,10 @@
         <v>1</v>
       </c>
       <c r="B4" s="19" t="s">
+        <v>165</v>
+      </c>
+      <c r="C4" s="42" t="s">
         <v>166</v>
-      </c>
-      <c r="C4" s="42" t="s">
-        <v>167</v>
       </c>
       <c r="D4" s="19" t="s">
         <v>40</v>
@@ -2547,7 +2547,7 @@
         <v>39</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="H4" s="23">
         <v>0.03</v>
@@ -2567,10 +2567,10 @@
         <v>2</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D5" s="19" t="s">
         <v>65</v>
@@ -2582,7 +2582,7 @@
         <v>67</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="H5" s="23">
         <v>0.04</v>
@@ -2605,7 +2605,7 @@
         <v>19</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>66</v>
@@ -2617,7 +2617,7 @@
         <v>68</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="H6" s="23">
         <v>0.06</v>
@@ -2640,19 +2640,19 @@
         <v>19</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="19" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
       <c r="H7" s="23">
         <v>7.0000000000000007E-2</v>
@@ -2672,22 +2672,22 @@
         <v>5</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C8" s="43" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E8" s="15" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G8" s="16" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
       <c r="H8" s="23">
         <v>0.04</v>
@@ -2707,22 +2707,22 @@
         <v>6</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C9" s="42" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E9" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="19" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G9" s="20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="H9" s="23">
         <v>0.04</v>
@@ -2745,19 +2745,19 @@
         <v>19</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E10" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G10" s="20" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
       <c r="H10" s="23">
         <v>7.0000000000000007E-2</v>
@@ -2777,22 +2777,22 @@
         <v>8</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E11" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F11" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G11" s="20" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
       <c r="H11" s="23">
         <v>0.04</v>
@@ -2812,22 +2812,22 @@
         <v>9</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F12" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G12" s="20" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
       <c r="H12" s="23">
         <v>0.04</v>
@@ -2850,19 +2850,19 @@
         <v>19</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E13" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F13" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G13" s="20" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
       <c r="H13" s="23">
         <v>7.0000000000000007E-2</v>
@@ -2882,19 +2882,19 @@
         <v>11</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C14" s="42" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D14" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F14" s="19" t="s">
         <v>133</v>
-      </c>
-      <c r="E14" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="19" t="s">
-        <v>134</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="23">
@@ -2915,22 +2915,22 @@
         <v>12</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="E15" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="G15" s="20" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="H15" s="23">
         <v>0.04</v>
@@ -2950,22 +2950,22 @@
         <v>13</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="E16" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="G16" s="23" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="H16" s="23">
         <v>0.04</v>
@@ -3021,10 +3021,10 @@
         <v>11</v>
       </c>
       <c r="C19" s="48" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E19" s="15" t="s">
         <v>20</v>
@@ -3058,10 +3058,10 @@
         <v>19</v>
       </c>
       <c r="C20" s="44" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E20" s="15" t="s">
         <v>20</v>
@@ -3070,7 +3070,7 @@
         <v>30</v>
       </c>
       <c r="G20" s="15" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="H20" s="17">
         <v>0.21</v>
@@ -3095,7 +3095,7 @@
         <v>18</v>
       </c>
       <c r="C21" s="43" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D21" s="15" t="s">
         <v>42</v>
@@ -3130,7 +3130,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="42" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D22" s="19" t="s">
         <v>44</v>
@@ -3165,7 +3165,7 @@
         <v>18</v>
       </c>
       <c r="C23" s="42" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="D23" s="19" t="s">
         <v>47</v>
@@ -3200,7 +3200,7 @@
         <v>18</v>
       </c>
       <c r="C24" s="42" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D24" s="19" t="s">
         <v>50</v>
@@ -3235,7 +3235,7 @@
         <v>18</v>
       </c>
       <c r="C25" s="42" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="D25" s="19" t="s">
         <v>56</v>
@@ -3270,7 +3270,7 @@
         <v>18</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D26" s="19" t="s">
         <v>55</v>
@@ -3305,7 +3305,7 @@
         <v>18</v>
       </c>
       <c r="C27" s="42" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D27" s="19" t="s">
         <v>59</v>
@@ -3340,7 +3340,7 @@
         <v>16</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D28" s="19" t="s">
         <v>63</v>
@@ -3372,22 +3372,22 @@
         <v>11</v>
       </c>
       <c r="B29" s="19" t="s">
+        <v>189</v>
+      </c>
+      <c r="C29" s="46" t="s">
         <v>190</v>
       </c>
-      <c r="C29" s="46" t="s">
-        <v>191</v>
-      </c>
       <c r="D29" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="E29" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F29" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="E29" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F29" s="31" t="s">
-        <v>125</v>
-      </c>
       <c r="G29" s="31" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="H29" s="32">
         <v>0.05</v>
@@ -3407,22 +3407,22 @@
         <v>12</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D30" s="31" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E30" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F30" s="31" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G30" s="19" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="H30" s="32">
         <v>0.3</v>
@@ -3442,22 +3442,22 @@
         <v>13</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C31" s="45" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D31" s="19" t="s">
+        <v>277</v>
+      </c>
+      <c r="E31" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>316</v>
+      </c>
+      <c r="G31" s="19" t="s">
         <v>279</v>
-      </c>
-      <c r="E31" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F31" s="19" t="s">
-        <v>318</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>281</v>
       </c>
       <c r="H31" s="23">
         <v>0.56499999999999995</v>
@@ -3480,19 +3480,19 @@
         <v>18</v>
       </c>
       <c r="C32" s="45" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D32" s="19" t="s">
+        <v>278</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>319</v>
+      </c>
+      <c r="G32" s="19" t="s">
         <v>280</v>
-      </c>
-      <c r="E32" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F32" s="19" t="s">
-        <v>321</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>282</v>
       </c>
       <c r="H32" s="23">
         <v>0.39</v>
@@ -3545,10 +3545,10 @@
         <v>1</v>
       </c>
       <c r="B35" s="19" t="s">
+        <v>192</v>
+      </c>
+      <c r="C35" s="42" t="s">
         <v>193</v>
-      </c>
-      <c r="C35" s="42" t="s">
-        <v>194</v>
       </c>
       <c r="D35" s="21" t="s">
         <v>26</v>
@@ -3574,28 +3574,28 @@
       </c>
       <c r="K35" s="21"/>
     </row>
-    <row r="36" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A36" s="24">
         <f>1+A35</f>
         <v>2</v>
       </c>
       <c r="B36" s="19" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C36" s="42" t="s">
-        <v>199</v>
+        <v>360</v>
       </c>
       <c r="D36" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E36" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="G36" s="19" t="s">
         <v>77</v>
-      </c>
-      <c r="E36" s="19" t="s">
-        <v>75</v>
-      </c>
-      <c r="F36" s="19" t="s">
-        <v>76</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>78</v>
       </c>
       <c r="H36" s="23">
         <v>5.24</v>
@@ -3615,22 +3615,22 @@
         <v>3</v>
       </c>
       <c r="B37" s="19" t="s">
+        <v>195</v>
+      </c>
+      <c r="C37" s="46" t="s">
         <v>196</v>
       </c>
-      <c r="C37" s="46" t="s">
-        <v>197</v>
-      </c>
       <c r="D37" s="36" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E37" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F37" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="G37" s="19" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="H37" s="32">
         <v>5.08</v>
@@ -3650,32 +3650,32 @@
         <v>4</v>
       </c>
       <c r="B38" s="19" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="C38" s="42" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="E38" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F38" s="31" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="G38" s="19" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="H38" s="32">
-        <v>7.53</v>
+        <v>7.5</v>
       </c>
       <c r="I38" s="40">
         <v>1</v>
       </c>
       <c r="J38" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>7.53</v>
+        <v>7.5</v>
       </c>
       <c r="K38" s="35"/>
     </row>
@@ -3685,22 +3685,22 @@
         <v>5</v>
       </c>
       <c r="B39" s="19" t="s">
+        <v>283</v>
+      </c>
+      <c r="C39" s="42" t="s">
         <v>285</v>
       </c>
-      <c r="C39" s="42" t="s">
-        <v>287</v>
-      </c>
       <c r="D39" s="19" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="E39" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="G39" s="19" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="H39" s="23">
         <v>5.63</v>
@@ -3753,13 +3753,13 @@
         <v>1</v>
       </c>
       <c r="B42" s="15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C42" s="43" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E42" s="15" t="s">
         <v>20</v>
@@ -3768,7 +3768,7 @@
         <v>21</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="H42" s="17">
         <v>0.49</v>
@@ -3788,10 +3788,10 @@
         <v>2</v>
       </c>
       <c r="B43" s="15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C43" s="49" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D43" s="18" t="s">
         <v>23</v>
@@ -3803,7 +3803,7 @@
         <v>22</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="H43" s="17">
         <v>0.74</v>
@@ -3823,13 +3823,13 @@
         <v>3</v>
       </c>
       <c r="B44" s="19" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C44" s="44" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D44" s="21" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="E44" s="15" t="s">
         <v>20</v>
@@ -3858,13 +3858,13 @@
         <v>4</v>
       </c>
       <c r="B45" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C45" s="44" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="E45" s="15" t="s">
         <v>20</v>
@@ -3873,7 +3873,7 @@
         <v>28</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="H45" s="17">
         <v>0.42</v>
@@ -3893,10 +3893,10 @@
         <v>5</v>
       </c>
       <c r="B46" s="19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C46" s="48" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D46" s="21" t="s">
         <v>37</v>
@@ -3928,22 +3928,22 @@
         <v>6</v>
       </c>
       <c r="B47" s="19" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C47" s="45" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="D47" s="19" t="s">
+        <v>97</v>
+      </c>
+      <c r="E47" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="E47" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" s="19" t="s">
-        <v>99</v>
-      </c>
       <c r="G47" s="19" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="H47" s="23">
         <v>0.39</v>
@@ -3963,22 +3963,22 @@
         <v>7</v>
       </c>
       <c r="B48" s="19" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C48" s="42" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="D48" s="19" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E48" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F48" s="19" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G48" s="19" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="H48" s="23">
         <v>1.05</v>
@@ -3998,10 +3998,10 @@
         <v>8</v>
       </c>
       <c r="B49" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C49" s="42" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="D49" s="19" t="s">
         <v>69</v>
@@ -4013,7 +4013,7 @@
         <v>70</v>
       </c>
       <c r="G49" s="19" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
       <c r="H49" s="23">
         <v>0.05</v>
@@ -4033,10 +4033,10 @@
         <v>9</v>
       </c>
       <c r="B50" s="19" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C50" s="42" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="D50" s="19" t="s">
         <v>71</v>
@@ -4048,7 +4048,7 @@
         <v>72</v>
       </c>
       <c r="G50" s="19" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
       <c r="H50" s="23">
         <v>0.05</v>
@@ -4068,10 +4068,10 @@
         <v>10</v>
       </c>
       <c r="B51" s="19" t="s">
+        <v>215</v>
+      </c>
+      <c r="C51" s="42" t="s">
         <v>217</v>
-      </c>
-      <c r="C51" s="42" t="s">
-        <v>219</v>
       </c>
       <c r="D51" s="19" t="s">
         <v>73</v>
@@ -4083,7 +4083,7 @@
         <v>74</v>
       </c>
       <c r="G51" s="19" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="H51" s="23">
         <v>0.05</v>
@@ -4103,22 +4103,22 @@
         <v>11</v>
       </c>
       <c r="B52" s="19" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C52" s="45" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="D52" s="19" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E52" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="G52" s="19" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
       <c r="H52" s="23">
         <v>2.36</v>
@@ -4138,19 +4138,19 @@
         <v>12</v>
       </c>
       <c r="B53" s="19" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C53" s="42" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D53" s="19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E53" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="G53" s="19"/>
       <c r="H53" s="23">
@@ -4171,22 +4171,22 @@
         <v>13</v>
       </c>
       <c r="B54" s="19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="E54" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="G54" s="19" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="H54" s="23">
         <v>0.49</v>
@@ -4206,22 +4206,22 @@
         <v>14</v>
       </c>
       <c r="B55" s="19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C55" s="42" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D55" s="19" t="s">
+        <v>295</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>265</v>
+      </c>
+      <c r="G55" s="19" t="s">
         <v>297</v>
-      </c>
-      <c r="E55" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F55" s="19" t="s">
-        <v>267</v>
-      </c>
-      <c r="G55" s="19" t="s">
-        <v>299</v>
       </c>
       <c r="H55" s="23">
         <v>1</v>
@@ -4241,22 +4241,22 @@
         <v>15</v>
       </c>
       <c r="B56" s="19" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C56" s="45" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D56" s="19" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="E56" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F56" s="19" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="H56" s="23">
         <v>0.38</v>
@@ -4276,22 +4276,22 @@
         <v>16</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="C57" s="42" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D57" s="19" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="E57" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F57" s="19" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="H57" s="23">
         <v>0.56999999999999995</v>
@@ -4311,22 +4311,22 @@
         <v>17</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="C58" s="45" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D58" s="19" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="E58" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F58" s="19" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="G58" s="19" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="H58" s="23">
         <v>0.38</v>
@@ -4346,22 +4346,22 @@
         <v>18</v>
       </c>
       <c r="B59" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="C59" s="45" t="s">
         <v>310</v>
       </c>
-      <c r="C59" s="45" t="s">
-        <v>312</v>
-      </c>
       <c r="D59" s="19" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="E59" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F59" s="19" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="G59" s="19" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="H59" s="23">
         <v>0.33</v>
@@ -4381,19 +4381,19 @@
         <v>19</v>
       </c>
       <c r="B60" s="31" t="s">
+        <v>336</v>
+      </c>
+      <c r="C60" s="46" t="s">
+        <v>337</v>
+      </c>
+      <c r="D60" s="31" t="s">
         <v>338</v>
       </c>
-      <c r="C60" s="46" t="s">
-        <v>339</v>
-      </c>
-      <c r="D60" s="31" t="s">
-        <v>340</v>
-      </c>
       <c r="E60" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F60" s="31" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="G60" s="31"/>
       <c r="H60" s="32">
@@ -4414,19 +4414,19 @@
         <v>20</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C61" s="46" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="E61" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F61" s="31" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="G61" s="31"/>
       <c r="H61" s="32">
@@ -4459,7 +4459,7 @@
     </row>
     <row r="63" spans="1:11" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A63" s="30" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B63" s="37"/>
       <c r="C63" s="37"/>
@@ -4481,19 +4481,19 @@
         <v>1</v>
       </c>
       <c r="B64" s="19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C64" s="41" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="D64" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F64" s="19" t="s">
         <v>101</v>
-      </c>
-      <c r="E64" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F64" s="19" t="s">
-        <v>102</v>
       </c>
       <c r="G64" s="19"/>
       <c r="H64" s="23">
@@ -4514,19 +4514,19 @@
         <v>2</v>
       </c>
       <c r="B65" s="19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C65" s="41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D65" s="31" t="s">
+        <v>83</v>
+      </c>
+      <c r="E65" s="31" t="s">
         <v>84</v>
       </c>
-      <c r="E65" s="31" t="s">
+      <c r="F65" s="31" t="s">
         <v>85</v>
-      </c>
-      <c r="F65" s="31" t="s">
-        <v>86</v>
       </c>
       <c r="G65" s="31"/>
       <c r="H65" s="32">
@@ -4547,19 +4547,19 @@
         <v>3</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C66" s="41" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D66" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E66" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F66" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="G66" s="31"/>
       <c r="H66" s="32">
@@ -4580,19 +4580,19 @@
         <v>4</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C67" s="41" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="D67" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E67" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F67" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G67" s="31"/>
       <c r="H67" s="32">
@@ -4613,19 +4613,19 @@
         <v>5</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C68" s="46" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="D68" s="31" t="s">
+        <v>90</v>
+      </c>
+      <c r="E68" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F68" s="31" t="s">
         <v>91</v>
-      </c>
-      <c r="E68" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F68" s="31" t="s">
-        <v>92</v>
       </c>
       <c r="G68" s="31"/>
       <c r="H68" s="32">
@@ -4646,19 +4646,19 @@
         <v>6</v>
       </c>
       <c r="B69" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="C69" s="41" t="s">
         <v>226</v>
       </c>
-      <c r="C69" s="41" t="s">
-        <v>228</v>
-      </c>
       <c r="D69" s="31" t="s">
+        <v>92</v>
+      </c>
+      <c r="E69" s="31" t="s">
+        <v>84</v>
+      </c>
+      <c r="F69" s="19" t="s">
         <v>93</v>
-      </c>
-      <c r="E69" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="F69" s="19" t="s">
-        <v>94</v>
       </c>
       <c r="G69" s="31"/>
       <c r="H69" s="32">
@@ -4679,19 +4679,19 @@
         <v>7</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C70" s="41" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="E70" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F70" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G70" s="31"/>
       <c r="H70" s="32">
@@ -4712,19 +4712,19 @@
         <v>8</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C71" s="41" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="D71" s="31" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="E71" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F71" s="31" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="G71" s="31"/>
       <c r="H71" s="32">
@@ -4745,19 +4745,19 @@
         <v>9</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C72" s="41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D72" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E72" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F72" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G72" s="31"/>
       <c r="H72" s="32">
@@ -4778,19 +4778,19 @@
         <v>10</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C73" s="41" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D73" s="31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E73" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F73" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G73" s="31"/>
       <c r="H73" s="32">
@@ -4811,19 +4811,19 @@
         <v>11</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C74" s="41" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="D74" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E74" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F74" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G74" s="31"/>
       <c r="H74" s="32">
@@ -4844,19 +4844,19 @@
         <v>12</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C75" s="47" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D75" s="19" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E75" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F75" s="31" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G75" s="31"/>
       <c r="H75" s="32">
@@ -4877,19 +4877,19 @@
         <v>13</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C76" s="47" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D76" s="19" t="s">
+        <v>159</v>
+      </c>
+      <c r="E76" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F76" s="31" t="s">
         <v>160</v>
-      </c>
-      <c r="E76" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F76" s="31" t="s">
-        <v>161</v>
       </c>
       <c r="G76" s="31"/>
       <c r="H76" s="32">
@@ -4910,19 +4910,19 @@
         <v>14</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C77" s="47" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="D77" s="31" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="E77" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F77" s="31" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G77" s="31"/>
       <c r="H77" s="32">
@@ -4943,19 +4943,19 @@
         <v>15</v>
       </c>
       <c r="B78" s="19" t="s">
+        <v>240</v>
+      </c>
+      <c r="C78" s="41" t="s">
         <v>242</v>
       </c>
-      <c r="C78" s="41" t="s">
-        <v>244</v>
-      </c>
       <c r="D78" s="31" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E78" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F78" s="31" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G78" s="31"/>
       <c r="H78" s="32">
@@ -4976,19 +4976,19 @@
         <v>16</v>
       </c>
       <c r="B79" s="19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C79" s="46" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
       <c r="D79" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="E79" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F79" s="31" t="s">
         <v>118</v>
-      </c>
-      <c r="E79" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F79" s="31" t="s">
-        <v>119</v>
       </c>
       <c r="G79" s="31"/>
       <c r="H79" s="32">
@@ -5009,19 +5009,19 @@
         <v>17</v>
       </c>
       <c r="B80" s="19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C80" s="46" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="D80" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E80" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F80" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G80" s="31"/>
       <c r="H80" s="32">
@@ -5042,19 +5042,19 @@
         <v>18</v>
       </c>
       <c r="B81" s="19" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C81" s="41" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="D81" s="31" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="E81" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F81" s="31" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G81" s="31"/>
       <c r="H81" s="32">
@@ -5078,16 +5078,16 @@
         <v>17</v>
       </c>
       <c r="C82" s="41" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="D82" s="31" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E82" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F82" s="31" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="G82" s="31"/>
       <c r="H82" s="32">
@@ -5108,19 +5108,19 @@
         <v>20</v>
       </c>
       <c r="B83" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C83" s="41" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="D83" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E83" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F83" s="19" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G83" s="31"/>
       <c r="H83" s="32">
@@ -5141,19 +5141,19 @@
         <v>21</v>
       </c>
       <c r="B84" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C84" s="42" t="s">
         <v>222</v>
       </c>
-      <c r="C84" s="42" t="s">
-        <v>224</v>
-      </c>
       <c r="D84" s="19" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E84" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F84" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G84" s="19"/>
       <c r="H84" s="23">
@@ -5174,19 +5174,19 @@
         <v>22</v>
       </c>
       <c r="B85" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C85" s="45" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D85" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E85" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G85" s="19"/>
       <c r="H85" s="23">
@@ -5207,19 +5207,19 @@
         <v>23</v>
       </c>
       <c r="B86" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C86" s="42" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="D86" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E86" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F86" s="19" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G86" s="19"/>
       <c r="H86" s="23">
@@ -5241,16 +5241,16 @@
       </c>
       <c r="B87" s="31"/>
       <c r="C87" s="31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="D87" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E87" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F87" s="31" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G87" s="31"/>
       <c r="H87" s="32">
@@ -5265,7 +5265,7 @@
         <v>10.649999999999999</v>
       </c>
       <c r="K87" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="88" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5275,16 +5275,16 @@
       </c>
       <c r="B88" s="19"/>
       <c r="C88" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E88" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G88" s="19"/>
       <c r="H88" s="32">
@@ -5299,7 +5299,7 @@
         <v>10.649999999999999</v>
       </c>
       <c r="K88" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="89" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5309,16 +5309,16 @@
       </c>
       <c r="B89" s="19"/>
       <c r="C89" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D89" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E89" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F89" s="19" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G89" s="19"/>
       <c r="H89" s="23">
@@ -5333,7 +5333,7 @@
         <v>11.435</v>
       </c>
       <c r="K89" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="90" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5343,16 +5343,16 @@
       </c>
       <c r="B90" s="19"/>
       <c r="C90" s="19" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D90" s="19" t="s">
+        <v>162</v>
+      </c>
+      <c r="E90" s="19" t="s">
+        <v>148</v>
+      </c>
+      <c r="F90" s="19" t="s">
         <v>163</v>
-      </c>
-      <c r="E90" s="19" t="s">
-        <v>149</v>
-      </c>
-      <c r="F90" s="19" t="s">
-        <v>164</v>
       </c>
       <c r="G90" s="19"/>
       <c r="H90" s="23">
@@ -5367,7 +5367,7 @@
         <v>11.435</v>
       </c>
       <c r="K90" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="91" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5377,16 +5377,16 @@
       </c>
       <c r="B91" s="19"/>
       <c r="C91" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="D91" s="19" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E91" s="19" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F91" s="19" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G91" s="19"/>
       <c r="H91" s="23">
@@ -5400,7 +5400,7 @@
         <v>11.434999999999999</v>
       </c>
       <c r="K91" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="92" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5409,19 +5409,19 @@
         <v>29</v>
       </c>
       <c r="B92" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C92" s="45" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D92" s="19" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="E92" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="G92" s="19"/>
       <c r="H92" s="23">
@@ -5446,19 +5446,19 @@
         <v>30</v>
       </c>
       <c r="B93" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C93" s="45" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D93" s="19" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="E93" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F93" s="19" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="G93" s="19"/>
       <c r="H93" s="23">
@@ -5472,7 +5472,7 @@
         <v>0.65</v>
       </c>
       <c r="K93" s="21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="94" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5481,19 +5481,19 @@
         <v>31</v>
       </c>
       <c r="B94" s="19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C94" s="45" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D94" s="19" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="E94" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F94" s="19" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="G94" s="19"/>
       <c r="H94" s="23">
@@ -5507,7 +5507,7 @@
         <v>0.53</v>
       </c>
       <c r="K94" s="21" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="95" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
@@ -5516,19 +5516,19 @@
         <v>32</v>
       </c>
       <c r="B95" s="19" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C95" s="45" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D95" s="19" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="E95" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F95" s="19" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="G95" s="19"/>
       <c r="H95" s="23">
@@ -5566,7 +5566,7 @@
       <c r="A99" s="1"/>
       <c r="C99" s="3"/>
       <c r="D99" s="3" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="E99" s="3"/>
     </row>
@@ -5574,70 +5574,70 @@
       <c r="A100" s="1"/>
       <c r="C100" s="3"/>
       <c r="D100" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="E100" t="s">
         <v>20</v>
       </c>
       <c r="F100" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
     </row>
     <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="C101" s="3"/>
       <c r="D101" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E101" t="s">
         <v>20</v>
       </c>
       <c r="F101" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D102" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F102" t="s">
         <v>355</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F102" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D103" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E103" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F103" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D104" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E104" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F104" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D105" s="3" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="E105" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F105" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added level shifter to motor driver interface
</commit_message>
<xml_diff>
--- a/hardware/Wheelchair Receiver BOM.xlsx
+++ b/hardware/Wheelchair Receiver BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="366">
   <si>
     <t>ID #</t>
   </si>
@@ -885,9 +885,6 @@
     <t>LT1160CS#PBF</t>
   </si>
   <si>
-    <t>q4, q5, q6, q7, q8, q9</t>
-  </si>
-  <si>
     <t>q2, q3, q10, q11, q12, q13, q16, q17</t>
   </si>
   <si>
@@ -924,15 +921,9 @@
     <t>d1, d3, d4, d5, d6</t>
   </si>
   <si>
-    <t>d17, d18, d19</t>
-  </si>
-  <si>
     <t>BZV55C3V3-TP</t>
   </si>
   <si>
-    <t>d10, d11, d12, d13, d14, d15, d16</t>
-  </si>
-  <si>
     <t>3.3V TVS</t>
   </si>
   <si>
@@ -1111,6 +1102,27 @@
   </si>
   <si>
     <t>Newark or Sparkfun or Mouser</t>
+  </si>
+  <si>
+    <t>5V TVS</t>
+  </si>
+  <si>
+    <t>UCLAMP0504ACT-ND</t>
+  </si>
+  <si>
+    <t>D14, D15, D16, D47</t>
+  </si>
+  <si>
+    <t>d10, d11, d12, d13</t>
+  </si>
+  <si>
+    <t>UCLAMP0504A.TCT</t>
+  </si>
+  <si>
+    <t>q4, q5, q6, q7, q8, q9, Q14</t>
+  </si>
+  <si>
+    <t>d17, d18, d19, D45</t>
   </si>
 </sst>
 </file>
@@ -2121,8 +2133,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:K96" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A2:K96"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:K97" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A2:K97"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID #" dataDxfId="10">
       <calculatedColumnFormula>1+A2</calculatedColumnFormula>
@@ -2434,10 +2446,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M105"/>
+  <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2469,7 +2481,7 @@
       </c>
       <c r="J1" s="29">
         <f>SUM(Table2[Sub Total])</f>
-        <v>398.79999999999995</v>
+        <v>399.42999999999989</v>
       </c>
       <c r="K1" s="5"/>
     </row>
@@ -2818,7 +2830,7 @@
         <v>174</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="E12" s="19" t="s">
         <v>20</v>
@@ -2918,7 +2930,7 @@
         <v>165</v>
       </c>
       <c r="C15" s="42" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="D15" s="19" t="s">
         <v>268</v>
@@ -2927,7 +2939,7 @@
         <v>20</v>
       </c>
       <c r="F15" s="19" t="s">
-        <v>321</v>
+        <v>318</v>
       </c>
       <c r="G15" s="20" t="s">
         <v>269</v>
@@ -2953,7 +2965,7 @@
         <v>165</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="D16" s="19" t="s">
         <v>270</v>
@@ -2962,7 +2974,7 @@
         <v>20</v>
       </c>
       <c r="F16" s="19" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="G16" s="23" t="s">
         <v>271</v>
@@ -3442,10 +3454,10 @@
         <v>13</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>317</v>
+        <v>314</v>
       </c>
       <c r="C31" s="45" t="s">
-        <v>318</v>
+        <v>315</v>
       </c>
       <c r="D31" s="19" t="s">
         <v>277</v>
@@ -3454,7 +3466,7 @@
         <v>20</v>
       </c>
       <c r="F31" s="19" t="s">
-        <v>316</v>
+        <v>313</v>
       </c>
       <c r="G31" s="19" t="s">
         <v>279</v>
@@ -3480,7 +3492,7 @@
         <v>18</v>
       </c>
       <c r="C32" s="45" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
       <c r="D32" s="19" t="s">
         <v>278</v>
@@ -3489,7 +3501,7 @@
         <v>20</v>
       </c>
       <c r="F32" s="19" t="s">
-        <v>319</v>
+        <v>316</v>
       </c>
       <c r="G32" s="19" t="s">
         <v>280</v>
@@ -3583,13 +3595,13 @@
         <v>197</v>
       </c>
       <c r="C36" s="42" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>76</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="F36" s="19" t="s">
         <v>75</v>
@@ -3653,16 +3665,16 @@
         <v>198</v>
       </c>
       <c r="C38" s="42" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>84</v>
       </c>
       <c r="F38" s="31" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="G38" s="19" t="s">
         <v>254</v>
@@ -3768,7 +3780,7 @@
         <v>21</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>286</v>
+        <v>364</v>
       </c>
       <c r="H42" s="17">
         <v>0.49</v>
@@ -3803,7 +3815,7 @@
         <v>22</v>
       </c>
       <c r="G43" s="15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="H43" s="17">
         <v>0.74</v>
@@ -3864,7 +3876,7 @@
         <v>207</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="E45" s="15" t="s">
         <v>20</v>
@@ -3873,7 +3885,7 @@
         <v>28</v>
       </c>
       <c r="G45" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="H45" s="17">
         <v>0.42</v>
@@ -3943,7 +3955,7 @@
         <v>98</v>
       </c>
       <c r="G47" s="19" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="H47" s="23">
         <v>0.39</v>
@@ -3978,7 +3990,7 @@
         <v>95</v>
       </c>
       <c r="G48" s="19" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="H48" s="23">
         <v>1.05</v>
@@ -4167,17 +4179,17 @@
     </row>
     <row r="54" spans="1:11" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A54" s="24">
-        <f t="shared" ref="A54:A59" si="4">1+A53</f>
+        <f t="shared" ref="A54:A60" si="4">1+A53</f>
         <v>13</v>
       </c>
       <c r="B54" s="19" t="s">
         <v>206</v>
       </c>
       <c r="C54" s="42" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="D54" s="19" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="E54" s="19" t="s">
         <v>20</v>
@@ -4186,7 +4198,7 @@
         <v>261</v>
       </c>
       <c r="G54" s="19" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="H54" s="23">
         <v>0.49</v>
@@ -4209,10 +4221,10 @@
         <v>206</v>
       </c>
       <c r="C55" s="42" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="D55" s="19" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="E55" s="19" t="s">
         <v>20</v>
@@ -4221,7 +4233,7 @@
         <v>265</v>
       </c>
       <c r="G55" s="19" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="H55" s="23">
         <v>1</v>
@@ -4235,7 +4247,7 @@
       </c>
       <c r="K55" s="21"/>
     </row>
-    <row r="56" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A56" s="24">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -4244,7 +4256,7 @@
         <v>206</v>
       </c>
       <c r="C56" s="45" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D56" s="19" t="s">
         <v>264</v>
@@ -4256,33 +4268,33 @@
         <v>263</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>299</v>
+        <v>365</v>
       </c>
       <c r="H56" s="23">
         <v>0.38</v>
       </c>
       <c r="I56" s="20">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="J56" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.1400000000000001</v>
+        <v>1.52</v>
       </c>
       <c r="K56" s="21"/>
     </row>
-    <row r="57" spans="1:11" s="39" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A57" s="24">
         <f t="shared" si="4"/>
         <v>16</v>
       </c>
       <c r="B57" s="19" t="s">
-        <v>303</v>
+        <v>300</v>
       </c>
       <c r="C57" s="42" t="s">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="D57" s="19" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="E57" s="19" t="s">
         <v>20</v>
@@ -4291,122 +4303,124 @@
         <v>262</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>301</v>
+        <v>362</v>
       </c>
       <c r="H57" s="23">
         <v>0.56999999999999995</v>
       </c>
       <c r="I57" s="20">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="J57" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>3.9899999999999998</v>
+        <v>2.2799999999999998</v>
       </c>
       <c r="K57" s="21"/>
     </row>
-    <row r="58" spans="1:11" s="39" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A58" s="24">
-        <f t="shared" si="4"/>
+    <row r="58" spans="1:11" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A58" s="30">
+        <f>1+A57</f>
         <v>17</v>
       </c>
       <c r="B58" s="19" t="s">
-        <v>308</v>
-      </c>
-      <c r="C58" s="45" t="s">
-        <v>309</v>
-      </c>
-      <c r="D58" s="19" t="s">
-        <v>307</v>
-      </c>
-      <c r="E58" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F58" s="19" t="s">
+        <v>300</v>
+      </c>
+      <c r="C58" s="41" t="s">
+        <v>363</v>
+      </c>
+      <c r="D58" s="31" t="s">
+        <v>359</v>
+      </c>
+      <c r="E58" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F58" s="31" t="s">
+        <v>360</v>
+      </c>
+      <c r="G58" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="H58" s="32">
+        <v>0.49</v>
+      </c>
+      <c r="I58" s="40">
+        <v>4</v>
+      </c>
+      <c r="J58" s="32">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>1.96</v>
+      </c>
+      <c r="K58" s="35"/>
+    </row>
+    <row r="59" spans="1:11" s="39" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A59" s="30">
+        <f>1+A58</f>
+        <v>18</v>
+      </c>
+      <c r="B59" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C59" s="45" t="s">
+        <v>306</v>
+      </c>
+      <c r="D59" s="19" t="s">
+        <v>304</v>
+      </c>
+      <c r="E59" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F59" s="19" t="s">
         <v>266</v>
       </c>
-      <c r="G58" s="19" t="s">
-        <v>305</v>
-      </c>
-      <c r="H58" s="23">
+      <c r="G59" s="19" t="s">
+        <v>302</v>
+      </c>
+      <c r="H59" s="23">
         <v>0.38</v>
-      </c>
-      <c r="I58" s="20">
-        <v>8</v>
-      </c>
-      <c r="J58" s="23">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>3.04</v>
-      </c>
-      <c r="K58" s="21"/>
-    </row>
-    <row r="59" spans="1:11" s="39" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A59" s="24">
-        <f t="shared" si="4"/>
-        <v>18</v>
-      </c>
-      <c r="B59" s="19" t="s">
-        <v>308</v>
-      </c>
-      <c r="C59" s="45" t="s">
-        <v>310</v>
-      </c>
-      <c r="D59" s="19" t="s">
-        <v>311</v>
-      </c>
-      <c r="E59" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="F59" s="19" t="s">
-        <v>267</v>
-      </c>
-      <c r="G59" s="19" t="s">
-        <v>306</v>
-      </c>
-      <c r="H59" s="23">
-        <v>0.33</v>
       </c>
       <c r="I59" s="20">
         <v>8</v>
       </c>
       <c r="J59" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>3.04</v>
+      </c>
+      <c r="K59" s="21"/>
+    </row>
+    <row r="60" spans="1:11" s="39" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A60" s="24">
+        <f t="shared" si="4"/>
+        <v>19</v>
+      </c>
+      <c r="B60" s="19" t="s">
+        <v>305</v>
+      </c>
+      <c r="C60" s="45" t="s">
+        <v>307</v>
+      </c>
+      <c r="D60" s="19" t="s">
+        <v>308</v>
+      </c>
+      <c r="E60" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F60" s="19" t="s">
+        <v>267</v>
+      </c>
+      <c r="G60" s="19" t="s">
+        <v>303</v>
+      </c>
+      <c r="H60" s="23">
+        <v>0.33</v>
+      </c>
+      <c r="I60" s="20">
+        <v>8</v>
+      </c>
+      <c r="J60" s="23">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>2.64</v>
       </c>
-      <c r="K59" s="21"/>
-    </row>
-    <row r="60" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="30">
-        <f>1+A59</f>
-        <v>19</v>
-      </c>
-      <c r="B60" s="31" t="s">
-        <v>336</v>
-      </c>
-      <c r="C60" s="46" t="s">
-        <v>337</v>
-      </c>
-      <c r="D60" s="31" t="s">
-        <v>338</v>
-      </c>
-      <c r="E60" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F60" s="31" t="s">
-        <v>335</v>
-      </c>
-      <c r="G60" s="31"/>
-      <c r="H60" s="32">
-        <v>0.48</v>
-      </c>
-      <c r="I60" s="40">
-        <v>1</v>
-      </c>
-      <c r="J60" s="32">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.48</v>
-      </c>
-      <c r="K60" s="35"/>
+      <c r="K60" s="21"/>
     </row>
     <row r="61" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="30">
@@ -4414,53 +4428,68 @@
         <v>20</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>336</v>
+        <v>333</v>
       </c>
       <c r="C61" s="46" t="s">
-        <v>341</v>
+        <v>334</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="E61" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F61" s="31" t="s">
-        <v>339</v>
+        <v>332</v>
       </c>
       <c r="G61" s="31"/>
       <c r="H61" s="32">
-        <v>4</v>
+        <v>0.48</v>
       </c>
       <c r="I61" s="40">
         <v>1</v>
       </c>
       <c r="J61" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.48</v>
+      </c>
+      <c r="K61" s="35"/>
+    </row>
+    <row r="62" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="30">
+        <f>1+A61</f>
+        <v>21</v>
+      </c>
+      <c r="B62" s="31" t="s">
+        <v>333</v>
+      </c>
+      <c r="C62" s="46" t="s">
+        <v>338</v>
+      </c>
+      <c r="D62" s="31" t="s">
+        <v>337</v>
+      </c>
+      <c r="E62" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F62" s="31" t="s">
+        <v>336</v>
+      </c>
+      <c r="G62" s="31"/>
+      <c r="H62" s="32">
         <v>4</v>
       </c>
-      <c r="K61" s="35"/>
-    </row>
-    <row r="62" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="30"/>
-      <c r="B62" s="37"/>
-      <c r="C62" s="37"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="37"/>
-      <c r="G62" s="37"/>
-      <c r="H62" s="34"/>
-      <c r="I62" s="33"/>
-      <c r="J62" s="34">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
-      </c>
-      <c r="K62" s="38"/>
-    </row>
-    <row r="63" spans="1:11" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A63" s="30" t="s">
-        <v>82</v>
-      </c>
+      <c r="I62" s="40">
+        <v>1</v>
+      </c>
+      <c r="J62" s="32">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>4</v>
+      </c>
+      <c r="K62" s="35"/>
+    </row>
+    <row r="63" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="30"/>
       <c r="B63" s="37"/>
       <c r="C63" s="37"/>
       <c r="D63" s="37"/>
@@ -4475,421 +4504,406 @@
       </c>
       <c r="K63" s="38"/>
     </row>
-    <row r="64" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="30">
+    <row r="64" spans="1:11" s="3" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A64" s="30" t="s">
+        <v>82</v>
+      </c>
+      <c r="B64" s="37"/>
+      <c r="C64" s="37"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="37"/>
+      <c r="G64" s="37"/>
+      <c r="H64" s="34"/>
+      <c r="I64" s="33"/>
+      <c r="J64" s="34">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+      <c r="K64" s="38"/>
+    </row>
+    <row r="65" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="30">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="B64" s="19" t="s">
+      <c r="B65" s="19" t="s">
         <v>224</v>
       </c>
-      <c r="C64" s="41" t="s">
+      <c r="C65" s="41" t="s">
         <v>223</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D65" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="E64" s="19" t="s">
+      <c r="E65" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="F64" s="19" t="s">
+      <c r="F65" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="G64" s="19"/>
-      <c r="H64" s="23">
+      <c r="G65" s="19"/>
+      <c r="H65" s="23">
         <v>0.67</v>
       </c>
-      <c r="I64" s="19">
+      <c r="I65" s="19">
         <v>1</v>
       </c>
-      <c r="J64" s="32">
+      <c r="J65" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.67</v>
-      </c>
-      <c r="K64" s="35"/>
-    </row>
-    <row r="65" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="30">
-        <f t="shared" ref="A65:A70" si="5">1+A64</f>
-        <v>2</v>
-      </c>
-      <c r="B65" s="19" t="s">
-        <v>225</v>
-      </c>
-      <c r="C65" s="41" t="s">
-        <v>85</v>
-      </c>
-      <c r="D65" s="31" t="s">
-        <v>83</v>
-      </c>
-      <c r="E65" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="F65" s="31" t="s">
-        <v>85</v>
-      </c>
-      <c r="G65" s="31"/>
-      <c r="H65" s="32">
-        <v>0.94</v>
-      </c>
-      <c r="I65" s="40">
-        <v>7</v>
-      </c>
-      <c r="J65" s="32">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>6.58</v>
       </c>
       <c r="K65" s="35"/>
     </row>
     <row r="66" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="30">
-        <f t="shared" si="5"/>
-        <v>3</v>
+        <f t="shared" ref="A66:A71" si="5">1+A65</f>
+        <v>2</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C66" s="41" t="s">
-        <v>228</v>
+        <v>85</v>
       </c>
       <c r="D66" s="31" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E66" s="31" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="F66" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="G66" s="31"/>
       <c r="H66" s="32">
-        <v>1.57</v>
+        <v>0.94</v>
       </c>
       <c r="I66" s="40">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J66" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.57</v>
+        <v>6.58</v>
       </c>
       <c r="K66" s="35"/>
     </row>
     <row r="67" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="30">
         <f t="shared" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B67" s="19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C67" s="41" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="D67" s="31" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E67" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F67" s="31" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G67" s="31"/>
       <c r="H67" s="32">
-        <v>2.34</v>
+        <v>1.57</v>
       </c>
       <c r="I67" s="40">
         <v>1</v>
       </c>
       <c r="J67" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>2.34</v>
+        <v>1.57</v>
       </c>
       <c r="K67" s="35"/>
     </row>
     <row r="68" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="30">
         <f t="shared" si="5"/>
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B68" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="C68" s="46" t="s">
-        <v>232</v>
+        <v>231</v>
+      </c>
+      <c r="C68" s="41" t="s">
+        <v>230</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E68" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F68" s="31" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="G68" s="31"/>
       <c r="H68" s="32">
-        <v>1.1200000000000001</v>
+        <v>2.34</v>
       </c>
       <c r="I68" s="40">
         <v>1</v>
       </c>
       <c r="J68" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.1200000000000001</v>
+        <v>2.34</v>
       </c>
       <c r="K68" s="35"/>
     </row>
     <row r="69" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="30">
         <f t="shared" si="5"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B69" s="19" t="s">
-        <v>224</v>
-      </c>
-      <c r="C69" s="41" t="s">
-        <v>226</v>
+        <v>233</v>
+      </c>
+      <c r="C69" s="46" t="s">
+        <v>232</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E69" s="31" t="s">
-        <v>84</v>
-      </c>
-      <c r="F69" s="19" t="s">
-        <v>93</v>
+        <v>20</v>
+      </c>
+      <c r="F69" s="31" t="s">
+        <v>91</v>
       </c>
       <c r="G69" s="31"/>
       <c r="H69" s="32">
-        <v>0.57999999999999996</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="I69" s="40">
         <v>1</v>
       </c>
       <c r="J69" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.57999999999999996</v>
+        <v>1.1200000000000001</v>
       </c>
       <c r="K69" s="35"/>
     </row>
     <row r="70" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="30">
         <f t="shared" si="5"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B70" s="19" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="C70" s="41" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>103</v>
+        <v>92</v>
       </c>
       <c r="E70" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F70" s="31" t="s">
-        <v>94</v>
+        <v>84</v>
+      </c>
+      <c r="F70" s="19" t="s">
+        <v>93</v>
       </c>
       <c r="G70" s="31"/>
       <c r="H70" s="32">
-        <v>6.03</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I70" s="40">
         <v>1</v>
       </c>
       <c r="J70" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>6.03</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="K70" s="35"/>
     </row>
     <row r="71" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="30">
-        <f>1+A70</f>
-        <v>8</v>
+        <f t="shared" si="5"/>
+        <v>7</v>
       </c>
       <c r="B71" s="19" t="s">
-        <v>224</v>
+        <v>235</v>
       </c>
       <c r="C71" s="41" t="s">
-        <v>350</v>
+        <v>234</v>
       </c>
       <c r="D71" s="31" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E71" s="31" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="F71" s="31" t="s">
-        <v>349</v>
+        <v>94</v>
       </c>
       <c r="G71" s="31"/>
       <c r="H71" s="32">
-        <v>0.84</v>
+        <v>6.03</v>
       </c>
       <c r="I71" s="40">
         <v>1</v>
       </c>
       <c r="J71" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.84</v>
+        <v>6.03</v>
       </c>
       <c r="K71" s="35"/>
     </row>
     <row r="72" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="30">
         <f>1+A71</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B72" s="19" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C72" s="41" t="s">
-        <v>104</v>
+        <v>347</v>
       </c>
       <c r="D72" s="31" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="E72" s="31" t="s">
         <v>84</v>
       </c>
       <c r="F72" s="31" t="s">
-        <v>104</v>
+        <v>346</v>
       </c>
       <c r="G72" s="31"/>
       <c r="H72" s="32">
-        <v>2.35</v>
+        <v>0.84</v>
       </c>
       <c r="I72" s="40">
         <v>1</v>
       </c>
       <c r="J72" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>2.35</v>
+        <v>0.84</v>
       </c>
       <c r="K72" s="35"/>
     </row>
     <row r="73" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="30">
         <f>1+A72</f>
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B73" s="19" t="s">
         <v>225</v>
       </c>
       <c r="C73" s="41" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D73" s="31" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E73" s="31" t="s">
         <v>84</v>
       </c>
       <c r="F73" s="31" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G73" s="31"/>
       <c r="H73" s="32">
-        <v>3.15</v>
+        <v>2.35</v>
       </c>
       <c r="I73" s="40">
         <v>1</v>
       </c>
       <c r="J73" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>3.15</v>
+        <v>2.35</v>
       </c>
       <c r="K73" s="35"/>
     </row>
     <row r="74" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="30">
         <f>1+A73</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B74" s="19" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C74" s="41" t="s">
-        <v>227</v>
+        <v>105</v>
       </c>
       <c r="D74" s="31" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E74" s="31" t="s">
         <v>84</v>
       </c>
       <c r="F74" s="31" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="G74" s="31"/>
       <c r="H74" s="32">
-        <v>0.98</v>
+        <v>3.15</v>
       </c>
       <c r="I74" s="40">
         <v>1</v>
       </c>
       <c r="J74" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.98</v>
+        <v>3.15</v>
       </c>
       <c r="K74" s="35"/>
     </row>
     <row r="75" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="30">
         <f>1+A74</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B75" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="C75" s="47" t="s">
-        <v>238</v>
-      </c>
-      <c r="D75" s="19" t="s">
-        <v>147</v>
+        <v>224</v>
+      </c>
+      <c r="C75" s="41" t="s">
+        <v>227</v>
+      </c>
+      <c r="D75" s="31" t="s">
+        <v>107</v>
       </c>
       <c r="E75" s="31" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="F75" s="31" t="s">
-        <v>158</v>
+        <v>106</v>
       </c>
       <c r="G75" s="31"/>
       <c r="H75" s="32">
-        <v>0.59</v>
+        <v>0.98</v>
       </c>
       <c r="I75" s="40">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J75" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.18</v>
+        <v>0.98</v>
       </c>
       <c r="K75" s="35"/>
     </row>
     <row r="76" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="30">
-        <f t="shared" ref="A76:A78" si="6">1+A75</f>
-        <v>13</v>
+        <f>1+A75</f>
+        <v>12</v>
       </c>
       <c r="B76" s="19" t="s">
         <v>220</v>
       </c>
       <c r="C76" s="47" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="D76" s="19" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="E76" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F76" s="31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="G76" s="31"/>
       <c r="H76" s="32">
@@ -4906,395 +4920,394 @@
     </row>
     <row r="77" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="30">
-        <f t="shared" si="6"/>
-        <v>14</v>
+        <f t="shared" ref="A77:A79" si="6">1+A76</f>
+        <v>13</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>240</v>
+        <v>220</v>
       </c>
       <c r="C77" s="47" t="s">
-        <v>241</v>
-      </c>
-      <c r="D77" s="31" t="s">
-        <v>110</v>
+        <v>239</v>
+      </c>
+      <c r="D77" s="19" t="s">
+        <v>159</v>
       </c>
       <c r="E77" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F77" s="31" t="s">
-        <v>109</v>
+        <v>160</v>
       </c>
       <c r="G77" s="31"/>
       <c r="H77" s="32">
-        <v>1.44</v>
+        <v>0.59</v>
       </c>
       <c r="I77" s="40">
         <v>2</v>
       </c>
       <c r="J77" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>2.88</v>
+        <v>1.18</v>
       </c>
       <c r="K77" s="35"/>
     </row>
     <row r="78" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="30">
         <f t="shared" si="6"/>
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B78" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="C78" s="41" t="s">
-        <v>242</v>
+      <c r="C78" s="47" t="s">
+        <v>241</v>
       </c>
       <c r="D78" s="31" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E78" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F78" s="31" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G78" s="31"/>
       <c r="H78" s="32">
-        <v>1.1499999999999999</v>
+        <v>1.44</v>
       </c>
       <c r="I78" s="40">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="J78" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>3.4499999999999997</v>
+        <v>2.88</v>
       </c>
       <c r="K78" s="35"/>
     </row>
     <row r="79" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="30">
-        <f>1+A78</f>
-        <v>16</v>
+        <f t="shared" si="6"/>
+        <v>15</v>
       </c>
       <c r="B79" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="C79" s="46" t="s">
-        <v>243</v>
+      <c r="C79" s="41" t="s">
+        <v>242</v>
       </c>
       <c r="D79" s="31" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="E79" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F79" s="31" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="G79" s="31"/>
       <c r="H79" s="32">
-        <v>1.79</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="I79" s="40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J79" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.79</v>
+        <v>3.4499999999999997</v>
       </c>
       <c r="K79" s="35"/>
     </row>
     <row r="80" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="30">
-        <f t="shared" ref="A80:A90" si="7">1+A79</f>
-        <v>17</v>
+        <f>1+A79</f>
+        <v>16</v>
       </c>
       <c r="B80" s="19" t="s">
         <v>240</v>
       </c>
       <c r="C80" s="46" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D80" s="31" t="s">
-        <v>113</v>
+        <v>117</v>
       </c>
       <c r="E80" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F80" s="31" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="G80" s="31"/>
       <c r="H80" s="32">
-        <v>1.6</v>
+        <v>1.79</v>
       </c>
       <c r="I80" s="40">
         <v>1</v>
       </c>
       <c r="J80" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.6</v>
+        <v>1.79</v>
       </c>
       <c r="K80" s="35"/>
     </row>
     <row r="81" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="30">
-        <f t="shared" si="7"/>
-        <v>18</v>
+        <f t="shared" ref="A81:A91" si="7">1+A80</f>
+        <v>17</v>
       </c>
       <c r="B81" s="19" t="s">
         <v>240</v>
       </c>
-      <c r="C81" s="41" t="s">
-        <v>245</v>
+      <c r="C81" s="46" t="s">
+        <v>244</v>
       </c>
       <c r="D81" s="31" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E81" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F81" s="31" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G81" s="31"/>
       <c r="H81" s="32">
-        <v>0.95</v>
+        <v>1.6</v>
       </c>
       <c r="I81" s="40">
         <v>1</v>
       </c>
       <c r="J81" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.95</v>
+        <v>1.6</v>
       </c>
       <c r="K81" s="35"/>
     </row>
     <row r="82" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="30">
         <f t="shared" si="7"/>
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>17</v>
+        <v>240</v>
       </c>
       <c r="C82" s="41" t="s">
-        <v>345</v>
+        <v>245</v>
       </c>
       <c r="D82" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="E82" s="19" t="s">
-        <v>84</v>
+        <v>114</v>
+      </c>
+      <c r="E82" s="31" t="s">
+        <v>20</v>
       </c>
       <c r="F82" s="31" t="s">
-        <v>346</v>
+        <v>116</v>
       </c>
       <c r="G82" s="31"/>
       <c r="H82" s="32">
-        <v>0.11</v>
+        <v>0.95</v>
       </c>
       <c r="I82" s="40">
         <v>1</v>
       </c>
       <c r="J82" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.11</v>
+        <v>0.95</v>
       </c>
       <c r="K82" s="35"/>
     </row>
     <row r="83" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="30">
-        <f>1+A82</f>
-        <v>20</v>
+        <f t="shared" si="7"/>
+        <v>19</v>
       </c>
       <c r="B83" s="19" t="s">
-        <v>220</v>
+        <v>17</v>
       </c>
       <c r="C83" s="41" t="s">
-        <v>237</v>
-      </c>
-      <c r="D83" s="19" t="s">
-        <v>143</v>
-      </c>
-      <c r="E83" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F83" s="19" t="s">
-        <v>157</v>
+        <v>342</v>
+      </c>
+      <c r="D83" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="E83" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="F83" s="31" t="s">
+        <v>343</v>
       </c>
       <c r="G83" s="31"/>
       <c r="H83" s="32">
-        <v>0.83</v>
+        <v>0.11</v>
       </c>
       <c r="I83" s="40">
         <v>1</v>
       </c>
       <c r="J83" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.83</v>
+        <v>0.11</v>
       </c>
       <c r="K83" s="35"/>
     </row>
     <row r="84" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="30">
-        <f t="shared" si="7"/>
-        <v>21</v>
+        <f>1+A83</f>
+        <v>20</v>
       </c>
       <c r="B84" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C84" s="42" t="s">
-        <v>222</v>
+      <c r="C84" s="41" t="s">
+        <v>237</v>
       </c>
       <c r="D84" s="19" t="s">
-        <v>146</v>
-      </c>
-      <c r="E84" s="19" t="s">
-        <v>84</v>
+        <v>143</v>
+      </c>
+      <c r="E84" s="31" t="s">
+        <v>20</v>
       </c>
       <c r="F84" s="19" t="s">
-        <v>155</v>
-      </c>
-      <c r="G84" s="19"/>
-      <c r="H84" s="23">
-        <v>0.17</v>
-      </c>
-      <c r="I84" s="20">
-        <v>50</v>
-      </c>
-      <c r="J84" s="23">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>8.5</v>
-      </c>
-      <c r="K84" s="21"/>
+        <v>157</v>
+      </c>
+      <c r="G84" s="31"/>
+      <c r="H84" s="32">
+        <v>0.83</v>
+      </c>
+      <c r="I84" s="40">
+        <v>1</v>
+      </c>
+      <c r="J84" s="32">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.83</v>
+      </c>
+      <c r="K84" s="35"/>
     </row>
     <row r="85" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="30">
         <f t="shared" si="7"/>
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B85" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C85" s="45" t="s">
-        <v>236</v>
+      <c r="C85" s="42" t="s">
+        <v>222</v>
       </c>
       <c r="D85" s="19" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E85" s="19" t="s">
-        <v>20</v>
+        <v>84</v>
       </c>
       <c r="F85" s="19" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G85" s="19"/>
       <c r="H85" s="23">
-        <v>0.77</v>
+        <v>0.17</v>
       </c>
       <c r="I85" s="20">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="J85" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.77</v>
+        <v>8.5</v>
       </c>
       <c r="K85" s="21"/>
     </row>
     <row r="86" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="30">
         <f t="shared" si="7"/>
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B86" s="19" t="s">
         <v>220</v>
       </c>
-      <c r="C86" s="42" t="s">
-        <v>221</v>
+      <c r="C86" s="45" t="s">
+        <v>236</v>
       </c>
       <c r="D86" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E86" s="19" t="s">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="F86" s="19" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="G86" s="19"/>
       <c r="H86" s="23">
-        <v>0.23</v>
+        <v>0.77</v>
       </c>
       <c r="I86" s="20">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="J86" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>11.5</v>
+        <v>0.77</v>
       </c>
       <c r="K86" s="21"/>
     </row>
     <row r="87" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="30">
         <f t="shared" si="7"/>
-        <v>24</v>
-      </c>
-      <c r="B87" s="31"/>
-      <c r="C87" s="31" t="s">
-        <v>152</v>
+        <v>23</v>
+      </c>
+      <c r="B87" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C87" s="42" t="s">
+        <v>221</v>
       </c>
       <c r="D87" s="19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="E87" s="19" t="s">
-        <v>148</v>
-      </c>
-      <c r="F87" s="31" t="s">
-        <v>152</v>
-      </c>
-      <c r="G87" s="31"/>
-      <c r="H87" s="32">
-        <f>7.1/100</f>
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="I87" s="40">
-        <v>150</v>
-      </c>
-      <c r="J87" s="32">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>10.649999999999999</v>
-      </c>
-      <c r="K87" s="21" t="s">
-        <v>149</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="F87" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="G87" s="19"/>
+      <c r="H87" s="23">
+        <v>0.23</v>
+      </c>
+      <c r="I87" s="20">
+        <v>50</v>
+      </c>
+      <c r="J87" s="23">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>11.5</v>
+      </c>
+      <c r="K87" s="21"/>
     </row>
     <row r="88" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="30">
         <f t="shared" si="7"/>
-        <v>25</v>
-      </c>
-      <c r="B88" s="19"/>
-      <c r="C88" s="19" t="s">
-        <v>153</v>
+        <v>24</v>
+      </c>
+      <c r="B88" s="31"/>
+      <c r="C88" s="31" t="s">
+        <v>152</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E88" s="19" t="s">
         <v>148</v>
       </c>
-      <c r="F88" s="19" t="s">
-        <v>153</v>
-      </c>
-      <c r="G88" s="19"/>
+      <c r="F88" s="31" t="s">
+        <v>152</v>
+      </c>
+      <c r="G88" s="31"/>
       <c r="H88" s="32">
         <f>7.1/100</f>
         <v>7.0999999999999994E-2</v>
       </c>
-      <c r="I88" s="20">
+      <c r="I88" s="40">
         <v>150</v>
       </c>
-      <c r="J88" s="23">
+      <c r="J88" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>10.649999999999999</v>
       </c>
@@ -5305,32 +5318,32 @@
     <row r="89" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="30">
         <f t="shared" si="7"/>
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B89" s="19"/>
       <c r="C89" s="19" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D89" s="19" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="E89" s="19" t="s">
         <v>148</v>
       </c>
       <c r="F89" s="19" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="G89" s="19"/>
-      <c r="H89" s="23">
-        <f>22.87/100</f>
-        <v>0.22870000000000001</v>
+      <c r="H89" s="32">
+        <f>7.1/100</f>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="I89" s="20">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="J89" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>11.435</v>
+        <v>10.649999999999999</v>
       </c>
       <c r="K89" s="21" t="s">
         <v>149</v>
@@ -5339,20 +5352,20 @@
     <row r="90" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="30">
         <f t="shared" si="7"/>
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B90" s="19"/>
       <c r="C90" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="D90" s="19" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="E90" s="19" t="s">
         <v>148</v>
       </c>
       <c r="F90" s="19" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G90" s="19"/>
       <c r="H90" s="23">
@@ -5371,33 +5384,34 @@
       </c>
     </row>
     <row r="91" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="24">
-        <f>1+A90</f>
-        <v>28</v>
+      <c r="A91" s="30">
+        <f t="shared" si="7"/>
+        <v>27</v>
       </c>
       <c r="B91" s="19"/>
       <c r="C91" s="19" t="s">
-        <v>348</v>
+        <v>163</v>
       </c>
       <c r="D91" s="19" t="s">
-        <v>347</v>
+        <v>162</v>
       </c>
       <c r="E91" s="19" t="s">
         <v>148</v>
       </c>
       <c r="F91" s="19" t="s">
-        <v>348</v>
+        <v>163</v>
       </c>
       <c r="G91" s="19"/>
       <c r="H91" s="23">
-        <v>0.22869999999999999</v>
+        <f>22.87/100</f>
+        <v>0.22870000000000001</v>
       </c>
       <c r="I91" s="20">
         <v>50</v>
       </c>
       <c r="J91" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>11.434999999999999</v>
+        <v>11.435</v>
       </c>
       <c r="K91" s="21" t="s">
         <v>149</v>
@@ -5405,124 +5419,122 @@
     </row>
     <row r="92" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="24">
-        <f t="shared" ref="A92:A95" si="8">1+A91</f>
-        <v>29</v>
-      </c>
-      <c r="B92" s="19" t="s">
-        <v>220</v>
-      </c>
-      <c r="C92" s="45" t="s">
-        <v>326</v>
+        <f>1+A91</f>
+        <v>28</v>
+      </c>
+      <c r="B92" s="19"/>
+      <c r="C92" s="19" t="s">
+        <v>345</v>
       </c>
       <c r="D92" s="19" t="s">
-        <v>288</v>
+        <v>344</v>
       </c>
       <c r="E92" s="19" t="s">
-        <v>20</v>
+        <v>148</v>
       </c>
       <c r="F92" s="19" t="s">
-        <v>325</v>
+        <v>345</v>
       </c>
       <c r="G92" s="19"/>
       <c r="H92" s="23">
-        <v>1.0900000000000001</v>
+        <v>0.22869999999999999</v>
       </c>
       <c r="I92" s="20">
-        <v>1</v>
+        <v>50</v>
       </c>
       <c r="J92" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="K92" s="21"/>
-      <c r="M92" s="50">
-        <f>SUM(J87:J91)</f>
-        <v>55.605000000000004</v>
+        <v>11.434999999999999</v>
+      </c>
+      <c r="K92" s="21" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="93" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="24">
-        <f t="shared" si="8"/>
-        <v>30</v>
+        <f t="shared" ref="A93:A96" si="8">1+A92</f>
+        <v>29</v>
       </c>
       <c r="B93" s="19" t="s">
         <v>220</v>
       </c>
       <c r="C93" s="45" t="s">
-        <v>333</v>
+        <v>323</v>
       </c>
       <c r="D93" s="19" t="s">
-        <v>312</v>
+        <v>287</v>
       </c>
       <c r="E93" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F93" s="19" t="s">
-        <v>332</v>
+        <v>322</v>
       </c>
       <c r="G93" s="19"/>
       <c r="H93" s="23">
-        <v>0.65</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="I93" s="20">
         <v>1</v>
       </c>
       <c r="J93" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.65</v>
-      </c>
-      <c r="K93" s="21" t="s">
-        <v>314</v>
+        <v>1.0900000000000001</v>
+      </c>
+      <c r="K93" s="21"/>
+      <c r="M93" s="50">
+        <f>SUM(J88:J92)</f>
+        <v>55.605000000000004</v>
       </c>
     </row>
     <row r="94" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="24">
         <f t="shared" si="8"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B94" s="19" t="s">
         <v>220</v>
       </c>
       <c r="C94" s="45" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D94" s="19" t="s">
-        <v>315</v>
+        <v>309</v>
       </c>
       <c r="E94" s="19" t="s">
         <v>20</v>
       </c>
       <c r="F94" s="19" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G94" s="19"/>
       <c r="H94" s="23">
-        <v>0.53</v>
+        <v>0.65</v>
       </c>
       <c r="I94" s="20">
         <v>1</v>
       </c>
       <c r="J94" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.53</v>
+        <v>0.65</v>
       </c>
       <c r="K94" s="21" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="95" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="24">
         <f t="shared" si="8"/>
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B95" s="19" t="s">
+        <v>220</v>
+      </c>
+      <c r="C95" s="45" t="s">
         <v>328</v>
       </c>
-      <c r="C95" s="45" t="s">
-        <v>329</v>
-      </c>
       <c r="D95" s="19" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E95" s="19" t="s">
         <v>20</v>
@@ -5532,112 +5544,147 @@
       </c>
       <c r="G95" s="19"/>
       <c r="H95" s="23">
+        <v>0.53</v>
+      </c>
+      <c r="I95" s="20">
+        <v>1</v>
+      </c>
+      <c r="J95" s="23">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.53</v>
+      </c>
+      <c r="K95" s="21" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="96" spans="1:13" s="39" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A96" s="24">
+        <f t="shared" si="8"/>
+        <v>32</v>
+      </c>
+      <c r="B96" s="19" t="s">
+        <v>325</v>
+      </c>
+      <c r="C96" s="45" t="s">
+        <v>326</v>
+      </c>
+      <c r="D96" s="19" t="s">
+        <v>310</v>
+      </c>
+      <c r="E96" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="F96" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="G96" s="19"/>
+      <c r="H96" s="23">
         <v>0.191</v>
       </c>
-      <c r="I95" s="20">
+      <c r="I96" s="20">
         <v>5</v>
       </c>
-      <c r="J95" s="23">
+      <c r="J96" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.95500000000000007</v>
       </c>
-      <c r="K95" s="21"/>
-    </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A96" s="13"/>
-      <c r="B96" s="9"/>
-      <c r="C96" s="9"/>
-      <c r="D96" s="9"/>
-      <c r="E96" s="9"/>
-      <c r="F96" s="9"/>
-      <c r="G96" s="9"/>
-      <c r="H96" s="10"/>
-      <c r="I96" s="27"/>
-      <c r="J96" s="10">
+      <c r="K96" s="21"/>
+    </row>
+    <row r="97" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A97" s="13"/>
+      <c r="B97" s="9"/>
+      <c r="C97" s="9"/>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9"/>
+      <c r="F97" s="9"/>
+      <c r="G97" s="9"/>
+      <c r="H97" s="10"/>
+      <c r="I97" s="27"/>
+      <c r="J97" s="10">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K96" s="12"/>
-    </row>
-    <row r="98" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C98" s="1"/>
-    </row>
-    <row r="99" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A99" s="1"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="E99" s="3"/>
-    </row>
-    <row r="100" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="K97" s="12"/>
+    </row>
+    <row r="99" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="1"/>
       <c r="C100" s="3"/>
-      <c r="D100" t="s">
-        <v>351</v>
-      </c>
-      <c r="E100" t="s">
-        <v>20</v>
-      </c>
-      <c r="F100" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="D100" s="3" t="s">
+        <v>331</v>
+      </c>
+      <c r="E100" s="3"/>
+    </row>
+    <row r="101" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="1"/>
       <c r="C101" s="3"/>
-      <c r="D101" s="3" t="s">
+      <c r="D101" t="s">
+        <v>348</v>
+      </c>
+      <c r="E101" t="s">
+        <v>20</v>
+      </c>
+      <c r="F101" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="102" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+      <c r="C102" s="3"/>
+      <c r="D102" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E102" t="s">
+        <v>20</v>
+      </c>
+      <c r="F102" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="103" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D103" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F103" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D104" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F104" t="s">
         <v>353</v>
       </c>
-      <c r="E101" t="s">
-        <v>20</v>
-      </c>
-      <c r="F101" t="s">
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D105" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F105" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D102" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="E102" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F102" t="s">
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D106" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F106" t="s">
         <v>355</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D103" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="E103" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F103" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D104" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F104" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D105" s="3" t="s">
-        <v>353</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F105" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finished LCD interface. Todo - limit switch, proportional joystick, photointerrupter, buttons
</commit_message>
<xml_diff>
--- a/hardware/Wheelchair Receiver BOM.xlsx
+++ b/hardware/Wheelchair Receiver BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="366">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="364">
   <si>
     <t>ID #</t>
   </si>
@@ -1080,21 +1080,9 @@
     <t>Photointerrupter</t>
   </si>
   <si>
-    <t>425-1950-5-ND</t>
-  </si>
-  <si>
-    <t>425-1953-5-ND</t>
-  </si>
-  <si>
-    <t>425-1948-5-ND</t>
-  </si>
-  <si>
     <t>425-1954-5-ND</t>
   </si>
   <si>
-    <t>425-1949-5-ND</t>
-  </si>
-  <si>
     <t>Xmega64A1</t>
   </si>
   <si>
@@ -1110,12 +1098,6 @@
     <t>UCLAMP0504ACT-ND</t>
   </si>
   <si>
-    <t>D14, D15, D16, D47</t>
-  </si>
-  <si>
-    <t>d10, d11, d12, d13</t>
-  </si>
-  <si>
     <t>UCLAMP0504A.TCT</t>
   </si>
   <si>
@@ -1123,6 +1105,18 @@
   </si>
   <si>
     <t>d17, d18, d19, D45</t>
+  </si>
+  <si>
+    <t>D47</t>
+  </si>
+  <si>
+    <t>d10, d11, d12, d13, D14, D15, D16</t>
+  </si>
+  <si>
+    <t>Potentiometer</t>
+  </si>
+  <si>
+    <t>3362P-203LF-ND</t>
   </si>
 </sst>
 </file>
@@ -2446,10 +2440,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M106"/>
+  <dimension ref="A1:M103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="D103" sqref="D103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2481,7 +2475,7 @@
       </c>
       <c r="J1" s="29">
         <f>SUM(Table2[Sub Total])</f>
-        <v>399.42999999999989</v>
+        <v>399.66999999999996</v>
       </c>
       <c r="K1" s="5"/>
     </row>
@@ -3595,13 +3589,13 @@
         <v>197</v>
       </c>
       <c r="C36" s="42" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>76</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="F36" s="19" t="s">
         <v>75</v>
@@ -3668,7 +3662,7 @@
         <v>339</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>84</v>
@@ -3780,7 +3774,7 @@
         <v>21</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="H42" s="17">
         <v>0.49</v>
@@ -4268,7 +4262,7 @@
         <v>263</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="H56" s="23">
         <v>0.38</v>
@@ -4282,7 +4276,7 @@
       </c>
       <c r="K56" s="21"/>
     </row>
-    <row r="57" spans="1:11" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="39" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A57" s="24">
         <f t="shared" si="4"/>
         <v>16</v>
@@ -4303,21 +4297,21 @@
         <v>262</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H57" s="23">
         <v>0.56999999999999995</v>
       </c>
       <c r="I57" s="20">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="J57" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>2.2799999999999998</v>
+        <v>3.9899999999999998</v>
       </c>
       <c r="K57" s="21"/>
     </row>
-    <row r="58" spans="1:11" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A58" s="30">
         <f>1+A57</f>
         <v>17</v>
@@ -4326,29 +4320,29 @@
         <v>300</v>
       </c>
       <c r="C58" s="41" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="E58" s="31" t="s">
         <v>20</v>
       </c>
       <c r="F58" s="31" t="s">
+        <v>356</v>
+      </c>
+      <c r="G58" s="19" t="s">
         <v>360</v>
-      </c>
-      <c r="G58" s="19" t="s">
-        <v>361</v>
       </c>
       <c r="H58" s="32">
         <v>0.49</v>
       </c>
       <c r="I58" s="40">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="J58" s="32">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.96</v>
+        <v>0.49</v>
       </c>
       <c r="K58" s="35"/>
     </row>
@@ -5644,47 +5638,14 @@
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D103" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E103" s="3" t="s">
+      <c r="D103" t="s">
+        <v>362</v>
+      </c>
+      <c r="E103" t="s">
         <v>20</v>
       </c>
       <c r="F103" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D104" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E104" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F104" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D105" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E105" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F105" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="D106" s="3" t="s">
-        <v>350</v>
-      </c>
-      <c r="E106" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F106" t="s">
-        <v>355</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Found a real level converter for the motor driver interface
</commit_message>
<xml_diff>
--- a/hardware/Wheelchair Receiver BOM.xlsx
+++ b/hardware/Wheelchair Receiver BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="368">
   <si>
     <t>ID #</t>
   </si>
@@ -1101,12 +1101,6 @@
     <t>UCLAMP0504A.TCT</t>
   </si>
   <si>
-    <t>q4, q5, q6, q7, q8, q9, Q14</t>
-  </si>
-  <si>
-    <t>d17, d18, d19, D45</t>
-  </si>
-  <si>
     <t>D47</t>
   </si>
   <si>
@@ -1117,6 +1111,24 @@
   </si>
   <si>
     <t>3362P-203LF-ND</t>
+  </si>
+  <si>
+    <t>IC9</t>
+  </si>
+  <si>
+    <t>74LVC2T45DC,125</t>
+  </si>
+  <si>
+    <t>568-5479-1-ND</t>
+  </si>
+  <si>
+    <t>2-bit Level Translator</t>
+  </si>
+  <si>
+    <t>q4, q5, q6, q7, q8, q9</t>
+  </si>
+  <si>
+    <t>d17, d18, d19</t>
   </si>
 </sst>
 </file>
@@ -2440,10 +2452,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M103"/>
+  <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="D103" sqref="D103"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="D56" sqref="D56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2475,7 +2487,7 @@
       </c>
       <c r="J1" s="29">
         <f>SUM(Table2[Sub Total])</f>
-        <v>399.66999999999996</v>
+        <v>399.28999999999996</v>
       </c>
       <c r="K1" s="5"/>
     </row>
@@ -3774,7 +3786,7 @@
         <v>21</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>358</v>
+        <v>366</v>
       </c>
       <c r="H42" s="17">
         <v>0.49</v>
@@ -4241,7 +4253,7 @@
       </c>
       <c r="K55" s="21"/>
     </row>
-    <row r="56" spans="1:11" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="24">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -4262,17 +4274,17 @@
         <v>263</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>359</v>
+        <v>367</v>
       </c>
       <c r="H56" s="23">
         <v>0.38</v>
       </c>
       <c r="I56" s="20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="J56" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.52</v>
+        <v>1.1400000000000001</v>
       </c>
       <c r="K56" s="21"/>
     </row>
@@ -4297,7 +4309,7 @@
         <v>262</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="H57" s="23">
         <v>0.56999999999999995</v>
@@ -4332,7 +4344,7 @@
         <v>356</v>
       </c>
       <c r="G58" s="19" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="H58" s="32">
         <v>0.49</v>
@@ -5639,13 +5651,30 @@
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D103" t="s">
+        <v>360</v>
+      </c>
+      <c r="E103" t="s">
+        <v>20</v>
+      </c>
+      <c r="F103" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="104" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C104" t="s">
+        <v>363</v>
+      </c>
+      <c r="D104" t="s">
+        <v>365</v>
+      </c>
+      <c r="E104" t="s">
+        <v>20</v>
+      </c>
+      <c r="F104" t="s">
+        <v>364</v>
+      </c>
+      <c r="G104" t="s">
         <v>362</v>
-      </c>
-      <c r="E103" t="s">
-        <v>20</v>
-      </c>
-      <c r="F103" t="s">
-        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a real level translator to the LCD interface
</commit_message>
<xml_diff>
--- a/hardware/Wheelchair Receiver BOM.xlsx
+++ b/hardware/Wheelchair Receiver BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="510" uniqueCount="368">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="371">
   <si>
     <t>ID #</t>
   </si>
@@ -1129,6 +1129,15 @@
   </si>
   <si>
     <t>d17, d18, d19</t>
+  </si>
+  <si>
+    <t>8-bit Level Translator</t>
+  </si>
+  <si>
+    <t>SN74LVC8T245DGVR</t>
+  </si>
+  <si>
+    <t>296-19287-1-ND</t>
   </si>
 </sst>
 </file>
@@ -2452,10 +2461,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M104"/>
+  <dimension ref="A1:M105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="D56" sqref="D56"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5676,6 +5685,26 @@
       <c r="G104" t="s">
         <v>362</v>
       </c>
+      <c r="H104">
+        <v>0.62</v>
+      </c>
+    </row>
+    <row r="105" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="C105" t="s">
+        <v>369</v>
+      </c>
+      <c r="D105" t="s">
+        <v>368</v>
+      </c>
+      <c r="E105" t="s">
+        <v>20</v>
+      </c>
+      <c r="F105" t="s">
+        <v>370</v>
+      </c>
+      <c r="H105">
+        <v>1.26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Started to add motor current sensor - needs work
</commit_message>
<xml_diff>
--- a/hardware/Wheelchair Receiver BOM.xlsx
+++ b/hardware/Wheelchair Receiver BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="374">
   <si>
     <t>ID #</t>
   </si>
@@ -1080,9 +1080,6 @@
     <t>Photointerrupter</t>
   </si>
   <si>
-    <t>425-1954-5-ND</t>
-  </si>
-  <si>
     <t>Xmega64A1</t>
   </si>
   <si>
@@ -1138,6 +1135,18 @@
   </si>
   <si>
     <t>296-19287-1-ND</t>
+  </si>
+  <si>
+    <t>±100A current sensor</t>
+  </si>
+  <si>
+    <t>ACS758LCB-100B-PFF-T</t>
+  </si>
+  <si>
+    <t>620-1321-ND</t>
+  </si>
+  <si>
+    <t>425-1949-5-ND</t>
   </si>
 </sst>
 </file>
@@ -1147,7 +1156,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1360,6 +1369,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="36">
@@ -1721,7 +1736,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1859,6 +1874,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2461,10 +2477,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M105"/>
+  <dimension ref="A1:M106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F101" sqref="F101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3610,13 +3627,13 @@
         <v>197</v>
       </c>
       <c r="C36" s="42" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="D36" s="19" t="s">
         <v>76</v>
       </c>
       <c r="E36" s="19" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="F36" s="19" t="s">
         <v>75</v>
@@ -3683,7 +3700,7 @@
         <v>339</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>84</v>
@@ -3795,7 +3812,7 @@
         <v>21</v>
       </c>
       <c r="G42" s="15" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H42" s="17">
         <v>0.49</v>
@@ -4283,7 +4300,7 @@
         <v>263</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H56" s="23">
         <v>0.38</v>
@@ -4318,7 +4335,7 @@
         <v>262</v>
       </c>
       <c r="G57" s="19" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H57" s="23">
         <v>0.56999999999999995</v>
@@ -4341,19 +4358,19 @@
         <v>300</v>
       </c>
       <c r="C58" s="41" t="s">
+        <v>356</v>
+      </c>
+      <c r="D58" s="31" t="s">
+        <v>354</v>
+      </c>
+      <c r="E58" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="F58" s="31" t="s">
+        <v>355</v>
+      </c>
+      <c r="G58" s="19" t="s">
         <v>357</v>
-      </c>
-      <c r="D58" s="31" t="s">
-        <v>355</v>
-      </c>
-      <c r="E58" s="31" t="s">
-        <v>20</v>
-      </c>
-      <c r="F58" s="31" t="s">
-        <v>356</v>
-      </c>
-      <c r="G58" s="19" t="s">
-        <v>358</v>
       </c>
       <c r="H58" s="32">
         <v>0.49</v>
@@ -5655,35 +5672,35 @@
         <v>20</v>
       </c>
       <c r="F102" t="s">
-        <v>351</v>
+        <v>373</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D103" t="s">
+        <v>359</v>
+      </c>
+      <c r="E103" t="s">
+        <v>20</v>
+      </c>
+      <c r="F103" t="s">
         <v>360</v>
-      </c>
-      <c r="E103" t="s">
-        <v>20</v>
-      </c>
-      <c r="F103" t="s">
-        <v>361</v>
       </c>
     </row>
     <row r="104" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C104" t="s">
+        <v>362</v>
+      </c>
+      <c r="D104" t="s">
+        <v>364</v>
+      </c>
+      <c r="E104" t="s">
+        <v>20</v>
+      </c>
+      <c r="F104" t="s">
         <v>363</v>
       </c>
-      <c r="D104" t="s">
-        <v>365</v>
-      </c>
-      <c r="E104" t="s">
-        <v>20</v>
-      </c>
-      <c r="F104" t="s">
-        <v>364</v>
-      </c>
       <c r="G104" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="H104">
         <v>0.62</v>
@@ -5691,19 +5708,42 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C105" t="s">
+        <v>368</v>
+      </c>
+      <c r="D105" t="s">
+        <v>367</v>
+      </c>
+      <c r="E105" t="s">
+        <v>20</v>
+      </c>
+      <c r="F105" t="s">
         <v>369</v>
-      </c>
-      <c r="D105" t="s">
-        <v>368</v>
-      </c>
-      <c r="E105" t="s">
-        <v>20</v>
-      </c>
-      <c r="F105" t="s">
-        <v>370</v>
       </c>
       <c r="H105">
         <v>1.26</v>
+      </c>
+    </row>
+    <row r="106" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>195</v>
+      </c>
+      <c r="C106" t="s">
+        <v>371</v>
+      </c>
+      <c r="D106" s="51" t="s">
+        <v>370</v>
+      </c>
+      <c r="E106" t="s">
+        <v>20</v>
+      </c>
+      <c r="F106" t="s">
+        <v>372</v>
+      </c>
+      <c r="H106">
+        <v>7</v>
+      </c>
+      <c r="I106">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added inputs for proportional joystick, linear actuator feedback, photointerrupter, and LCD buttons
</commit_message>
<xml_diff>
--- a/hardware/Wheelchair Receiver BOM.xlsx
+++ b/hardware/Wheelchair Receiver BOM.xlsx
@@ -1125,9 +1125,6 @@
     <t>q4, q5, q6, q7, q8, q9</t>
   </si>
   <si>
-    <t>d17, d18, d19</t>
-  </si>
-  <si>
     <t>8-bit Level Translator</t>
   </si>
   <si>
@@ -1147,6 +1144,9 @@
   </si>
   <si>
     <t>425-1949-5-ND</t>
+  </si>
+  <si>
+    <t>d17, d18, d19, D48, D49</t>
   </si>
 </sst>
 </file>
@@ -2480,8 +2480,8 @@
   <dimension ref="A1:M106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A90" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F101" sqref="F101"/>
+      <pane ySplit="2" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G56" sqref="G56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2513,7 +2513,7 @@
       </c>
       <c r="J1" s="29">
         <f>SUM(Table2[Sub Total])</f>
-        <v>399.28999999999996</v>
+        <v>400.04999999999995</v>
       </c>
       <c r="K1" s="5"/>
     </row>
@@ -4279,7 +4279,7 @@
       </c>
       <c r="K55" s="21"/>
     </row>
-    <row r="56" spans="1:11" s="39" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="39" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A56" s="24">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -4300,17 +4300,17 @@
         <v>263</v>
       </c>
       <c r="G56" s="19" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="H56" s="23">
         <v>0.38</v>
       </c>
       <c r="I56" s="20">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="J56" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.1400000000000001</v>
+        <v>1.9</v>
       </c>
       <c r="K56" s="21"/>
     </row>
@@ -5672,7 +5672,7 @@
         <v>20</v>
       </c>
       <c r="F102" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
     </row>
     <row r="103" spans="1:11" x14ac:dyDescent="0.25">
@@ -5708,16 +5708,16 @@
     </row>
     <row r="105" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C105" t="s">
+        <v>367</v>
+      </c>
+      <c r="D105" t="s">
+        <v>366</v>
+      </c>
+      <c r="E105" t="s">
+        <v>20</v>
+      </c>
+      <c r="F105" t="s">
         <v>368</v>
-      </c>
-      <c r="D105" t="s">
-        <v>367</v>
-      </c>
-      <c r="E105" t="s">
-        <v>20</v>
-      </c>
-      <c r="F105" t="s">
-        <v>369</v>
       </c>
       <c r="H105">
         <v>1.26</v>
@@ -5728,16 +5728,16 @@
         <v>195</v>
       </c>
       <c r="C106" t="s">
+        <v>370</v>
+      </c>
+      <c r="D106" s="51" t="s">
+        <v>369</v>
+      </c>
+      <c r="E106" t="s">
+        <v>20</v>
+      </c>
+      <c r="F106" t="s">
         <v>371</v>
-      </c>
-      <c r="D106" s="51" t="s">
-        <v>370</v>
-      </c>
-      <c r="E106" t="s">
-        <v>20</v>
-      </c>
-      <c r="F106" t="s">
-        <v>372</v>
       </c>
       <c r="H106">
         <v>7</v>

</xml_diff>

<commit_message>
Wheelchair code - changed pins to match rev 2012A hardware, other cleanup
</commit_message>
<xml_diff>
--- a/hardware/Wheelchair Receiver BOM.xlsx
+++ b/hardware/Wheelchair Receiver BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="343">
   <si>
     <t>ID #</t>
   </si>
@@ -1045,6 +1045,15 @@
   </si>
   <si>
     <t>EG4699-ND</t>
+  </si>
+  <si>
+    <t>Keystone Electronics</t>
+  </si>
+  <si>
+    <t>Hex standoff 3/8"</t>
+  </si>
+  <si>
+    <t>7200K-ND</t>
   </si>
 </sst>
 </file>
@@ -1622,7 +1631,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1634,9 +1643,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2422,81 +2428,81 @@
   <dimension ref="A1:M89"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <pane ySplit="2" topLeftCell="A72" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="45" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" style="45" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="45" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" style="45" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="45" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" style="45" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="45" customWidth="1"/>
-    <col min="8" max="8" width="10" style="45" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="45" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="45" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.5703125" style="56" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="45"/>
+    <col min="1" max="1" width="12.140625" style="44" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" style="44" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="44" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" style="44" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="44" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="44" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="44" customWidth="1"/>
+    <col min="8" max="8" width="10" style="44" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="44" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="44" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.5703125" style="55" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="44"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="46"/>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="47" t="s">
+      <c r="A1" s="45"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
+      <c r="H1" s="45"/>
+      <c r="I1" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="48">
+      <c r="J1" s="47">
         <f>SUM(Table2[Sub Total])</f>
-        <v>161.17999999999992</v>
-      </c>
-      <c r="K1" s="49"/>
+        <v>163.89999999999992</v>
+      </c>
+      <c r="K1" s="48"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="50" t="s">
+      <c r="C2" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="50" t="s">
+      <c r="D2" s="49" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="50" t="s">
+      <c r="E2" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="50" t="s">
+      <c r="F2" s="49" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="50" t="s">
+      <c r="G2" s="49" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="51" t="s">
+      <c r="H2" s="50" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="50" t="s">
+      <c r="I2" s="49" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="52" t="s">
+      <c r="K2" s="51" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="1"/>
@@ -2513,476 +2519,476 @@
       </c>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" s="53" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="16">
+    <row r="4" spans="1:11" s="52" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E4" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="11" t="s">
+      <c r="E4" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="11" t="s">
+      <c r="G4" s="10" t="s">
         <v>260</v>
       </c>
-      <c r="H4" s="15">
+      <c r="H4" s="14">
         <v>0.03</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="10">
         <v>48</v>
       </c>
-      <c r="J4" s="15">
+      <c r="J4" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.44</v>
       </c>
-      <c r="K4" s="13"/>
-    </row>
-    <row r="5" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="16">
+      <c r="K4" s="12"/>
+    </row>
+    <row r="5" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
         <f>1+A4</f>
         <v>2</v>
       </c>
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="11" t="s">
+      <c r="E5" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="G5" s="11" t="s">
+      <c r="G5" s="10" t="s">
         <v>171</v>
       </c>
-      <c r="H5" s="15">
+      <c r="H5" s="14">
         <v>0.04</v>
       </c>
-      <c r="I5" s="11">
+      <c r="I5" s="10">
         <v>1</v>
       </c>
-      <c r="J5" s="15">
+      <c r="J5" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.04</v>
       </c>
-      <c r="K5" s="13"/>
-    </row>
-    <row r="6" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="16">
+      <c r="K5" s="12"/>
+    </row>
+    <row r="6" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="15">
         <f>1+A5</f>
         <v>3</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="11" t="s">
+      <c r="E6" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="G6" s="11" t="s">
+      <c r="G6" s="10" t="s">
         <v>261</v>
       </c>
-      <c r="H6" s="15">
+      <c r="H6" s="14">
         <v>0.1</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="10">
         <v>1</v>
       </c>
-      <c r="J6" s="15">
+      <c r="J6" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.1</v>
       </c>
-      <c r="K6" s="13"/>
-    </row>
-    <row r="7" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="16">
+      <c r="K6" s="12"/>
+    </row>
+    <row r="7" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="15">
         <f t="shared" ref="A7:A27" si="0">1+A6</f>
         <v>4</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="10" t="s">
         <v>113</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="11" t="s">
+      <c r="E7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="G7" s="11" t="s">
+      <c r="G7" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="H7" s="15">
+      <c r="H7" s="14">
         <v>0.1</v>
       </c>
-      <c r="I7" s="11">
+      <c r="I7" s="10">
         <v>3</v>
       </c>
-      <c r="J7" s="15">
+      <c r="J7" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.30000000000000004</v>
       </c>
-      <c r="K7" s="13"/>
-    </row>
-    <row r="8" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+      <c r="K7" s="12"/>
+    </row>
+    <row r="8" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="D8" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="E8" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="6" t="s">
         <v>103</v>
       </c>
-      <c r="G8" s="8" t="s">
+      <c r="G8" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="H8" s="15">
+      <c r="H8" s="14">
         <v>0.04</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="10">
         <v>1</v>
       </c>
-      <c r="J8" s="15">
+      <c r="J8" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.04</v>
       </c>
-      <c r="K8" s="10"/>
-    </row>
-    <row r="9" spans="1:11" s="53" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A9" s="57">
+      <c r="K8" s="9"/>
+    </row>
+    <row r="9" spans="1:11" s="52" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A9" s="56">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="C9" s="30" t="s">
+      <c r="C9" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="D9" s="30" t="s">
+      <c r="D9" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="E9" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="30" t="s">
+      <c r="E9" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="58" t="s">
+      <c r="G9" s="57" t="s">
         <v>264</v>
       </c>
-      <c r="H9" s="59">
+      <c r="H9" s="58">
         <v>0.04</v>
       </c>
-      <c r="I9" s="30">
+      <c r="I9" s="29">
         <v>7</v>
       </c>
-      <c r="J9" s="59">
+      <c r="J9" s="58">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="K9" s="60" t="s">
+      <c r="K9" s="59" t="s">
         <v>304</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="16">
+    <row r="10" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="C10" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="11" t="s">
+      <c r="E10" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="11" t="s">
         <v>167</v>
       </c>
-      <c r="H10" s="15">
+      <c r="H10" s="14">
         <v>0.1</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="10">
         <v>1</v>
       </c>
-      <c r="J10" s="15">
+      <c r="J10" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.1</v>
       </c>
-      <c r="K10" s="13"/>
-    </row>
-    <row r="11" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="16">
+      <c r="K10" s="12"/>
+    </row>
+    <row r="11" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="C11" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="D11" s="11" t="s">
+      <c r="D11" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="11" t="s">
+      <c r="E11" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F11" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="11" t="s">
         <v>265</v>
       </c>
-      <c r="H11" s="15">
+      <c r="H11" s="14">
         <v>0.04</v>
       </c>
-      <c r="I11" s="11">
+      <c r="I11" s="10">
         <v>1</v>
       </c>
-      <c r="J11" s="15">
+      <c r="J11" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.04</v>
       </c>
-      <c r="K11" s="13"/>
-    </row>
-    <row r="12" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="57">
+      <c r="K11" s="12"/>
+    </row>
+    <row r="12" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="56">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="29" t="s">
         <v>116</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="E12" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="30" t="s">
+      <c r="E12" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="G12" s="58" t="s">
+      <c r="G12" s="57" t="s">
         <v>266</v>
       </c>
-      <c r="H12" s="59">
+      <c r="H12" s="58">
         <v>0.04</v>
       </c>
-      <c r="I12" s="30">
+      <c r="I12" s="29">
         <v>3</v>
       </c>
-      <c r="J12" s="59">
+      <c r="J12" s="58">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.12</v>
       </c>
-      <c r="K12" s="60" t="s">
+      <c r="K12" s="59" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="16">
+    <row r="13" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="D13" s="11" t="s">
+      <c r="D13" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="11" t="s">
+      <c r="E13" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="10" t="s">
         <v>108</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="H13" s="15">
+      <c r="H13" s="14">
         <v>0.1</v>
       </c>
-      <c r="I13" s="11">
+      <c r="I13" s="10">
         <v>1</v>
       </c>
-      <c r="J13" s="15">
+      <c r="J13" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.1</v>
       </c>
-      <c r="K13" s="13"/>
-    </row>
-    <row r="14" spans="1:11" s="53" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A14" s="16">
+      <c r="K13" s="12"/>
+    </row>
+    <row r="14" spans="1:11" s="52" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
         <f>1+A13</f>
         <v>11</v>
       </c>
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="10" t="s">
         <v>272</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="10" t="s">
         <v>263</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="7" t="s">
+      <c r="E14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>271</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="11" t="s">
         <v>179</v>
       </c>
-      <c r="H14" s="15">
+      <c r="H14" s="14">
         <v>0.03</v>
       </c>
-      <c r="I14" s="12">
+      <c r="I14" s="11">
         <v>8</v>
       </c>
-      <c r="J14" s="15">
+      <c r="J14" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.24</v>
       </c>
-      <c r="K14" s="13"/>
-    </row>
-    <row r="15" spans="1:11" s="53" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A15" s="16">
+      <c r="K14" s="12"/>
+    </row>
+    <row r="15" spans="1:11" s="52" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A15" s="15">
         <f>1+A14</f>
         <v>12</v>
       </c>
-      <c r="B15" s="11" t="s">
+      <c r="B15" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="C15" s="10" t="s">
         <v>215</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="10" t="s">
         <v>180</v>
       </c>
-      <c r="E15" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F15" s="11" t="s">
+      <c r="E15" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>214</v>
       </c>
-      <c r="G15" s="15" t="s">
+      <c r="G15" s="14" t="s">
         <v>181</v>
       </c>
-      <c r="H15" s="15">
+      <c r="H15" s="14">
         <v>0.04</v>
       </c>
-      <c r="I15" s="12">
+      <c r="I15" s="11">
         <v>6</v>
       </c>
-      <c r="J15" s="15">
+      <c r="J15" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.24</v>
       </c>
-      <c r="K15" s="13"/>
-    </row>
-    <row r="16" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="57">
+      <c r="K15" s="12"/>
+    </row>
+    <row r="16" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="56">
         <f>1+A15</f>
         <v>13</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="29" t="s">
         <v>109</v>
       </c>
-      <c r="C16" s="30" t="s">
+      <c r="C16" s="29" t="s">
         <v>269</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="29" t="s">
         <v>267</v>
       </c>
-      <c r="E16" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="F16" s="30" t="s">
+      <c r="E16" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F16" s="29" t="s">
         <v>270</v>
       </c>
-      <c r="G16" s="59" t="s">
+      <c r="G16" s="58" t="s">
         <v>268</v>
       </c>
-      <c r="H16" s="59">
+      <c r="H16" s="58">
         <v>0.03</v>
       </c>
-      <c r="I16" s="58">
+      <c r="I16" s="57">
         <v>2</v>
       </c>
-      <c r="J16" s="59">
+      <c r="J16" s="58">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.06</v>
       </c>
-      <c r="K16" s="60" t="s">
+      <c r="K16" s="59" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="17" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="20">
+    <row r="17" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="19">
         <f>1+A16</f>
         <v>14</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C17" s="21" t="s">
+      <c r="C17" s="20" t="s">
         <v>257</v>
       </c>
       <c r="D17" s="1" t="s">
@@ -2994,46 +3000,46 @@
       <c r="F17" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="G17" s="15" t="s">
+      <c r="G17" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="H17" s="22">
+      <c r="H17" s="21">
         <v>1.05</v>
       </c>
-      <c r="I17" s="29">
+      <c r="I17" s="28">
         <v>1</v>
       </c>
-      <c r="J17" s="22">
+      <c r="J17" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.05</v>
       </c>
-      <c r="K17" s="25"/>
+      <c r="K17" s="24"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="16"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="9"/>
+      <c r="A18" s="15"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="8"/>
       <c r="I18" s="1"/>
       <c r="J18" s="2">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K18" s="10"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="17" t="s">
+      <c r="A19" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="6"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="14"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="13"/>
+      <c r="D19" s="10"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="13"/>
       <c r="G19" s="1"/>
       <c r="H19" s="2"/>
       <c r="I19" s="1"/>
@@ -3041,2228 +3047,2245 @@
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K19" s="10"/>
-    </row>
-    <row r="20" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="16">
+      <c r="K19" s="9"/>
+    </row>
+    <row r="20" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
         <v>1</v>
       </c>
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="18" t="s">
+      <c r="C20" s="17" t="s">
         <v>120</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="E20" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="18" t="s">
+      <c r="E20" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F20" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="7" t="s">
+      <c r="G20" s="6" t="s">
         <v>305</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>1.34</v>
       </c>
-      <c r="I20" s="11">
+      <c r="I20" s="10">
         <v>2</v>
       </c>
-      <c r="J20" s="15">
+      <c r="J20" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>2.68</v>
       </c>
-      <c r="K20" s="10" t="s">
+      <c r="K20" s="9" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="53" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A21" s="16">
+    <row r="21" spans="1:11" s="52" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="B21" s="7" t="s">
+      <c r="B21" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="17" t="s">
         <v>308</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="D21" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="E21" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F21" s="18" t="s">
+      <c r="E21" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F21" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="G21" s="7" t="s">
+      <c r="G21" s="6" t="s">
         <v>183</v>
       </c>
-      <c r="H21" s="9">
+      <c r="H21" s="8">
         <v>0.05</v>
       </c>
-      <c r="I21" s="11">
+      <c r="I21" s="10">
         <v>5</v>
       </c>
-      <c r="J21" s="15">
+      <c r="J21" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.25</v>
       </c>
-      <c r="K21" s="13" t="s">
+      <c r="K21" s="12" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="16">
+    <row r="22" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B22" s="7" t="s">
+      <c r="B22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="D22" s="7" t="s">
+      <c r="D22" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F22" s="7" t="s">
+      <c r="E22" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="G22" s="8" t="s">
+      <c r="G22" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="8">
         <v>0.05</v>
       </c>
-      <c r="I22" s="11">
+      <c r="I22" s="10">
         <v>1</v>
       </c>
-      <c r="J22" s="15">
+      <c r="J22" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.05</v>
       </c>
-      <c r="K22" s="10"/>
-    </row>
-    <row r="23" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="16">
+      <c r="K22" s="9"/>
+    </row>
+    <row r="23" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E23" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="11" t="s">
+      <c r="E23" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F23" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="G23" s="11" t="s">
+      <c r="G23" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="9">
+      <c r="H23" s="8">
         <v>0.05</v>
       </c>
-      <c r="I23" s="11">
+      <c r="I23" s="10">
         <v>1</v>
       </c>
-      <c r="J23" s="15">
+      <c r="J23" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.05</v>
       </c>
-      <c r="K23" s="13"/>
-    </row>
-    <row r="24" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="16">
+      <c r="K23" s="12"/>
+    </row>
+    <row r="24" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="C24" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="D24" s="11" t="s">
+      <c r="D24" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F24" s="11" t="s">
+      <c r="E24" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F24" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G24" s="11" t="s">
+      <c r="G24" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="8">
         <v>0.05</v>
       </c>
-      <c r="I24" s="11">
+      <c r="I24" s="10">
         <v>1</v>
       </c>
-      <c r="J24" s="15">
+      <c r="J24" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.05</v>
       </c>
-      <c r="K24" s="13"/>
-    </row>
-    <row r="25" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="16">
+      <c r="K24" s="12"/>
+    </row>
+    <row r="25" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B25" s="7" t="s">
+      <c r="B25" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="C25" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="D25" s="11" t="s">
+      <c r="D25" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="E25" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="11" t="s">
+      <c r="E25" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F25" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="11" t="s">
+      <c r="G25" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H25" s="15">
+      <c r="H25" s="14">
         <v>0.06</v>
       </c>
-      <c r="I25" s="11">
+      <c r="I25" s="10">
         <v>2</v>
       </c>
-      <c r="J25" s="15">
+      <c r="J25" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.12</v>
       </c>
-      <c r="K25" s="13"/>
-    </row>
-    <row r="26" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="16">
+      <c r="K25" s="12"/>
+    </row>
+    <row r="26" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="C26" s="10" t="s">
         <v>310</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="D26" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E26" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F26" s="11" t="s">
+      <c r="E26" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F26" s="10" t="s">
         <v>311</v>
       </c>
-      <c r="G26" s="11" t="s">
+      <c r="G26" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="H26" s="15">
+      <c r="H26" s="14">
         <v>0.19</v>
       </c>
-      <c r="I26" s="11">
+      <c r="I26" s="10">
         <v>1</v>
       </c>
-      <c r="J26" s="15">
+      <c r="J26" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.19</v>
       </c>
-      <c r="K26" s="13"/>
-    </row>
-    <row r="27" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="16">
+      <c r="K26" s="12"/>
+    </row>
+    <row r="27" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B27" s="7" t="s">
+      <c r="B27" s="6" t="s">
         <v>149</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="C27" s="10" t="s">
         <v>312</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="D27" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="E27" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F27" s="11" t="s">
+      <c r="E27" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F27" s="10" t="s">
         <v>313</v>
       </c>
-      <c r="G27" s="11" t="s">
+      <c r="G27" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H27" s="15">
+      <c r="H27" s="14">
         <v>0.26</v>
       </c>
-      <c r="I27" s="11">
+      <c r="I27" s="10">
         <v>1</v>
       </c>
-      <c r="J27" s="15">
+      <c r="J27" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.26</v>
       </c>
-      <c r="K27" s="13"/>
-    </row>
-    <row r="28" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="16">
+      <c r="K27" s="12"/>
+    </row>
+    <row r="28" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
         <f t="shared" ref="A28:A33" si="1">1+A27</f>
         <v>9</v>
       </c>
-      <c r="B28" s="7" t="s">
+      <c r="B28" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="C28" s="10" t="s">
         <v>314</v>
       </c>
-      <c r="D28" s="11" t="s">
+      <c r="D28" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E28" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F28" s="11" t="s">
+      <c r="E28" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F28" s="10" t="s">
         <v>315</v>
       </c>
-      <c r="G28" s="11" t="s">
+      <c r="G28" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="H28" s="15">
+      <c r="H28" s="14">
         <v>0.16</v>
       </c>
-      <c r="I28" s="12">
+      <c r="I28" s="11">
         <v>1</v>
       </c>
-      <c r="J28" s="15">
+      <c r="J28" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.16</v>
       </c>
-      <c r="K28" s="13"/>
-    </row>
-    <row r="29" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="16">
+      <c r="K28" s="12"/>
+    </row>
+    <row r="29" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="10" t="s">
         <v>306</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="C29" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="D29" s="11" t="s">
+      <c r="D29" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="E29" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F29" s="11" t="s">
+      <c r="E29" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="G29" s="11" t="s">
+      <c r="G29" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="H29" s="15">
+      <c r="H29" s="14">
         <v>0.04</v>
       </c>
-      <c r="I29" s="12">
+      <c r="I29" s="11">
         <v>1</v>
       </c>
-      <c r="J29" s="15">
+      <c r="J29" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.04</v>
       </c>
-      <c r="K29" s="13" t="s">
+      <c r="K29" s="12" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="30" spans="1:11" s="53" customFormat="1" ht="72" x14ac:dyDescent="0.25">
-      <c r="A30" s="61">
+    <row r="30" spans="1:11" s="52" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="A30" s="60">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="C30" s="31" t="s">
+      <c r="C30" s="30" t="s">
         <v>127</v>
       </c>
-      <c r="D30" s="31" t="s">
+      <c r="D30" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="E30" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="F30" s="31" t="s">
+      <c r="E30" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="G30" s="31" t="s">
+      <c r="G30" s="30" t="s">
         <v>254</v>
       </c>
-      <c r="H30" s="62">
+      <c r="H30" s="61">
         <v>0.05</v>
       </c>
-      <c r="I30" s="63">
+      <c r="I30" s="62">
         <v>22</v>
       </c>
-      <c r="J30" s="62">
+      <c r="J30" s="61">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="K30" s="64" t="s">
+      <c r="K30" s="63" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="31" spans="1:11" s="53" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A31" s="61">
+    <row r="31" spans="1:11" s="52" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A31" s="60">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="29" t="s">
         <v>126</v>
       </c>
-      <c r="C31" s="31" t="s">
+      <c r="C31" s="30" t="s">
         <v>128</v>
       </c>
-      <c r="D31" s="31" t="s">
+      <c r="D31" s="30" t="s">
         <v>100</v>
       </c>
-      <c r="E31" s="31" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="31" t="s">
+      <c r="E31" s="30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="G31" s="30" t="s">
+      <c r="G31" s="29" t="s">
         <v>255</v>
       </c>
-      <c r="H31" s="62">
+      <c r="H31" s="61">
         <v>0.3</v>
       </c>
-      <c r="I31" s="63">
+      <c r="I31" s="62">
         <v>6</v>
       </c>
-      <c r="J31" s="62">
+      <c r="J31" s="61">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.7999999999999998</v>
       </c>
-      <c r="K31" s="64" t="s">
+      <c r="K31" s="63" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="32" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="16">
+    <row r="32" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="15">
         <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="10" t="s">
         <v>210</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="C32" s="10" t="s">
         <v>211</v>
       </c>
-      <c r="D32" s="11" t="s">
+      <c r="D32" s="10" t="s">
         <v>184</v>
       </c>
-      <c r="E32" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="11" t="s">
+      <c r="E32" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="G32" s="11" t="s">
+      <c r="G32" s="10" t="s">
         <v>186</v>
       </c>
-      <c r="H32" s="15">
+      <c r="H32" s="14">
         <v>0.26</v>
       </c>
-      <c r="I32" s="12">
+      <c r="I32" s="11">
         <v>4</v>
       </c>
-      <c r="J32" s="15">
+      <c r="J32" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.04</v>
       </c>
-      <c r="K32" s="13"/>
-    </row>
-    <row r="33" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="57">
+      <c r="K32" s="12"/>
+    </row>
+    <row r="33" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="56">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C33" s="30" t="s">
+      <c r="C33" s="29" t="s">
         <v>213</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="29" t="s">
         <v>185</v>
       </c>
-      <c r="E33" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="F33" s="30" t="s">
+      <c r="E33" s="29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="29" t="s">
         <v>212</v>
       </c>
-      <c r="G33" s="30" t="s">
+      <c r="G33" s="29" t="s">
         <v>187</v>
       </c>
-      <c r="H33" s="59">
+      <c r="H33" s="58">
         <v>0.39</v>
       </c>
-      <c r="I33" s="58">
+      <c r="I33" s="57">
         <v>4</v>
       </c>
-      <c r="J33" s="59">
+      <c r="J33" s="58">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.56</v>
       </c>
-      <c r="K33" s="60" t="s">
+      <c r="K33" s="59" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" s="16"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="11"/>
-      <c r="H34" s="15"/>
+      <c r="A34" s="15"/>
+      <c r="B34" s="10"/>
+      <c r="C34" s="10"/>
+      <c r="D34" s="10"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="10"/>
+      <c r="H34" s="14"/>
       <c r="I34" s="1"/>
       <c r="J34" s="2">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K34" s="13"/>
+      <c r="K34" s="12"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B35" s="11"/>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="11"/>
-      <c r="H35" s="15"/>
+      <c r="B35" s="10"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="10"/>
+      <c r="H35" s="14"/>
       <c r="I35" s="1"/>
       <c r="J35" s="2">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K35" s="13"/>
-    </row>
-    <row r="36" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="16">
+      <c r="K35" s="12"/>
+    </row>
+    <row r="36" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="15">
         <v>1</v>
       </c>
-      <c r="B36" s="11" t="s">
+      <c r="B36" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="C36" s="10" t="s">
         <v>130</v>
       </c>
-      <c r="D36" s="13" t="s">
+      <c r="D36" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="E36" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F36" s="11" t="s">
+      <c r="E36" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G36" s="11" t="s">
+      <c r="G36" s="10" t="s">
         <v>274</v>
       </c>
-      <c r="H36" s="15">
+      <c r="H36" s="14">
         <v>3.47</v>
       </c>
-      <c r="I36" s="11">
+      <c r="I36" s="10">
         <v>1</v>
       </c>
-      <c r="J36" s="15">
+      <c r="J36" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>3.47</v>
       </c>
-      <c r="K36" s="13"/>
-    </row>
-    <row r="37" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="16">
+      <c r="K36" s="12"/>
+    </row>
+    <row r="37" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="15">
         <f>1+A36</f>
         <v>2</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="C37" s="11" t="s">
+      <c r="C37" s="10" t="s">
         <v>275</v>
       </c>
-      <c r="D37" s="11" t="s">
+      <c r="D37" s="10" t="s">
         <v>276</v>
       </c>
-      <c r="E37" s="11" t="s">
+      <c r="E37" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F37" s="11" t="s">
+      <c r="F37" s="10" t="s">
         <v>277</v>
       </c>
-      <c r="G37" s="11" t="s">
+      <c r="G37" s="10" t="s">
         <v>278</v>
       </c>
-      <c r="H37" s="15">
+      <c r="H37" s="14">
         <v>3.6</v>
       </c>
-      <c r="I37" s="12">
+      <c r="I37" s="11">
         <v>1</v>
       </c>
-      <c r="J37" s="15">
+      <c r="J37" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>3.6</v>
       </c>
-      <c r="K37" s="13"/>
-    </row>
-    <row r="38" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="16">
+      <c r="K37" s="12"/>
+    </row>
+    <row r="38" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="15">
         <f t="shared" ref="A38:A39" si="2">1+A37</f>
         <v>3</v>
       </c>
-      <c r="B38" s="11" t="s">
+      <c r="B38" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="C38" s="10" t="s">
         <v>280</v>
       </c>
-      <c r="D38" s="26" t="s">
+      <c r="D38" s="25" t="s">
         <v>281</v>
       </c>
-      <c r="E38" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F38" s="21" t="s">
+      <c r="E38" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="20" t="s">
         <v>282</v>
       </c>
-      <c r="G38" s="11" t="s">
+      <c r="G38" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="H38" s="22">
+      <c r="H38" s="21">
         <v>4.3499999999999996</v>
       </c>
-      <c r="I38" s="29">
+      <c r="I38" s="28">
         <v>4</v>
       </c>
-      <c r="J38" s="22">
+      <c r="J38" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>17.399999999999999</v>
       </c>
-      <c r="K38" s="25"/>
-    </row>
-    <row r="39" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="16">
+      <c r="K38" s="24"/>
+    </row>
+    <row r="39" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="15">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="B39" s="11" t="s">
+      <c r="B39" s="10" t="s">
         <v>134</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="10" t="s">
         <v>229</v>
       </c>
-      <c r="D39" s="11" t="s">
+      <c r="D39" s="10" t="s">
         <v>237</v>
       </c>
-      <c r="E39" s="11" t="s">
+      <c r="E39" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F39" s="21" t="s">
+      <c r="F39" s="20" t="s">
         <v>230</v>
       </c>
-      <c r="G39" s="11" t="s">
+      <c r="G39" s="10" t="s">
         <v>283</v>
       </c>
-      <c r="H39" s="22">
+      <c r="H39" s="21">
         <v>7.5</v>
       </c>
-      <c r="I39" s="29">
+      <c r="I39" s="28">
         <v>1</v>
       </c>
-      <c r="J39" s="22">
+      <c r="J39" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>7.5</v>
       </c>
-      <c r="K39" s="25"/>
-    </row>
-    <row r="40" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="16">
+      <c r="K39" s="24"/>
+    </row>
+    <row r="40" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="15">
         <f>1+A39</f>
         <v>5</v>
       </c>
-      <c r="B40" s="11" t="s">
+      <c r="B40" s="10" t="s">
         <v>189</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="C40" s="10" t="s">
         <v>191</v>
       </c>
-      <c r="D40" s="11" t="s">
+      <c r="D40" s="10" t="s">
         <v>190</v>
       </c>
-      <c r="E40" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="11" t="s">
+      <c r="E40" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="10" t="s">
         <v>188</v>
       </c>
-      <c r="G40" s="11" t="s">
+      <c r="G40" s="10" t="s">
         <v>284</v>
       </c>
-      <c r="H40" s="15">
+      <c r="H40" s="14">
         <v>5.65</v>
       </c>
-      <c r="I40" s="12">
+      <c r="I40" s="11">
         <v>4</v>
       </c>
-      <c r="J40" s="15">
+      <c r="J40" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>22.6</v>
       </c>
-      <c r="K40" s="13"/>
-    </row>
-    <row r="41" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="20">
+      <c r="K40" s="12"/>
+    </row>
+    <row r="41" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="19">
         <f>1+A40</f>
         <v>6</v>
       </c>
-      <c r="B41" s="11" t="s">
+      <c r="B41" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="C41" s="21" t="s">
+      <c r="C41" s="20" t="s">
         <v>243</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="D41" s="20" t="s">
         <v>245</v>
       </c>
-      <c r="E41" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F41" s="21" t="s">
+      <c r="E41" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="20" t="s">
         <v>244</v>
       </c>
-      <c r="G41" s="21" t="s">
+      <c r="G41" s="20" t="s">
         <v>242</v>
       </c>
-      <c r="H41" s="22">
+      <c r="H41" s="21">
         <v>0.62</v>
       </c>
-      <c r="I41" s="29">
+      <c r="I41" s="28">
         <v>1</v>
       </c>
-      <c r="J41" s="22">
+      <c r="J41" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.62</v>
       </c>
-      <c r="K41" s="25"/>
-    </row>
-    <row r="42" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="20">
+      <c r="K41" s="24"/>
+    </row>
+    <row r="42" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="19">
         <f>1+A41</f>
         <v>7</v>
       </c>
-      <c r="B42" s="11" t="s">
+      <c r="B42" s="10" t="s">
         <v>286</v>
       </c>
-      <c r="C42" s="21" t="s">
+      <c r="C42" s="20" t="s">
         <v>248</v>
       </c>
-      <c r="D42" s="21" t="s">
+      <c r="D42" s="20" t="s">
         <v>247</v>
       </c>
-      <c r="E42" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F42" s="21" t="s">
+      <c r="E42" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="20" t="s">
         <v>249</v>
       </c>
-      <c r="G42" s="11" t="s">
+      <c r="G42" s="10" t="s">
         <v>285</v>
       </c>
-      <c r="H42" s="22">
+      <c r="H42" s="21">
         <v>1.26</v>
       </c>
-      <c r="I42" s="29">
+      <c r="I42" s="28">
         <v>2</v>
       </c>
-      <c r="J42" s="22">
+      <c r="J42" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>2.52</v>
       </c>
-      <c r="K42" s="25"/>
-    </row>
-    <row r="43" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="32">
+      <c r="K42" s="24"/>
+    </row>
+    <row r="43" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="31">
         <f>1+A42</f>
         <v>8</v>
       </c>
-      <c r="B43" s="33" t="s">
+      <c r="B43" s="32" t="s">
         <v>132</v>
       </c>
-      <c r="C43" s="33" t="s">
+      <c r="C43" s="32" t="s">
         <v>251</v>
       </c>
-      <c r="D43" s="33" t="s">
+      <c r="D43" s="32" t="s">
         <v>250</v>
       </c>
-      <c r="E43" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="F43" s="33" t="s">
+      <c r="E43" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="32" t="s">
         <v>252</v>
       </c>
-      <c r="G43" s="33"/>
-      <c r="H43" s="34">
+      <c r="G43" s="32"/>
+      <c r="H43" s="33">
         <v>7</v>
       </c>
-      <c r="I43" s="35">
+      <c r="I43" s="34">
         <v>0</v>
       </c>
-      <c r="J43" s="34">
+      <c r="J43" s="33">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K43" s="36" t="s">
+      <c r="K43" s="35" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" s="16"/>
-      <c r="B44" s="7"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="7"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="7"/>
-      <c r="G44" s="7"/>
-      <c r="H44" s="9"/>
+      <c r="A44" s="15"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+      <c r="F44" s="6"/>
+      <c r="G44" s="6"/>
+      <c r="H44" s="8"/>
       <c r="I44" s="1"/>
       <c r="J44" s="2">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K44" s="10"/>
+      <c r="K44" s="9"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="B45" s="7"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="7"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="7"/>
-      <c r="G45" s="7"/>
-      <c r="H45" s="9"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+      <c r="F45" s="6"/>
+      <c r="G45" s="6"/>
+      <c r="H45" s="8"/>
       <c r="I45" s="1"/>
       <c r="J45" s="2">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K45" s="10"/>
-    </row>
-    <row r="46" spans="1:11" s="53" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A46" s="32">
+      <c r="K45" s="9"/>
+    </row>
+    <row r="46" spans="1:11" s="52" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A46" s="31">
         <v>1</v>
       </c>
-      <c r="B46" s="37" t="s">
+      <c r="B46" s="36" t="s">
         <v>135</v>
       </c>
-      <c r="C46" s="37" t="s">
+      <c r="C46" s="36" t="s">
         <v>136</v>
       </c>
-      <c r="D46" s="38" t="s">
+      <c r="D46" s="37" t="s">
         <v>89</v>
       </c>
-      <c r="E46" s="37" t="s">
-        <v>18</v>
-      </c>
-      <c r="F46" s="37" t="s">
+      <c r="E46" s="36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="G46" s="37" t="s">
+      <c r="G46" s="36" t="s">
         <v>246</v>
       </c>
-      <c r="H46" s="39">
+      <c r="H46" s="38">
         <v>0.49</v>
       </c>
-      <c r="I46" s="33">
+      <c r="I46" s="32">
         <v>0</v>
       </c>
-      <c r="J46" s="34">
+      <c r="J46" s="33">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K46" s="36" t="s">
+      <c r="K46" s="35" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="53" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="16">
+    <row r="47" spans="1:11" s="52" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="15">
         <f>1+A46</f>
         <v>2</v>
       </c>
-      <c r="B47" s="7" t="s">
+      <c r="B47" s="6" t="s">
         <v>131</v>
       </c>
-      <c r="C47" s="7" t="s">
+      <c r="C47" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="D47" s="10" t="s">
+      <c r="D47" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E47" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F47" s="7" t="s">
+      <c r="E47" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G47" s="7" t="s">
+      <c r="G47" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="H47" s="9">
+      <c r="H47" s="8">
         <v>0.69</v>
       </c>
-      <c r="I47" s="11">
+      <c r="I47" s="10">
         <v>8</v>
       </c>
-      <c r="J47" s="15">
+      <c r="J47" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>5.52</v>
       </c>
-      <c r="K47" s="25"/>
-    </row>
-    <row r="48" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="16">
+      <c r="K47" s="24"/>
+    </row>
+    <row r="48" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="15">
         <f>1+A47</f>
         <v>3</v>
       </c>
-      <c r="B48" s="11" t="s">
+      <c r="B48" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="C48" s="18" t="s">
+      <c r="C48" s="17" t="s">
         <v>139</v>
       </c>
-      <c r="D48" s="13" t="s">
+      <c r="D48" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="E48" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F48" s="18" t="s">
+      <c r="E48" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="G48" s="11" t="s">
+      <c r="G48" s="10" t="s">
         <v>273</v>
       </c>
-      <c r="H48" s="15">
+      <c r="H48" s="14">
         <v>1.89</v>
       </c>
-      <c r="I48" s="11">
+      <c r="I48" s="10">
         <v>1</v>
       </c>
-      <c r="J48" s="15">
+      <c r="J48" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.89</v>
       </c>
-      <c r="K48" s="25"/>
-    </row>
-    <row r="49" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="16">
+      <c r="K48" s="24"/>
+    </row>
+    <row r="49" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="15">
         <f t="shared" ref="A49:A56" si="3">1+A48</f>
         <v>4</v>
       </c>
-      <c r="B49" s="7" t="s">
+      <c r="B49" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="C49" s="18" t="s">
+      <c r="C49" s="17" t="s">
         <v>141</v>
       </c>
-      <c r="D49" s="10" t="s">
+      <c r="D49" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="E49" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F49" s="7" t="s">
+      <c r="E49" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="G49" s="7" t="s">
+      <c r="G49" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="H49" s="9">
+      <c r="H49" s="8">
         <v>0.51</v>
       </c>
-      <c r="I49" s="11">
+      <c r="I49" s="10">
         <v>5</v>
       </c>
-      <c r="J49" s="15">
+      <c r="J49" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>2.5499999999999998</v>
       </c>
-      <c r="K49" s="25"/>
-    </row>
-    <row r="50" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="16">
+      <c r="K49" s="24"/>
+    </row>
+    <row r="50" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="15">
         <f t="shared" si="3"/>
         <v>5</v>
       </c>
-      <c r="B50" s="11" t="s">
+      <c r="B50" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="C50" s="18" t="s">
+      <c r="C50" s="17" t="s">
         <v>143</v>
       </c>
-      <c r="D50" s="13" t="s">
+      <c r="D50" s="12" t="s">
         <v>301</v>
       </c>
-      <c r="E50" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F50" s="11" t="s">
+      <c r="E50" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="G50" s="11" t="s">
+      <c r="G50" s="10" t="s">
         <v>302</v>
       </c>
-      <c r="H50" s="15">
+      <c r="H50" s="14">
         <v>0.46</v>
       </c>
-      <c r="I50" s="11">
+      <c r="I50" s="10">
         <v>1</v>
       </c>
-      <c r="J50" s="15">
+      <c r="J50" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.46</v>
       </c>
-      <c r="K50" s="25"/>
-    </row>
-    <row r="51" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="16">
+      <c r="K50" s="24"/>
+    </row>
+    <row r="51" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="15">
         <f t="shared" si="3"/>
         <v>6</v>
       </c>
-      <c r="B51" s="11" t="s">
+      <c r="B51" s="10" t="s">
         <v>144</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="C51" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D51" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E51" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F51" s="11" t="s">
+      <c r="E51" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" s="10" t="s">
         <v>81</v>
       </c>
-      <c r="G51" s="11" t="s">
+      <c r="G51" s="10" t="s">
         <v>288</v>
       </c>
-      <c r="H51" s="15">
+      <c r="H51" s="14">
         <v>0.47</v>
       </c>
-      <c r="I51" s="11">
+      <c r="I51" s="10">
         <v>1</v>
       </c>
-      <c r="J51" s="15">
+      <c r="J51" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.47</v>
       </c>
-      <c r="K51" s="13"/>
-    </row>
-    <row r="52" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="16">
+      <c r="K51" s="12"/>
+    </row>
+    <row r="52" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="15">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-      <c r="B52" s="11" t="s">
+      <c r="B52" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="C52" s="10" t="s">
         <v>147</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="D52" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="E52" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F52" s="11" t="s">
+      <c r="E52" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F52" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="G52" s="11" t="s">
+      <c r="G52" s="10" t="s">
         <v>300</v>
       </c>
-      <c r="H52" s="15">
+      <c r="H52" s="14">
         <v>0.95</v>
       </c>
-      <c r="I52" s="11">
+      <c r="I52" s="10">
         <v>1</v>
       </c>
-      <c r="J52" s="15">
+      <c r="J52" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.95</v>
       </c>
-      <c r="K52" s="10"/>
-    </row>
-    <row r="53" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="16">
+      <c r="K52" s="9"/>
+    </row>
+    <row r="53" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="15">
         <f t="shared" si="3"/>
         <v>8</v>
       </c>
-      <c r="B53" s="11" t="s">
+      <c r="B53" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="C53" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="D53" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E53" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F53" s="11" t="s">
+      <c r="E53" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="G53" s="11" t="s">
+      <c r="G53" s="10" t="s">
         <v>169</v>
       </c>
-      <c r="H53" s="15">
+      <c r="H53" s="14">
         <v>0.1</v>
       </c>
-      <c r="I53" s="11">
+      <c r="I53" s="10">
         <v>1</v>
       </c>
-      <c r="J53" s="15">
+      <c r="J53" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.1</v>
       </c>
-      <c r="K53" s="13"/>
-    </row>
-    <row r="54" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="16">
+      <c r="K53" s="12"/>
+    </row>
+    <row r="54" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="15">
         <f t="shared" si="3"/>
         <v>9</v>
       </c>
-      <c r="B54" s="11" t="s">
+      <c r="B54" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="C54" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="D54" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="E54" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F54" s="11" t="s">
+      <c r="E54" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="G54" s="11" t="s">
+      <c r="G54" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="H54" s="15">
+      <c r="H54" s="14">
         <v>0.1</v>
       </c>
-      <c r="I54" s="11">
+      <c r="I54" s="10">
         <v>1</v>
       </c>
-      <c r="J54" s="15">
+      <c r="J54" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.1</v>
       </c>
-      <c r="K54" s="13"/>
-    </row>
-    <row r="55" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="16">
+      <c r="K54" s="12"/>
+    </row>
+    <row r="55" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="15">
         <f t="shared" si="3"/>
         <v>10</v>
       </c>
-      <c r="B55" s="11" t="s">
+      <c r="B55" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="C55" s="10" t="s">
         <v>151</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="D55" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E55" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F55" s="11" t="s">
+      <c r="E55" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F55" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="G55" s="11" t="s">
+      <c r="G55" s="10" t="s">
         <v>170</v>
       </c>
-      <c r="H55" s="15">
+      <c r="H55" s="14">
         <v>0.1</v>
       </c>
-      <c r="I55" s="11">
+      <c r="I55" s="10">
         <v>1</v>
       </c>
-      <c r="J55" s="15">
+      <c r="J55" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.1</v>
       </c>
-      <c r="K55" s="13"/>
-    </row>
-    <row r="56" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="16">
+      <c r="K55" s="12"/>
+    </row>
+    <row r="56" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="15">
         <f t="shared" si="3"/>
         <v>11</v>
       </c>
-      <c r="B56" s="11" t="s">
+      <c r="B56" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="C56" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="D56" s="11" t="s">
+      <c r="D56" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="E56" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F56" s="11" t="s">
+      <c r="E56" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F56" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="G56" s="11" t="s">
+      <c r="G56" s="10" t="s">
         <v>299</v>
       </c>
-      <c r="H56" s="15">
+      <c r="H56" s="14">
         <v>1.5</v>
       </c>
-      <c r="I56" s="11">
+      <c r="I56" s="10">
         <v>1</v>
       </c>
-      <c r="J56" s="15">
+      <c r="J56" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.5</v>
       </c>
-      <c r="K56" s="13"/>
-    </row>
-    <row r="57" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="32">
+      <c r="K56" s="12"/>
+    </row>
+    <row r="57" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="31">
         <f>1+A56</f>
         <v>12</v>
       </c>
-      <c r="B57" s="33" t="s">
+      <c r="B57" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="C57" s="33" t="s">
+      <c r="C57" s="32" t="s">
         <v>195</v>
       </c>
-      <c r="D57" s="33" t="s">
+      <c r="D57" s="32" t="s">
         <v>194</v>
       </c>
-      <c r="E57" s="33" t="s">
-        <v>18</v>
-      </c>
-      <c r="F57" s="33" t="s">
+      <c r="E57" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="G57" s="33" t="s">
+      <c r="G57" s="32" t="s">
         <v>193</v>
       </c>
-      <c r="H57" s="34">
+      <c r="H57" s="33">
         <v>0.49</v>
       </c>
-      <c r="I57" s="35">
+      <c r="I57" s="34">
         <v>0</v>
       </c>
-      <c r="J57" s="34">
+      <c r="J57" s="33">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K57" s="36" t="s">
+      <c r="K57" s="35" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="58" spans="1:11" s="53" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A58" s="16">
+    <row r="58" spans="1:11" s="52" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A58" s="15">
         <f t="shared" ref="A58:A63" si="4">1+A57</f>
         <v>13</v>
       </c>
-      <c r="B58" s="11" t="s">
+      <c r="B58" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="C58" s="10" t="s">
         <v>198</v>
       </c>
-      <c r="D58" s="11" t="s">
+      <c r="D58" s="10" t="s">
         <v>197</v>
       </c>
-      <c r="E58" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F58" s="11" t="s">
+      <c r="E58" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F58" s="10" t="s">
         <v>176</v>
       </c>
-      <c r="G58" s="11" t="s">
+      <c r="G58" s="10" t="s">
         <v>292</v>
       </c>
-      <c r="H58" s="15">
+      <c r="H58" s="14">
         <v>1</v>
       </c>
-      <c r="I58" s="12">
+      <c r="I58" s="11">
         <v>8</v>
       </c>
-      <c r="J58" s="15">
+      <c r="J58" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>8</v>
       </c>
-      <c r="K58" s="13"/>
-    </row>
-    <row r="59" spans="1:11" s="53" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A59" s="16">
+      <c r="K58" s="12"/>
+    </row>
+    <row r="59" spans="1:11" s="52" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A59" s="15">
         <f t="shared" si="4"/>
         <v>14</v>
       </c>
-      <c r="B59" s="11" t="s">
+      <c r="B59" s="10" t="s">
         <v>140</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="C59" s="10" t="s">
         <v>199</v>
       </c>
-      <c r="D59" s="11" t="s">
+      <c r="D59" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="E59" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F59" s="11" t="s">
+      <c r="E59" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F59" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="G59" s="11" t="s">
+      <c r="G59" s="10" t="s">
         <v>290</v>
       </c>
-      <c r="H59" s="15">
+      <c r="H59" s="14">
         <v>0.38</v>
       </c>
-      <c r="I59" s="12">
+      <c r="I59" s="11">
         <v>5</v>
       </c>
-      <c r="J59" s="15">
+      <c r="J59" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.9</v>
       </c>
-      <c r="K59" s="13"/>
-    </row>
-    <row r="60" spans="1:11" s="53" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A60" s="16">
+      <c r="K59" s="12"/>
+    </row>
+    <row r="60" spans="1:11" s="52" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A60" s="15">
         <f t="shared" si="4"/>
         <v>15</v>
       </c>
-      <c r="B60" s="11" t="s">
+      <c r="B60" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="C60" s="10" t="s">
         <v>202</v>
       </c>
-      <c r="D60" s="11" t="s">
+      <c r="D60" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="E60" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F60" s="11" t="s">
+      <c r="E60" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" s="10" t="s">
         <v>173</v>
       </c>
-      <c r="G60" s="11" t="s">
+      <c r="G60" s="10" t="s">
         <v>289</v>
       </c>
-      <c r="H60" s="15">
+      <c r="H60" s="14">
         <v>0.56999999999999995</v>
       </c>
-      <c r="I60" s="12">
+      <c r="I60" s="11">
         <v>9</v>
       </c>
-      <c r="J60" s="15">
+      <c r="J60" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>5.13</v>
       </c>
-      <c r="K60" s="13"/>
-    </row>
-    <row r="61" spans="1:11" s="53" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="20">
+      <c r="K60" s="12"/>
+    </row>
+    <row r="61" spans="1:11" s="52" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="19">
         <f>1+A60</f>
         <v>16</v>
       </c>
-      <c r="B61" s="11" t="s">
+      <c r="B61" s="10" t="s">
         <v>201</v>
       </c>
-      <c r="C61" s="21" t="s">
+      <c r="C61" s="20" t="s">
         <v>240</v>
       </c>
-      <c r="D61" s="21" t="s">
+      <c r="D61" s="20" t="s">
         <v>238</v>
       </c>
-      <c r="E61" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F61" s="21" t="s">
+      <c r="E61" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" s="20" t="s">
         <v>239</v>
       </c>
-      <c r="G61" s="11" t="s">
+      <c r="G61" s="10" t="s">
         <v>259</v>
       </c>
-      <c r="H61" s="22">
+      <c r="H61" s="21">
         <v>0.49</v>
       </c>
-      <c r="I61" s="29">
+      <c r="I61" s="28">
         <v>4</v>
       </c>
-      <c r="J61" s="22">
+      <c r="J61" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.96</v>
       </c>
-      <c r="K61" s="25"/>
-    </row>
-    <row r="62" spans="1:11" s="53" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A62" s="20">
+      <c r="K61" s="24"/>
+    </row>
+    <row r="62" spans="1:11" s="52" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A62" s="19">
         <f>1+A61</f>
         <v>17</v>
       </c>
-      <c r="B62" s="11" t="s">
+      <c r="B62" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="C62" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D62" s="11" t="s">
+      <c r="D62" s="10" t="s">
         <v>203</v>
       </c>
-      <c r="E62" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F62" s="11" t="s">
+      <c r="E62" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F62" s="10" t="s">
         <v>177</v>
       </c>
-      <c r="G62" s="11" t="s">
+      <c r="G62" s="10" t="s">
         <v>293</v>
       </c>
-      <c r="H62" s="15">
+      <c r="H62" s="14">
         <v>0.3</v>
       </c>
-      <c r="I62" s="12">
+      <c r="I62" s="11">
         <v>8</v>
       </c>
-      <c r="J62" s="15">
+      <c r="J62" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>2.4</v>
       </c>
-      <c r="K62" s="13"/>
-    </row>
-    <row r="63" spans="1:11" s="53" customFormat="1" ht="36" x14ac:dyDescent="0.25">
-      <c r="A63" s="16">
+      <c r="K62" s="12"/>
+    </row>
+    <row r="63" spans="1:11" s="52" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+      <c r="A63" s="15">
         <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="B63" s="11" t="s">
+      <c r="B63" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="C63" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="D63" s="11" t="s">
+      <c r="D63" s="10" t="s">
         <v>207</v>
       </c>
-      <c r="E63" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F63" s="11" t="s">
+      <c r="E63" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F63" s="10" t="s">
         <v>178</v>
       </c>
-      <c r="G63" s="11" t="s">
+      <c r="G63" s="10" t="s">
         <v>294</v>
       </c>
-      <c r="H63" s="15">
+      <c r="H63" s="14">
         <v>0.34</v>
       </c>
-      <c r="I63" s="12">
+      <c r="I63" s="11">
         <v>8</v>
       </c>
-      <c r="J63" s="15">
+      <c r="J63" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>2.72</v>
       </c>
-      <c r="K63" s="13"/>
-    </row>
-    <row r="64" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="40">
+      <c r="K63" s="12"/>
+    </row>
+    <row r="64" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="39">
         <f>1+A63</f>
         <v>19</v>
       </c>
-      <c r="B64" s="41" t="s">
+      <c r="B64" s="40" t="s">
         <v>223</v>
       </c>
-      <c r="C64" s="41" t="s">
+      <c r="C64" s="40" t="s">
         <v>224</v>
       </c>
-      <c r="D64" s="41" t="s">
+      <c r="D64" s="40" t="s">
         <v>225</v>
       </c>
-      <c r="E64" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F64" s="41" t="s">
+      <c r="E64" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="40" t="s">
         <v>222</v>
       </c>
-      <c r="G64" s="41"/>
-      <c r="H64" s="42">
+      <c r="G64" s="40"/>
+      <c r="H64" s="41">
         <v>0.48</v>
       </c>
-      <c r="I64" s="43">
+      <c r="I64" s="42">
         <v>0</v>
       </c>
-      <c r="J64" s="42">
+      <c r="J64" s="41">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K64" s="44" t="s">
+      <c r="K64" s="43" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="65" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="40">
+    <row r="65" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="39">
         <f>1+A64</f>
         <v>20</v>
       </c>
-      <c r="B65" s="41" t="s">
+      <c r="B65" s="40" t="s">
         <v>223</v>
       </c>
-      <c r="C65" s="41" t="s">
+      <c r="C65" s="40" t="s">
         <v>228</v>
       </c>
-      <c r="D65" s="41" t="s">
+      <c r="D65" s="40" t="s">
         <v>227</v>
       </c>
-      <c r="E65" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F65" s="41" t="s">
+      <c r="E65" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" s="40" t="s">
         <v>226</v>
       </c>
-      <c r="G65" s="41"/>
-      <c r="H65" s="42">
+      <c r="G65" s="40"/>
+      <c r="H65" s="41">
         <v>4</v>
       </c>
-      <c r="I65" s="43">
+      <c r="I65" s="42">
         <v>0</v>
       </c>
-      <c r="J65" s="42">
+      <c r="J65" s="41">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K65" s="44" t="s">
+      <c r="K65" s="43" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="66" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="20">
+    <row r="66" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="19">
         <f>1+A65</f>
         <v>21</v>
       </c>
-      <c r="B66" s="21" t="s">
+      <c r="B66" s="20" t="s">
         <v>316</v>
       </c>
-      <c r="C66" s="21" t="s">
+      <c r="C66" s="20" t="s">
         <v>317</v>
       </c>
-      <c r="D66" s="11" t="s">
+      <c r="D66" s="10" t="s">
         <v>234</v>
       </c>
-      <c r="E66" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F66" s="21" t="s">
+      <c r="E66" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" s="20" t="s">
         <v>235</v>
       </c>
-      <c r="G66" s="21"/>
-      <c r="H66" s="22">
+      <c r="G66" s="20"/>
+      <c r="H66" s="21">
         <v>11.7</v>
       </c>
-      <c r="I66" s="29">
+      <c r="I66" s="28">
         <v>1</v>
       </c>
-      <c r="J66" s="22">
+      <c r="J66" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>11.7</v>
       </c>
-      <c r="K66" s="13" t="s">
+      <c r="K66" s="12" t="s">
         <v>318</v>
       </c>
     </row>
-    <row r="67" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="16">
+    <row r="67" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="15">
         <f>1+A66</f>
         <v>22</v>
       </c>
-      <c r="B67" s="11" t="s">
+      <c r="B67" s="10" t="s">
         <v>320</v>
       </c>
-      <c r="C67" s="11" t="s">
+      <c r="C67" s="10" t="s">
         <v>319</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D67" s="10" t="s">
         <v>236</v>
       </c>
-      <c r="E67" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F67" s="11" t="s">
+      <c r="E67" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="G67" s="11"/>
-      <c r="H67" s="15">
+      <c r="G67" s="10"/>
+      <c r="H67" s="14">
         <v>1.44</v>
       </c>
-      <c r="I67" s="12">
+      <c r="I67" s="11">
         <v>2</v>
       </c>
-      <c r="J67" s="15">
+      <c r="J67" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>2.88</v>
       </c>
-      <c r="K67" s="13"/>
+      <c r="K67" s="12"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" s="20"/>
-      <c r="B68" s="27"/>
-      <c r="C68" s="27"/>
-      <c r="D68" s="27"/>
-      <c r="E68" s="27"/>
-      <c r="F68" s="27"/>
-      <c r="G68" s="27"/>
-      <c r="H68" s="24"/>
-      <c r="I68" s="23"/>
-      <c r="J68" s="24">
+      <c r="A68" s="19"/>
+      <c r="B68" s="26"/>
+      <c r="C68" s="26"/>
+      <c r="D68" s="26"/>
+      <c r="E68" s="26"/>
+      <c r="F68" s="26"/>
+      <c r="G68" s="26"/>
+      <c r="H68" s="23"/>
+      <c r="I68" s="22"/>
+      <c r="J68" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K68" s="28"/>
+      <c r="K68" s="27"/>
     </row>
     <row r="69" spans="1:11" ht="24" x14ac:dyDescent="0.25">
-      <c r="A69" s="20" t="s">
+      <c r="A69" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B69" s="27"/>
-      <c r="C69" s="27"/>
-      <c r="D69" s="27"/>
-      <c r="E69" s="27"/>
-      <c r="F69" s="27"/>
-      <c r="G69" s="27"/>
-      <c r="H69" s="24"/>
-      <c r="I69" s="23"/>
-      <c r="J69" s="24">
+      <c r="B69" s="26"/>
+      <c r="C69" s="26"/>
+      <c r="D69" s="26"/>
+      <c r="E69" s="26"/>
+      <c r="F69" s="26"/>
+      <c r="G69" s="26"/>
+      <c r="H69" s="23"/>
+      <c r="I69" s="22"/>
+      <c r="J69" s="23">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K69" s="28"/>
-    </row>
-    <row r="70" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="40">
+      <c r="K69" s="27"/>
+    </row>
+    <row r="70" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="39">
         <f>1</f>
         <v>1</v>
       </c>
-      <c r="B70" s="33" t="s">
+      <c r="B70" s="32" t="s">
         <v>156</v>
       </c>
-      <c r="C70" s="41" t="s">
+      <c r="C70" s="40" t="s">
         <v>155</v>
       </c>
-      <c r="D70" s="33" t="s">
+      <c r="D70" s="32" t="s">
         <v>324</v>
       </c>
-      <c r="E70" s="33" t="s">
+      <c r="E70" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="F70" s="33" t="s">
+      <c r="F70" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="G70" s="33"/>
-      <c r="H70" s="34">
+      <c r="G70" s="32"/>
+      <c r="H70" s="33">
         <v>0.67</v>
       </c>
-      <c r="I70" s="33">
+      <c r="I70" s="32">
         <v>0</v>
       </c>
-      <c r="J70" s="42">
+      <c r="J70" s="41">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K70" s="36" t="s">
+      <c r="K70" s="35" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="71" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="20">
+    <row r="71" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="19">
         <f t="shared" ref="A71:A79" si="5">1+A70</f>
         <v>2</v>
       </c>
-      <c r="B71" s="11" t="s">
+      <c r="B71" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="C71" s="21" t="s">
+      <c r="C71" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="D71" s="21" t="s">
+      <c r="D71" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="E71" s="21" t="s">
+      <c r="E71" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F71" s="21" t="s">
+      <c r="F71" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="G71" s="21"/>
-      <c r="H71" s="22">
+      <c r="G71" s="20"/>
+      <c r="H71" s="21">
         <v>1.04</v>
       </c>
-      <c r="I71" s="29">
+      <c r="I71" s="28">
         <v>6</v>
       </c>
-      <c r="J71" s="22">
+      <c r="J71" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>6.24</v>
       </c>
-      <c r="K71" s="13" t="s">
+      <c r="K71" s="12" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="72" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="20">
+    <row r="72" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="19">
         <f t="shared" si="5"/>
         <v>3</v>
       </c>
-      <c r="B72" s="11" t="s">
+      <c r="B72" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="C72" s="21" t="s">
+      <c r="C72" s="20" t="s">
         <v>159</v>
       </c>
-      <c r="D72" s="21" t="s">
+      <c r="D72" s="20" t="s">
         <v>71</v>
       </c>
-      <c r="E72" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F72" s="21" t="s">
+      <c r="E72" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F72" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="G72" s="21"/>
-      <c r="H72" s="22">
+      <c r="G72" s="20"/>
+      <c r="H72" s="21">
         <v>1.62</v>
       </c>
-      <c r="I72" s="29">
+      <c r="I72" s="28">
         <v>1</v>
       </c>
-      <c r="J72" s="22">
+      <c r="J72" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.62</v>
       </c>
-      <c r="K72" s="25"/>
-    </row>
-    <row r="73" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="20">
+      <c r="K72" s="24"/>
+    </row>
+    <row r="73" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="19">
         <f t="shared" si="5"/>
         <v>4</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="C73" s="21" t="s">
+      <c r="C73" s="20" t="s">
         <v>326</v>
       </c>
-      <c r="D73" s="21" t="s">
+      <c r="D73" s="20" t="s">
         <v>72</v>
       </c>
-      <c r="E73" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F73" s="21" t="s">
+      <c r="E73" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F73" s="20" t="s">
         <v>325</v>
       </c>
-      <c r="G73" s="21"/>
-      <c r="H73" s="22">
+      <c r="G73" s="20"/>
+      <c r="H73" s="21">
         <v>2.0499999999999998</v>
       </c>
-      <c r="I73" s="12">
+      <c r="I73" s="11">
         <v>2</v>
       </c>
-      <c r="J73" s="22">
+      <c r="J73" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>4.0999999999999996</v>
       </c>
-      <c r="K73" s="25"/>
-    </row>
-    <row r="74" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="16">
+      <c r="K73" s="24"/>
+    </row>
+    <row r="74" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="15">
         <f>1+A73</f>
         <v>5</v>
       </c>
-      <c r="B74" s="11" t="s">
+      <c r="B74" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="C74" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="D74" s="11" t="s">
+      <c r="D74" s="10" t="s">
         <v>333</v>
       </c>
-      <c r="E74" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F74" s="11" t="s">
+      <c r="E74" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F74" s="10" t="s">
         <v>331</v>
       </c>
-      <c r="G74" s="11"/>
-      <c r="H74" s="15">
+      <c r="G74" s="10"/>
+      <c r="H74" s="14">
         <v>2.75</v>
       </c>
-      <c r="I74" s="12">
+      <c r="I74" s="11">
         <v>1</v>
       </c>
-      <c r="J74" s="15">
+      <c r="J74" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>2.75</v>
       </c>
-      <c r="K74" s="13"/>
-    </row>
-    <row r="75" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="16">
+      <c r="K74" s="12"/>
+    </row>
+    <row r="75" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="15">
         <f>1+A74</f>
         <v>6</v>
       </c>
-      <c r="B75" s="11" t="s">
+      <c r="B75" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="C75" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="D75" s="11" t="s">
+      <c r="D75" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="E75" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F75" s="11" t="s">
+      <c r="E75" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="G75" s="11"/>
-      <c r="H75" s="15">
+      <c r="G75" s="10"/>
+      <c r="H75" s="14">
         <v>1.63</v>
       </c>
-      <c r="I75" s="12">
+      <c r="I75" s="11">
         <v>6</v>
       </c>
-      <c r="J75" s="15">
+      <c r="J75" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>9.7799999999999994</v>
       </c>
-      <c r="K75" s="13"/>
-    </row>
-    <row r="76" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="20">
+      <c r="K75" s="12"/>
+    </row>
+    <row r="76" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="19">
         <f>1+A75</f>
         <v>7</v>
       </c>
-      <c r="B76" s="21" t="s">
+      <c r="B76" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="C76" s="21" t="s">
+      <c r="C76" s="20" t="s">
         <v>337</v>
       </c>
-      <c r="D76" s="11" t="s">
+      <c r="D76" s="10" t="s">
         <v>338</v>
       </c>
-      <c r="E76" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F76" s="21" t="s">
+      <c r="E76" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F76" s="20" t="s">
         <v>339</v>
       </c>
-      <c r="G76" s="21"/>
-      <c r="H76" s="22">
+      <c r="G76" s="20"/>
+      <c r="H76" s="21">
         <v>1.43</v>
       </c>
-      <c r="I76" s="29">
+      <c r="I76" s="28">
         <v>2</v>
       </c>
-      <c r="J76" s="22">
+      <c r="J76" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>2.86</v>
       </c>
-      <c r="K76" s="25"/>
-    </row>
-    <row r="77" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="20">
+      <c r="K76" s="24"/>
+    </row>
+    <row r="77" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="19">
         <f>1+A76</f>
         <v>8</v>
       </c>
-      <c r="B77" s="11" t="s">
+      <c r="B77" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="C77" s="21" t="s">
+      <c r="C77" s="20" t="s">
         <v>161</v>
       </c>
-      <c r="D77" s="21" t="s">
+      <c r="D77" s="20" t="s">
         <v>73</v>
       </c>
-      <c r="E77" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="F77" s="21" t="s">
+      <c r="E77" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="F77" s="20" t="s">
         <v>74</v>
       </c>
-      <c r="G77" s="21"/>
-      <c r="H77" s="22">
+      <c r="G77" s="20"/>
+      <c r="H77" s="21">
         <v>1.17</v>
       </c>
-      <c r="I77" s="29">
+      <c r="I77" s="28">
         <v>1</v>
       </c>
-      <c r="J77" s="22">
+      <c r="J77" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.17</v>
       </c>
-      <c r="K77" s="25"/>
-    </row>
-    <row r="78" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="20">
+      <c r="K77" s="24"/>
+    </row>
+    <row r="78" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="19">
         <f t="shared" si="5"/>
         <v>9</v>
       </c>
-      <c r="B78" s="11" t="s">
+      <c r="B78" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="C78" s="21" t="s">
+      <c r="C78" s="20" t="s">
         <v>158</v>
       </c>
-      <c r="D78" s="21" t="s">
+      <c r="D78" s="20" t="s">
         <v>75</v>
       </c>
-      <c r="E78" s="21" t="s">
+      <c r="E78" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F78" s="11" t="s">
+      <c r="F78" s="10" t="s">
         <v>76</v>
       </c>
-      <c r="G78" s="21"/>
-      <c r="H78" s="22">
+      <c r="G78" s="20"/>
+      <c r="H78" s="21">
         <v>0.57999999999999996</v>
       </c>
-      <c r="I78" s="29">
+      <c r="I78" s="28">
         <v>2</v>
       </c>
-      <c r="J78" s="22">
+      <c r="J78" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.1599999999999999</v>
       </c>
-      <c r="K78" s="25"/>
-    </row>
-    <row r="79" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="40">
+      <c r="K78" s="24"/>
+    </row>
+    <row r="79" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="39">
         <f t="shared" si="5"/>
         <v>10</v>
       </c>
-      <c r="B79" s="33" t="s">
+      <c r="B79" s="32" t="s">
         <v>164</v>
       </c>
-      <c r="C79" s="41" t="s">
+      <c r="C79" s="40" t="s">
         <v>163</v>
       </c>
-      <c r="D79" s="41" t="s">
+      <c r="D79" s="40" t="s">
         <v>85</v>
       </c>
-      <c r="E79" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="F79" s="41" t="s">
+      <c r="E79" s="40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79" s="40" t="s">
         <v>77</v>
       </c>
-      <c r="G79" s="41"/>
-      <c r="H79" s="42">
+      <c r="G79" s="40"/>
+      <c r="H79" s="41">
         <v>3.71</v>
       </c>
-      <c r="I79" s="43">
+      <c r="I79" s="42">
         <v>0</v>
       </c>
-      <c r="J79" s="42">
+      <c r="J79" s="41">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K79" s="36" t="s">
+      <c r="K79" s="35" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="80" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="20">
+    <row r="80" spans="1:11" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="19">
         <f t="shared" ref="A80:A85" si="6">1+A79</f>
         <v>11</v>
       </c>
-      <c r="B80" s="11" t="s">
+      <c r="B80" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="C80" s="21" t="s">
+      <c r="C80" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="D80" s="21" t="s">
+      <c r="D80" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="E80" s="21" t="s">
+      <c r="E80" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F80" s="21" t="s">
+      <c r="F80" s="20" t="s">
         <v>86</v>
       </c>
-      <c r="G80" s="21"/>
-      <c r="H80" s="22">
+      <c r="G80" s="20"/>
+      <c r="H80" s="21">
         <v>2.35</v>
       </c>
-      <c r="I80" s="29">
+      <c r="I80" s="28">
         <v>1</v>
       </c>
-      <c r="J80" s="22">
+      <c r="J80" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>2.35</v>
       </c>
-      <c r="K80" s="13" t="s">
+      <c r="K80" s="12" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="81" spans="1:13" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="40">
+    <row r="81" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="39">
         <f t="shared" si="6"/>
         <v>12</v>
       </c>
-      <c r="B81" s="33" t="s">
+      <c r="B81" s="32" t="s">
         <v>157</v>
       </c>
-      <c r="C81" s="41" t="s">
+      <c r="C81" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="D81" s="41" t="s">
+      <c r="D81" s="40" t="s">
         <v>84</v>
       </c>
-      <c r="E81" s="41" t="s">
+      <c r="E81" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="F81" s="41" t="s">
+      <c r="F81" s="40" t="s">
         <v>87</v>
       </c>
-      <c r="G81" s="41"/>
-      <c r="H81" s="42">
+      <c r="G81" s="40"/>
+      <c r="H81" s="41">
         <v>3.15</v>
       </c>
-      <c r="I81" s="43">
+      <c r="I81" s="42">
         <v>0</v>
       </c>
-      <c r="J81" s="42">
+      <c r="J81" s="41">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0</v>
       </c>
-      <c r="K81" s="36" t="s">
+      <c r="K81" s="35" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="82" spans="1:13" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="20">
+    <row r="82" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="19">
         <f t="shared" si="6"/>
         <v>13</v>
       </c>
-      <c r="B82" s="11" t="s">
+      <c r="B82" s="10" t="s">
         <v>298</v>
       </c>
-      <c r="C82" s="21" t="s">
+      <c r="C82" s="20" t="s">
         <v>232</v>
       </c>
-      <c r="D82" s="21" t="s">
+      <c r="D82" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="E82" s="11" t="s">
+      <c r="E82" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="F82" s="21" t="s">
+      <c r="F82" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="G82" s="21" t="s">
+      <c r="G82" s="20" t="s">
         <v>297</v>
       </c>
-      <c r="H82" s="22">
+      <c r="H82" s="21">
         <v>0.12</v>
       </c>
-      <c r="I82" s="29">
+      <c r="I82" s="28">
         <v>1</v>
       </c>
-      <c r="J82" s="22">
+      <c r="J82" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.12</v>
       </c>
-      <c r="K82" s="25"/>
-    </row>
-    <row r="83" spans="1:13" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="16">
+      <c r="K82" s="24"/>
+    </row>
+    <row r="83" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="15">
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="B83" s="11" t="s">
+      <c r="B83" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="C83" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="D83" s="11" t="s">
+      <c r="D83" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="E83" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F83" s="11" t="s">
+      <c r="E83" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F83" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="G83" s="11"/>
-      <c r="H83" s="15">
+      <c r="G83" s="10"/>
+      <c r="H83" s="14">
         <v>1.18</v>
       </c>
-      <c r="I83" s="12">
+      <c r="I83" s="11">
         <v>4</v>
       </c>
-      <c r="J83" s="15">
+      <c r="J83" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>4.72</v>
       </c>
-      <c r="K83" s="13"/>
-      <c r="M83" s="54"/>
-    </row>
-    <row r="84" spans="1:13" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="16">
+      <c r="K83" s="12"/>
+      <c r="M83" s="53"/>
+    </row>
+    <row r="84" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="15">
         <f t="shared" si="6"/>
         <v>15</v>
       </c>
-      <c r="B84" s="11" t="s">
+      <c r="B84" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="C84" s="11" t="s">
+      <c r="C84" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="D84" s="11" t="s">
+      <c r="D84" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="E84" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F84" s="11" t="s">
+      <c r="E84" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F84" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="G84" s="11"/>
-      <c r="H84" s="15">
+      <c r="G84" s="10"/>
+      <c r="H84" s="14">
         <v>0.21299999999999999</v>
       </c>
-      <c r="I84" s="12">
+      <c r="I84" s="11">
         <v>10</v>
       </c>
-      <c r="J84" s="15">
+      <c r="J84" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>2.13</v>
       </c>
-      <c r="K84" s="13" t="s">
+      <c r="K84" s="12" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="85" spans="1:13" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="20">
-        <f t="shared" si="6"/>
+    <row r="85" spans="1:13" s="52" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="19">
+        <f>1+A84</f>
         <v>16</v>
       </c>
-      <c r="B85" s="21" t="s">
+      <c r="B85" s="20" t="s">
         <v>327</v>
       </c>
-      <c r="C85" s="21">
+      <c r="C85" s="20">
         <v>1935187</v>
       </c>
-      <c r="D85" s="11" t="s">
+      <c r="D85" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="E85" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F85" s="21" t="s">
+      <c r="E85" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F85" s="20" t="s">
         <v>329</v>
       </c>
-      <c r="G85" s="11" t="s">
+      <c r="G85" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="H85" s="22">
+      <c r="H85" s="21">
         <v>0.64</v>
       </c>
-      <c r="I85" s="29">
+      <c r="I85" s="28">
         <v>1</v>
       </c>
-      <c r="J85" s="22">
+      <c r="J85" s="21">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.64</v>
       </c>
-      <c r="K85" s="25"/>
+      <c r="K85" s="24"/>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" s="5"/>
-      <c r="B86" s="1"/>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
-      <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
+      <c r="A86" s="19">
+        <f>1+A85</f>
+        <v>17</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="C86" s="1">
+        <v>7200</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>341</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>342</v>
+      </c>
       <c r="G86" s="1"/>
-      <c r="H86" s="2"/>
-      <c r="I86" s="19"/>
+      <c r="H86" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="I86" s="18">
+        <v>4</v>
+      </c>
       <c r="J86" s="2">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
+        <v>2.72</v>
       </c>
       <c r="K86" s="4"/>
     </row>
     <row r="88" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C88" s="55"/>
+      <c r="C88" s="54"/>
     </row>
     <row r="89" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A89" s="55"/>
-      <c r="D89" s="45" t="s">
+      <c r="A89" s="54"/>
+      <c r="D89" s="44" t="s">
         <v>221</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Wheelchair code - added several additional menu options, decreased wireless timeout
</commit_message>
<xml_diff>
--- a/hardware/Wheelchair Receiver BOM.xlsx
+++ b/hardware/Wheelchair Receiver BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="362">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="371">
   <si>
     <t>ID #</t>
   </si>
@@ -1038,15 +1038,9 @@
     <t>EG2041-ND</t>
   </si>
   <si>
-    <t>PR144C1900</t>
-  </si>
-  <si>
     <t>E-stop button</t>
   </si>
   <si>
-    <t>EG4699-ND</t>
-  </si>
-  <si>
     <t>Sullins Connector Solutions</t>
   </si>
   <si>
@@ -1111,6 +1105,39 @@
   </si>
   <si>
     <t>7200K-ND</t>
+  </si>
+  <si>
+    <t>Apem</t>
+  </si>
+  <si>
+    <t>A01ESSP3</t>
+  </si>
+  <si>
+    <t>A01YL1</t>
+  </si>
+  <si>
+    <t>A0150B</t>
+  </si>
+  <si>
+    <t>Alternative: A0154B</t>
+  </si>
+  <si>
+    <t>Optional</t>
+  </si>
+  <si>
+    <t>E-stop switch block</t>
+  </si>
+  <si>
+    <t>E-stop sticker (optional)</t>
+  </si>
+  <si>
+    <t>642-A01ES-SP3</t>
+  </si>
+  <si>
+    <t>642-A0150B</t>
+  </si>
+  <si>
+    <t>642-A01YL1</t>
   </si>
 </sst>
 </file>
@@ -2166,8 +2193,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:K92" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
-  <autoFilter ref="A2:K92"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table2" displayName="Table2" ref="A2:K94" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
+  <autoFilter ref="A2:K94"/>
   <tableColumns count="11">
     <tableColumn id="1" name="ID #" dataDxfId="10">
       <calculatedColumnFormula>1+A2</calculatedColumnFormula>
@@ -2479,11 +2506,11 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M94"/>
+  <dimension ref="A1:M96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B86" sqref="B86"/>
+      <pane ySplit="2" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F78" sqref="F78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2516,7 +2543,7 @@
       </c>
       <c r="J1" s="46">
         <f>SUM(Table2[Sub Total])</f>
-        <v>170.58999999999989</v>
+        <v>224.44999999999985</v>
       </c>
       <c r="K1" s="47"/>
     </row>
@@ -4793,7 +4820,7 @@
     </row>
     <row r="71" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="18">
-        <f t="shared" ref="A71:A79" si="5">1+A70</f>
+        <f t="shared" ref="A71:A81" si="5">1+A70</f>
         <v>2</v>
       </c>
       <c r="B71" s="10" t="s">
@@ -4894,7 +4921,7 @@
     </row>
     <row r="74" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
-        <f>1+A73</f>
+        <f t="shared" ref="A74:A79" si="6">1+A73</f>
         <v>5</v>
       </c>
       <c r="B74" s="10" t="s">
@@ -4927,7 +4954,7 @@
     </row>
     <row r="75" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
-        <f>1+A74</f>
+        <f t="shared" si="6"/>
         <v>6</v>
       </c>
       <c r="B75" s="10" t="s">
@@ -4960,196 +4987,196 @@
     </row>
     <row r="76" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="18">
-        <f>1+A75</f>
+        <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>146</v>
+        <v>360</v>
       </c>
       <c r="C76" s="19" t="s">
+        <v>361</v>
+      </c>
+      <c r="D76" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="D76" s="10" t="s">
-        <v>338</v>
-      </c>
       <c r="E76" s="10" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>339</v>
+        <v>368</v>
       </c>
       <c r="G76" s="19"/>
       <c r="H76" s="20">
-        <v>1.43</v>
+        <v>19.38</v>
       </c>
       <c r="I76" s="27">
         <v>2</v>
       </c>
       <c r="J76" s="20">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>2.86</v>
+        <v>38.76</v>
       </c>
       <c r="K76" s="23"/>
     </row>
     <row r="77" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="18">
-        <f>1+A76</f>
+        <f t="shared" si="6"/>
         <v>8</v>
       </c>
-      <c r="B77" s="10" t="s">
-        <v>162</v>
+      <c r="B77" s="19" t="s">
+        <v>360</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>161</v>
+        <v>363</v>
       </c>
       <c r="D77" s="19" t="s">
-        <v>73</v>
+        <v>366</v>
       </c>
       <c r="E77" s="19" t="s">
-        <v>18</v>
+        <v>68</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>74</v>
+        <v>369</v>
       </c>
       <c r="G77" s="19"/>
       <c r="H77" s="20">
-        <v>1.17</v>
+        <v>6.77</v>
       </c>
       <c r="I77" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J77" s="20">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.17</v>
-      </c>
-      <c r="K77" s="23"/>
+        <v>13.54</v>
+      </c>
+      <c r="K77" s="23" t="s">
+        <v>364</v>
+      </c>
     </row>
     <row r="78" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>9</v>
       </c>
-      <c r="B78" s="10" t="s">
-        <v>156</v>
+      <c r="B78" s="19" t="s">
+        <v>360</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>158</v>
+        <v>362</v>
       </c>
       <c r="D78" s="19" t="s">
-        <v>75</v>
+        <v>367</v>
       </c>
       <c r="E78" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F78" s="10" t="s">
-        <v>76</v>
+      <c r="F78" s="19" t="s">
+        <v>370</v>
       </c>
       <c r="G78" s="19"/>
       <c r="H78" s="20">
-        <v>0.57999999999999996</v>
+        <v>2.21</v>
       </c>
       <c r="I78" s="27">
         <v>2</v>
       </c>
       <c r="J78" s="20">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.1599999999999999</v>
-      </c>
-      <c r="K78" s="23"/>
+        <v>4.42</v>
+      </c>
+      <c r="K78" s="23" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="79" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="38">
-        <f t="shared" si="5"/>
+      <c r="A79" s="18">
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="B79" s="31" t="s">
-        <v>164</v>
-      </c>
-      <c r="C79" s="39" t="s">
-        <v>163</v>
-      </c>
-      <c r="D79" s="39" t="s">
-        <v>85</v>
-      </c>
-      <c r="E79" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F79" s="39" t="s">
-        <v>77</v>
-      </c>
-      <c r="G79" s="39"/>
-      <c r="H79" s="40">
-        <v>3.71</v>
-      </c>
-      <c r="I79" s="41">
-        <v>0</v>
-      </c>
-      <c r="J79" s="40">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
-      </c>
-      <c r="K79" s="34" t="s">
-        <v>321</v>
-      </c>
+      <c r="B79" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="C79" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="D79" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="E79" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="G79" s="19"/>
+      <c r="H79" s="20">
+        <v>1.17</v>
+      </c>
+      <c r="I79" s="27">
+        <v>1</v>
+      </c>
+      <c r="J79" s="20">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>1.17</v>
+      </c>
+      <c r="K79" s="23"/>
     </row>
     <row r="80" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="18">
-        <f t="shared" ref="A80:A84" si="6">1+A79</f>
+        <f t="shared" si="5"/>
         <v>11</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C80" s="19" t="s">
-        <v>86</v>
+        <v>158</v>
       </c>
       <c r="D80" s="19" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E80" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F80" s="19" t="s">
-        <v>86</v>
+      <c r="F80" s="10" t="s">
+        <v>76</v>
       </c>
       <c r="G80" s="19"/>
       <c r="H80" s="20">
-        <v>2.35</v>
+        <v>0.57999999999999996</v>
       </c>
       <c r="I80" s="27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J80" s="20">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>2.35</v>
-      </c>
-      <c r="K80" s="12" t="s">
-        <v>322</v>
-      </c>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="K80" s="23"/>
     </row>
     <row r="81" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>12</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>157</v>
+        <v>164</v>
       </c>
       <c r="C81" s="39" t="s">
-        <v>87</v>
+        <v>163</v>
       </c>
       <c r="D81" s="39" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E81" s="39" t="s">
-        <v>68</v>
+        <v>18</v>
       </c>
       <c r="F81" s="39" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="G81" s="39"/>
       <c r="H81" s="40">
-        <v>3.15</v>
+        <v>3.71</v>
       </c>
       <c r="I81" s="41">
         <v>0</v>
@@ -5164,380 +5191,450 @@
     </row>
     <row r="82" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="18">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="A82:A86" si="7">1+A81</f>
         <v>13</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>298</v>
+        <v>157</v>
       </c>
       <c r="C82" s="19" t="s">
-        <v>232</v>
+        <v>86</v>
       </c>
       <c r="D82" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="E82" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="E82" s="19" t="s">
         <v>68</v>
       </c>
       <c r="F82" s="19" t="s">
-        <v>233</v>
-      </c>
-      <c r="G82" s="19" t="s">
-        <v>297</v>
-      </c>
+        <v>86</v>
+      </c>
+      <c r="G82" s="19"/>
       <c r="H82" s="20">
-        <v>0.12</v>
+        <v>2.35</v>
       </c>
       <c r="I82" s="27">
         <v>1</v>
       </c>
       <c r="J82" s="20">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>2.35</v>
+      </c>
+      <c r="K82" s="12" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="38">
+        <f t="shared" si="7"/>
+        <v>14</v>
+      </c>
+      <c r="B83" s="31" t="s">
+        <v>157</v>
+      </c>
+      <c r="C83" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="D83" s="39" t="s">
+        <v>84</v>
+      </c>
+      <c r="E83" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="F83" s="39" t="s">
+        <v>87</v>
+      </c>
+      <c r="G83" s="39"/>
+      <c r="H83" s="40">
+        <v>3.15</v>
+      </c>
+      <c r="I83" s="41">
+        <v>0</v>
+      </c>
+      <c r="J83" s="40">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0</v>
+      </c>
+      <c r="K83" s="34" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="18">
+        <f t="shared" si="7"/>
+        <v>15</v>
+      </c>
+      <c r="B84" s="10" t="s">
+        <v>298</v>
+      </c>
+      <c r="C84" s="19" t="s">
+        <v>232</v>
+      </c>
+      <c r="D84" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E84" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="F84" s="19" t="s">
+        <v>233</v>
+      </c>
+      <c r="G84" s="19" t="s">
+        <v>297</v>
+      </c>
+      <c r="H84" s="20">
         <v>0.12</v>
       </c>
-      <c r="K82" s="23"/>
-    </row>
-    <row r="83" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="15">
-        <f t="shared" si="6"/>
-        <v>14</v>
-      </c>
-      <c r="B83" s="10" t="s">
+      <c r="I84" s="27">
+        <v>1</v>
+      </c>
+      <c r="J84" s="20">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.12</v>
+      </c>
+      <c r="K84" s="23"/>
+    </row>
+    <row r="85" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="15">
+        <f t="shared" si="7"/>
+        <v>16</v>
+      </c>
+      <c r="B85" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="C83" s="10" t="s">
+      <c r="C85" s="10" t="s">
         <v>217</v>
       </c>
-      <c r="D83" s="10" t="s">
+      <c r="D85" s="10" t="s">
         <v>192</v>
       </c>
-      <c r="E83" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F83" s="10" t="s">
+      <c r="E85" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F85" s="10" t="s">
         <v>216</v>
       </c>
-      <c r="G83" s="10"/>
-      <c r="H83" s="14">
+      <c r="G85" s="10"/>
+      <c r="H85" s="14">
         <v>1.18</v>
       </c>
-      <c r="I83" s="11">
+      <c r="I85" s="11">
         <v>4</v>
       </c>
-      <c r="J83" s="14">
+      <c r="J85" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>4.72</v>
       </c>
-      <c r="K83" s="12"/>
-      <c r="M83" s="52"/>
-    </row>
-    <row r="84" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="15">
-        <f t="shared" si="6"/>
-        <v>15</v>
-      </c>
-      <c r="B84" s="10" t="s">
+      <c r="K85" s="12"/>
+      <c r="M85" s="52"/>
+    </row>
+    <row r="86" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="15">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="B86" s="10" t="s">
         <v>219</v>
       </c>
-      <c r="C84" s="10" t="s">
+      <c r="C86" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="D84" s="10" t="s">
+      <c r="D86" s="10" t="s">
         <v>208</v>
       </c>
-      <c r="E84" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F84" s="10" t="s">
+      <c r="E86" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F86" s="10" t="s">
         <v>218</v>
       </c>
-      <c r="G84" s="10"/>
-      <c r="H84" s="14">
+      <c r="G86" s="10"/>
+      <c r="H86" s="14">
         <v>0.21299999999999999</v>
       </c>
-      <c r="I84" s="11">
+      <c r="I86" s="11">
         <v>10</v>
       </c>
-      <c r="J84" s="14">
+      <c r="J86" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>2.13</v>
       </c>
-      <c r="K84" s="12" t="s">
+      <c r="K86" s="12" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="85" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="18">
-        <f t="shared" ref="A85:A92" si="7">1+A84</f>
-        <v>16</v>
-      </c>
-      <c r="B85" s="19" t="s">
+    <row r="87" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="18">
+        <f t="shared" ref="A87:A94" si="8">1+A86</f>
+        <v>18</v>
+      </c>
+      <c r="B87" s="19" t="s">
         <v>327</v>
       </c>
-      <c r="C85" s="19">
+      <c r="C87" s="19">
         <v>1935187</v>
       </c>
-      <c r="D85" s="10" t="s">
+      <c r="D87" s="10" t="s">
         <v>328</v>
       </c>
-      <c r="E85" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F85" s="19" t="s">
+      <c r="E87" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F87" s="19" t="s">
         <v>329</v>
       </c>
-      <c r="G85" s="10" t="s">
+      <c r="G87" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="H85" s="20">
+      <c r="H87" s="20">
         <v>0.64</v>
       </c>
-      <c r="I85" s="27">
+      <c r="I87" s="27">
         <v>1</v>
       </c>
-      <c r="J85" s="20">
+      <c r="J87" s="20">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.64</v>
       </c>
-      <c r="K85" s="23"/>
-    </row>
-    <row r="86" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A86" s="18">
-        <f>1+A85</f>
-        <v>17</v>
-      </c>
-      <c r="B86" s="19" t="s">
+      <c r="K87" s="23"/>
+    </row>
+    <row r="88" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="18">
+        <f>1+A87</f>
+        <v>19</v>
+      </c>
+      <c r="B88" s="19" t="s">
+        <v>357</v>
+      </c>
+      <c r="C88" s="19">
+        <v>7200</v>
+      </c>
+      <c r="D88" s="19" t="s">
+        <v>358</v>
+      </c>
+      <c r="E88" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F88" s="19" t="s">
         <v>359</v>
       </c>
-      <c r="C86" s="19">
-        <v>7200</v>
-      </c>
-      <c r="D86" s="19" t="s">
-        <v>360</v>
-      </c>
-      <c r="E86" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="F86" s="19" t="s">
-        <v>361</v>
-      </c>
-      <c r="G86" s="19"/>
-      <c r="H86" s="20">
+      <c r="G88" s="19"/>
+      <c r="H88" s="20">
         <v>0.68</v>
       </c>
-      <c r="I86" s="27">
+      <c r="I88" s="27">
         <v>4</v>
       </c>
-      <c r="J86" s="20">
+      <c r="J88" s="20">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>2.72</v>
       </c>
-      <c r="K86" s="23"/>
-    </row>
-    <row r="87" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A87" s="15">
-        <f>1+A86</f>
-        <v>18</v>
-      </c>
-      <c r="B87" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>341</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>342</v>
-      </c>
-      <c r="E87" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>343</v>
-      </c>
-      <c r="G87" s="1"/>
-      <c r="H87" s="2">
-        <v>1.22</v>
-      </c>
-      <c r="I87" s="3">
-        <v>1</v>
-      </c>
-      <c r="J87" s="14">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.22</v>
-      </c>
-      <c r="K87" s="12"/>
-    </row>
-    <row r="88" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="15">
-        <f t="shared" si="7"/>
-        <v>19</v>
-      </c>
-      <c r="B88" s="1" t="s">
-        <v>340</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>354</v>
-      </c>
-      <c r="D88" s="1" t="s">
-        <v>344</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F88" s="1" t="s">
-        <v>349</v>
-      </c>
-      <c r="G88" s="1"/>
-      <c r="H88" s="2">
-        <v>0.67</v>
-      </c>
-      <c r="I88" s="3">
-        <v>1</v>
-      </c>
-      <c r="J88" s="14">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.67</v>
-      </c>
-      <c r="K88" s="12"/>
+      <c r="K88" s="23"/>
     </row>
     <row r="89" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
-        <f t="shared" si="7"/>
+        <f>1+A88</f>
         <v>20</v>
       </c>
       <c r="B89" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C89" s="1" t="s">
+        <v>339</v>
+      </c>
+      <c r="D89" s="1" t="s">
         <v>340</v>
       </c>
-      <c r="C89" s="1" t="s">
-        <v>355</v>
-      </c>
-      <c r="D89" s="1" t="s">
-        <v>345</v>
-      </c>
       <c r="E89" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="G89" s="1"/>
       <c r="H89" s="2">
-        <v>0.63</v>
+        <v>1.22</v>
       </c>
       <c r="I89" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J89" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.26</v>
+        <v>1.22</v>
       </c>
       <c r="K89" s="12"/>
     </row>
     <row r="90" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="G90" s="1"/>
       <c r="H90" s="2">
-        <v>0.49</v>
+        <v>0.67</v>
       </c>
       <c r="I90" s="3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J90" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0.98</v>
+        <v>0.67</v>
       </c>
       <c r="K90" s="12"/>
     </row>
     <row r="91" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="2">
-        <v>1.73</v>
+        <v>0.63</v>
       </c>
       <c r="I91" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J91" s="14">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>1.73</v>
+        <v>1.26</v>
       </c>
       <c r="K91" s="12"/>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A92" s="18">
-        <f t="shared" si="7"/>
+    <row r="92" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="15">
+        <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="G92" s="1"/>
       <c r="H92" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="I92" s="3">
+        <v>2</v>
+      </c>
+      <c r="J92" s="14">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>0.98</v>
+      </c>
+      <c r="K92" s="12"/>
+    </row>
+    <row r="93" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A93" s="15">
+        <f t="shared" si="8"/>
+        <v>24</v>
+      </c>
+      <c r="B93" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>355</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="E93" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="G93" s="1"/>
+      <c r="H93" s="2">
+        <v>1.73</v>
+      </c>
+      <c r="I93" s="3">
+        <v>1</v>
+      </c>
+      <c r="J93" s="14">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>1.73</v>
+      </c>
+      <c r="K93" s="12"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A94" s="18">
+        <f t="shared" si="8"/>
+        <v>25</v>
+      </c>
+      <c r="B94" s="1" t="s">
+        <v>338</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>356</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="E94" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F94" s="1" t="s">
+        <v>351</v>
+      </c>
+      <c r="G94" s="1"/>
+      <c r="H94" s="2">
         <v>0.83</v>
       </c>
-      <c r="I92" s="3">
+      <c r="I94" s="3">
         <v>1</v>
       </c>
-      <c r="J92" s="2">
+      <c r="J94" s="2">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.83</v>
       </c>
-      <c r="K92" s="4"/>
-    </row>
-    <row r="93" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C93" s="53"/>
-    </row>
-    <row r="94" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A94" s="53"/>
-      <c r="D94" s="43" t="s">
+      <c r="K94" s="4"/>
+    </row>
+    <row r="95" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="C95" s="53"/>
+    </row>
+    <row r="96" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A96" s="53"/>
+      <c r="D96" s="43" t="s">
         <v>221</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added fuse to BOM
</commit_message>
<xml_diff>
--- a/hardware/Wheelchair Receiver BOM.xlsx
+++ b/hardware/Wheelchair Receiver BOM.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="509" uniqueCount="371">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="506" uniqueCount="370">
   <si>
     <t>ID #</t>
   </si>
@@ -690,30 +690,6 @@
     <t>881545-2</t>
   </si>
   <si>
-    <t>fuse!!!</t>
-  </si>
-  <si>
-    <t>283-2633-ND</t>
-  </si>
-  <si>
-    <t>Copper/Bussmann</t>
-  </si>
-  <si>
-    <t>BK/AGC-30-R</t>
-  </si>
-  <si>
-    <t>30A Fuse</t>
-  </si>
-  <si>
-    <t>283-2850-ND</t>
-  </si>
-  <si>
-    <t>Fuse Holder</t>
-  </si>
-  <si>
-    <t>BK/HKP-R</t>
-  </si>
-  <si>
     <t>ATXMEGA64A1-AU</t>
   </si>
   <si>
@@ -1138,6 +1114,27 @@
   </si>
   <si>
     <t>642-A01YL1</t>
+  </si>
+  <si>
+    <t>BD280-1927-25/16</t>
+  </si>
+  <si>
+    <t>25A Fuse</t>
+  </si>
+  <si>
+    <t>BD280-1927-25-ND</t>
+  </si>
+  <si>
+    <t>Fuse Holder (crimp)</t>
+  </si>
+  <si>
+    <t>Littelfuse, Inc</t>
+  </si>
+  <si>
+    <t>178.6152.0001</t>
+  </si>
+  <si>
+    <t>F5194-ND</t>
   </si>
 </sst>
 </file>
@@ -1715,7 +1712,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1838,9 +1835,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="28" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2509,76 +2503,76 @@
   <dimension ref="A1:M96"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A69" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F78" sqref="F78"/>
+      <pane ySplit="2" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D65" sqref="D65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="43" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" style="43" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="43" customWidth="1"/>
-    <col min="4" max="4" width="36.140625" style="43" customWidth="1"/>
-    <col min="5" max="5" width="18.42578125" style="43" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24" style="43" customWidth="1"/>
-    <col min="7" max="7" width="14.85546875" style="43" customWidth="1"/>
-    <col min="8" max="8" width="10" style="43" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.7109375" style="43" customWidth="1"/>
-    <col min="10" max="10" width="13.7109375" style="43" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.5703125" style="54" customWidth="1"/>
-    <col min="12" max="16384" width="9.140625" style="43"/>
+    <col min="1" max="1" width="12.140625" style="42" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="42" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" style="42" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" style="42" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24" style="42" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" style="42" customWidth="1"/>
+    <col min="8" max="8" width="10" style="42" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.7109375" style="42" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" style="42" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="36.5703125" style="53" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="42"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="44"/>
-      <c r="B1" s="44"/>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="45" t="s">
+      <c r="A1" s="43"/>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="46">
+      <c r="J1" s="45">
         <f>SUM(Table2[Sub Total])</f>
-        <v>224.44999999999985</v>
-      </c>
-      <c r="K1" s="47"/>
+        <v>239.42999999999986</v>
+      </c>
+      <c r="K1" s="46"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="48" t="s">
+      <c r="A2" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="47" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="48" t="s">
+      <c r="C2" s="47" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="48" t="s">
+      <c r="D2" s="47" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="48" t="s">
+      <c r="E2" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="48" t="s">
+      <c r="F2" s="47" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="48" t="s">
+      <c r="G2" s="47" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="49" t="s">
+      <c r="H2" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="I2" s="48" t="s">
+      <c r="I2" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="49" t="s">
+      <c r="J2" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="50" t="s">
+      <c r="K2" s="49" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2600,7 +2594,7 @@
       </c>
       <c r="K3" s="4"/>
     </row>
-    <row r="4" spans="1:11" s="51" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="50" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <f>1</f>
         <v>1</v>
@@ -2621,7 +2615,7 @@
         <v>31</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>260</v>
+        <v>252</v>
       </c>
       <c r="H4" s="14">
         <v>0.03</v>
@@ -2635,7 +2629,7 @@
       </c>
       <c r="K4" s="12"/>
     </row>
-    <row r="5" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <f>1+A4</f>
         <v>2</v>
@@ -2670,7 +2664,7 @@
       </c>
       <c r="K5" s="12"/>
     </row>
-    <row r="6" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <f>1+A5</f>
         <v>3</v>
@@ -2691,7 +2685,7 @@
         <v>57</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>261</v>
+        <v>253</v>
       </c>
       <c r="H6" s="14">
         <v>0.1</v>
@@ -2705,7 +2699,7 @@
       </c>
       <c r="K6" s="12"/>
     </row>
-    <row r="7" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
         <f t="shared" ref="A7:A27" si="0">1+A6</f>
         <v>4</v>
@@ -2726,7 +2720,7 @@
         <v>102</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>262</v>
+        <v>254</v>
       </c>
       <c r="H7" s="14">
         <v>0.1</v>
@@ -2740,7 +2734,7 @@
       </c>
       <c r="K7" s="12"/>
     </row>
-    <row r="8" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2775,8 +2769,8 @@
       </c>
       <c r="K8" s="9"/>
     </row>
-    <row r="9" spans="1:11" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A9" s="55">
+    <row r="9" spans="1:11" s="50" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A9" s="54">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
@@ -2795,24 +2789,24 @@
       <c r="F9" s="28" t="s">
         <v>104</v>
       </c>
-      <c r="G9" s="56" t="s">
-        <v>264</v>
-      </c>
-      <c r="H9" s="57">
+      <c r="G9" s="55" t="s">
+        <v>256</v>
+      </c>
+      <c r="H9" s="56">
         <v>0.04</v>
       </c>
       <c r="I9" s="28">
         <v>7</v>
       </c>
-      <c r="J9" s="57">
+      <c r="J9" s="56">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.28000000000000003</v>
       </c>
-      <c r="K9" s="58" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K9" s="57" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -2847,7 +2841,7 @@
       </c>
       <c r="K10" s="12"/>
     </row>
-    <row r="11" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -2868,7 +2862,7 @@
         <v>106</v>
       </c>
       <c r="G11" s="11" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="H11" s="14">
         <v>0.04</v>
@@ -2882,8 +2876,8 @@
       </c>
       <c r="K11" s="12"/>
     </row>
-    <row r="12" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="55">
+    <row r="12" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="54">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
@@ -2894,7 +2888,7 @@
         <v>116</v>
       </c>
       <c r="D12" s="28" t="s">
-        <v>231</v>
+        <v>223</v>
       </c>
       <c r="E12" s="28" t="s">
         <v>18</v>
@@ -2902,24 +2896,24 @@
       <c r="F12" s="28" t="s">
         <v>107</v>
       </c>
-      <c r="G12" s="56" t="s">
-        <v>266</v>
-      </c>
-      <c r="H12" s="57">
+      <c r="G12" s="55" t="s">
+        <v>258</v>
+      </c>
+      <c r="H12" s="56">
         <v>0.04</v>
       </c>
       <c r="I12" s="28">
         <v>3</v>
       </c>
-      <c r="J12" s="57">
+      <c r="J12" s="56">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.12</v>
       </c>
-      <c r="K12" s="58" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K12" s="57" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -2954,7 +2948,7 @@
       </c>
       <c r="K13" s="12"/>
     </row>
-    <row r="14" spans="1:11" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="50" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
         <f>1+A13</f>
         <v>11</v>
@@ -2963,16 +2957,16 @@
         <v>109</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>272</v>
+        <v>264</v>
       </c>
       <c r="D14" s="10" t="s">
+        <v>255</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>263</v>
-      </c>
-      <c r="E14" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>271</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>179</v>
@@ -2989,7 +2983,7 @@
       </c>
       <c r="K14" s="12"/>
     </row>
-    <row r="15" spans="1:11" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="50" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
         <f>1+A14</f>
         <v>12</v>
@@ -3024,8 +3018,8 @@
       </c>
       <c r="K15" s="12"/>
     </row>
-    <row r="16" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="55">
+    <row r="16" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="54">
         <f>1+A15</f>
         <v>13</v>
       </c>
@@ -3033,35 +3027,35 @@
         <v>109</v>
       </c>
       <c r="C16" s="28" t="s">
-        <v>269</v>
+        <v>261</v>
       </c>
       <c r="D16" s="28" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="E16" s="28" t="s">
         <v>18</v>
       </c>
       <c r="F16" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="G16" s="57" t="s">
-        <v>268</v>
-      </c>
-      <c r="H16" s="57">
+        <v>262</v>
+      </c>
+      <c r="G16" s="56" t="s">
+        <v>260</v>
+      </c>
+      <c r="H16" s="56">
         <v>0.03</v>
       </c>
-      <c r="I16" s="56">
+      <c r="I16" s="55">
         <v>2</v>
       </c>
-      <c r="J16" s="57">
+      <c r="J16" s="56">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>0.06</v>
       </c>
-      <c r="K16" s="58" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K16" s="57" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="18">
         <f>1+A16</f>
         <v>14</v>
@@ -3070,19 +3064,19 @@
         <v>204</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>257</v>
+        <v>249</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>256</v>
+        <v>248</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="G17" s="14" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="H17" s="20">
         <v>1.05</v>
@@ -3130,7 +3124,7 @@
       </c>
       <c r="K19" s="9"/>
     </row>
-    <row r="20" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15">
         <v>1</v>
       </c>
@@ -3150,7 +3144,7 @@
         <v>25</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="H20" s="8">
         <v>1.34</v>
@@ -3166,7 +3160,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:11" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="50" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A21" s="15">
         <f t="shared" si="0"/>
         <v>2</v>
@@ -3175,7 +3169,7 @@
         <v>11</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="D21" s="19" t="s">
         <v>91</v>
@@ -3184,7 +3178,7 @@
         <v>18</v>
       </c>
       <c r="F21" s="17" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="G21" s="6" t="s">
         <v>183</v>
@@ -3203,7 +3197,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15">
         <f t="shared" si="0"/>
         <v>3</v>
@@ -3238,7 +3232,7 @@
       </c>
       <c r="K22" s="9"/>
     </row>
-    <row r="23" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -3273,7 +3267,7 @@
       </c>
       <c r="K23" s="12"/>
     </row>
-    <row r="24" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -3308,7 +3302,7 @@
       </c>
       <c r="K24" s="12"/>
     </row>
-    <row r="25" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -3343,7 +3337,7 @@
       </c>
       <c r="K25" s="12"/>
     </row>
-    <row r="26" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="15">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -3352,7 +3346,7 @@
         <v>149</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="D26" s="10" t="s">
         <v>47</v>
@@ -3361,7 +3355,7 @@
         <v>18</v>
       </c>
       <c r="F26" s="10" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>45</v>
@@ -3378,7 +3372,7 @@
       </c>
       <c r="K26" s="12"/>
     </row>
-    <row r="27" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="15">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -3387,7 +3381,7 @@
         <v>149</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="D27" s="10" t="s">
         <v>46</v>
@@ -3396,7 +3390,7 @@
         <v>18</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>313</v>
+        <v>305</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>48</v>
@@ -3413,7 +3407,7 @@
       </c>
       <c r="K27" s="12"/>
     </row>
-    <row r="28" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15">
         <f t="shared" ref="A28:A33" si="1">1+A27</f>
         <v>9</v>
@@ -3422,7 +3416,7 @@
         <v>126</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>314</v>
+        <v>306</v>
       </c>
       <c r="D28" s="10" t="s">
         <v>49</v>
@@ -3431,7 +3425,7 @@
         <v>18</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>315</v>
+        <v>307</v>
       </c>
       <c r="G28" s="10" t="s">
         <v>50</v>
@@ -3448,13 +3442,13 @@
       </c>
       <c r="K28" s="12"/>
     </row>
-    <row r="29" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15">
         <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>125</v>
@@ -3482,11 +3476,11 @@
         <v>0.04</v>
       </c>
       <c r="K29" s="12" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" s="51" customFormat="1" ht="72" x14ac:dyDescent="0.25">
-      <c r="A30" s="59">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" s="50" customFormat="1" ht="72" x14ac:dyDescent="0.25">
+      <c r="A30" s="58">
         <f t="shared" si="1"/>
         <v>11</v>
       </c>
@@ -3506,24 +3500,24 @@
         <v>93</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>254</v>
-      </c>
-      <c r="H30" s="60">
+        <v>246</v>
+      </c>
+      <c r="H30" s="59">
         <v>0.05</v>
       </c>
-      <c r="I30" s="61">
+      <c r="I30" s="60">
         <v>22</v>
       </c>
-      <c r="J30" s="60">
+      <c r="J30" s="59">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="K30" s="62" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.25">
-      <c r="A31" s="59">
+      <c r="K30" s="61" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" s="50" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+      <c r="A31" s="58">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
@@ -3543,23 +3537,23 @@
         <v>101</v>
       </c>
       <c r="G31" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="H31" s="60">
+        <v>247</v>
+      </c>
+      <c r="H31" s="59">
         <v>0.3</v>
       </c>
-      <c r="I31" s="61">
+      <c r="I31" s="60">
         <v>6</v>
       </c>
-      <c r="J31" s="60">
+      <c r="J31" s="59">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.7999999999999998</v>
       </c>
-      <c r="K31" s="62" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="K31" s="61" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15">
         <f t="shared" si="1"/>
         <v>13</v>
@@ -3594,8 +3588,8 @@
       </c>
       <c r="K32" s="12"/>
     </row>
-    <row r="33" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="55">
+    <row r="33" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="54">
         <f t="shared" si="1"/>
         <v>14</v>
       </c>
@@ -3617,18 +3611,18 @@
       <c r="G33" s="28" t="s">
         <v>187</v>
       </c>
-      <c r="H33" s="57">
+      <c r="H33" s="56">
         <v>0.39</v>
       </c>
-      <c r="I33" s="56">
+      <c r="I33" s="55">
         <v>4</v>
       </c>
-      <c r="J33" s="57">
+      <c r="J33" s="56">
         <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
         <v>1.56</v>
       </c>
-      <c r="K33" s="58" t="s">
-        <v>303</v>
+      <c r="K33" s="57" t="s">
+        <v>295</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -3665,7 +3659,7 @@
       </c>
       <c r="K35" s="12"/>
     </row>
-    <row r="36" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15">
         <v>1</v>
       </c>
@@ -3685,7 +3679,7 @@
         <v>22</v>
       </c>
       <c r="G36" s="10" t="s">
-        <v>274</v>
+        <v>266</v>
       </c>
       <c r="H36" s="14">
         <v>3.47</v>
@@ -3699,7 +3693,7 @@
       </c>
       <c r="K36" s="12"/>
     </row>
-    <row r="37" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15">
         <f>1+A36</f>
         <v>2</v>
@@ -3708,19 +3702,19 @@
         <v>133</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>68</v>
       </c>
       <c r="F37" s="10" t="s">
-        <v>277</v>
+        <v>269</v>
       </c>
       <c r="G37" s="10" t="s">
-        <v>278</v>
+        <v>270</v>
       </c>
       <c r="H37" s="14">
         <v>3.6</v>
@@ -3734,7 +3728,7 @@
       </c>
       <c r="K37" s="12"/>
     </row>
-    <row r="38" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="15">
         <f t="shared" ref="A38:A39" si="2">1+A37</f>
         <v>3</v>
@@ -3743,19 +3737,19 @@
         <v>132</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>280</v>
+        <v>272</v>
       </c>
       <c r="D38" s="24" t="s">
-        <v>281</v>
+        <v>273</v>
       </c>
       <c r="E38" s="19" t="s">
         <v>18</v>
       </c>
       <c r="F38" s="19" t="s">
-        <v>282</v>
+        <v>274</v>
       </c>
       <c r="G38" s="10" t="s">
-        <v>279</v>
+        <v>271</v>
       </c>
       <c r="H38" s="20">
         <v>4.3499999999999996</v>
@@ -3769,7 +3763,7 @@
       </c>
       <c r="K38" s="23"/>
     </row>
-    <row r="39" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15">
         <f t="shared" si="2"/>
         <v>4</v>
@@ -3778,19 +3772,19 @@
         <v>134</v>
       </c>
       <c r="C39" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="D39" s="10" t="s">
         <v>229</v>
-      </c>
-      <c r="D39" s="10" t="s">
-        <v>237</v>
       </c>
       <c r="E39" s="10" t="s">
         <v>68</v>
       </c>
       <c r="F39" s="19" t="s">
-        <v>230</v>
+        <v>222</v>
       </c>
       <c r="G39" s="10" t="s">
-        <v>283</v>
+        <v>275</v>
       </c>
       <c r="H39" s="20">
         <v>7.5</v>
@@ -3804,7 +3798,7 @@
       </c>
       <c r="K39" s="23"/>
     </row>
-    <row r="40" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15">
         <f>1+A39</f>
         <v>5</v>
@@ -3825,7 +3819,7 @@
         <v>188</v>
       </c>
       <c r="G40" s="10" t="s">
-        <v>284</v>
+        <v>276</v>
       </c>
       <c r="H40" s="14">
         <v>5.65</v>
@@ -3839,7 +3833,7 @@
       </c>
       <c r="K40" s="12"/>
     </row>
-    <row r="41" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="18">
         <f>1+A40</f>
         <v>6</v>
@@ -3848,19 +3842,19 @@
         <v>144</v>
       </c>
       <c r="C41" s="19" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="D41" s="19" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="E41" s="19" t="s">
         <v>18</v>
       </c>
       <c r="F41" s="19" t="s">
-        <v>244</v>
+        <v>236</v>
       </c>
       <c r="G41" s="19" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="H41" s="20">
         <v>0.62</v>
@@ -3874,28 +3868,28 @@
       </c>
       <c r="K41" s="23"/>
     </row>
-    <row r="42" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="18">
         <f>1+A41</f>
         <v>7</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>286</v>
+        <v>278</v>
       </c>
       <c r="C42" s="19" t="s">
-        <v>248</v>
+        <v>240</v>
       </c>
       <c r="D42" s="19" t="s">
-        <v>247</v>
+        <v>239</v>
       </c>
       <c r="E42" s="19" t="s">
         <v>18</v>
       </c>
       <c r="F42" s="19" t="s">
-        <v>249</v>
+        <v>241</v>
       </c>
       <c r="G42" s="10" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="H42" s="20">
         <v>1.26</v>
@@ -3909,7 +3903,7 @@
       </c>
       <c r="K42" s="23"/>
     </row>
-    <row r="43" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="30">
         <f>1+A42</f>
         <v>8</v>
@@ -3918,16 +3912,16 @@
         <v>132</v>
       </c>
       <c r="C43" s="31" t="s">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="D43" s="31" t="s">
-        <v>250</v>
+        <v>242</v>
       </c>
       <c r="E43" s="31" t="s">
         <v>18</v>
       </c>
       <c r="F43" s="31" t="s">
-        <v>252</v>
+        <v>244</v>
       </c>
       <c r="G43" s="31"/>
       <c r="H43" s="32">
@@ -3941,7 +3935,7 @@
         <v>0</v>
       </c>
       <c r="K43" s="34" t="s">
-        <v>295</v>
+        <v>287</v>
       </c>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
@@ -3978,7 +3972,7 @@
       </c>
       <c r="K45" s="9"/>
     </row>
-    <row r="46" spans="1:11" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" s="50" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A46" s="30">
         <v>1</v>
       </c>
@@ -3998,7 +3992,7 @@
         <v>19</v>
       </c>
       <c r="G46" s="35" t="s">
-        <v>246</v>
+        <v>238</v>
       </c>
       <c r="H46" s="37">
         <v>0.49</v>
@@ -4011,10 +4005,10 @@
         <v>0</v>
       </c>
       <c r="K46" s="34" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="47" spans="1:11" s="51" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" s="50" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="15">
         <f>1+A46</f>
         <v>2</v>
@@ -4035,7 +4029,7 @@
         <v>20</v>
       </c>
       <c r="G47" s="6" t="s">
-        <v>296</v>
+        <v>288</v>
       </c>
       <c r="H47" s="8">
         <v>0.69</v>
@@ -4049,7 +4043,7 @@
       </c>
       <c r="K47" s="23"/>
     </row>
-    <row r="48" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="15">
         <f>1+A47</f>
         <v>3</v>
@@ -4070,7 +4064,7 @@
         <v>23</v>
       </c>
       <c r="G48" s="10" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="H48" s="14">
         <v>1.89</v>
@@ -4084,7 +4078,7 @@
       </c>
       <c r="K48" s="23"/>
     </row>
-    <row r="49" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A49" s="15">
         <f t="shared" ref="A49:A56" si="3">1+A48</f>
         <v>4</v>
@@ -4105,7 +4099,7 @@
         <v>26</v>
       </c>
       <c r="G49" s="6" t="s">
-        <v>287</v>
+        <v>279</v>
       </c>
       <c r="H49" s="8">
         <v>0.51</v>
@@ -4119,7 +4113,7 @@
       </c>
       <c r="K49" s="23"/>
     </row>
-    <row r="50" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="15">
         <f t="shared" si="3"/>
         <v>5</v>
@@ -4131,7 +4125,7 @@
         <v>143</v>
       </c>
       <c r="D50" s="12" t="s">
-        <v>301</v>
+        <v>293</v>
       </c>
       <c r="E50" s="10" t="s">
         <v>18</v>
@@ -4140,7 +4134,7 @@
         <v>30</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>302</v>
+        <v>294</v>
       </c>
       <c r="H50" s="14">
         <v>0.46</v>
@@ -4154,7 +4148,7 @@
       </c>
       <c r="K50" s="23"/>
     </row>
-    <row r="51" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="15">
         <f t="shared" si="3"/>
         <v>6</v>
@@ -4175,7 +4169,7 @@
         <v>81</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>288</v>
+        <v>280</v>
       </c>
       <c r="H51" s="14">
         <v>0.47</v>
@@ -4189,7 +4183,7 @@
       </c>
       <c r="K51" s="12"/>
     </row>
-    <row r="52" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="15">
         <f t="shared" si="3"/>
         <v>7</v>
@@ -4210,7 +4204,7 @@
         <v>78</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="H52" s="14">
         <v>0.95</v>
@@ -4224,7 +4218,7 @@
       </c>
       <c r="K52" s="9"/>
     </row>
-    <row r="53" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="15">
         <f t="shared" si="3"/>
         <v>8</v>
@@ -4259,7 +4253,7 @@
       </c>
       <c r="K53" s="12"/>
     </row>
-    <row r="54" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="15">
         <f t="shared" si="3"/>
         <v>9</v>
@@ -4294,7 +4288,7 @@
       </c>
       <c r="K54" s="12"/>
     </row>
-    <row r="55" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="15">
         <f t="shared" si="3"/>
         <v>10</v>
@@ -4329,7 +4323,7 @@
       </c>
       <c r="K55" s="12"/>
     </row>
-    <row r="56" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="15">
         <f t="shared" si="3"/>
         <v>11</v>
@@ -4350,7 +4344,7 @@
         <v>64</v>
       </c>
       <c r="G56" s="10" t="s">
-        <v>299</v>
+        <v>291</v>
       </c>
       <c r="H56" s="14">
         <v>1.5</v>
@@ -4364,7 +4358,7 @@
       </c>
       <c r="K56" s="12"/>
     </row>
-    <row r="57" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="30">
         <f>1+A56</f>
         <v>12</v>
@@ -4398,10 +4392,10 @@
         <v>0</v>
       </c>
       <c r="K57" s="34" t="s">
-        <v>291</v>
-      </c>
-    </row>
-    <row r="58" spans="1:11" s="51" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" s="50" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A58" s="15">
         <f t="shared" ref="A58:A63" si="4">1+A57</f>
         <v>13</v>
@@ -4422,7 +4416,7 @@
         <v>176</v>
       </c>
       <c r="G58" s="10" t="s">
-        <v>292</v>
+        <v>284</v>
       </c>
       <c r="H58" s="14">
         <v>1</v>
@@ -4436,7 +4430,7 @@
       </c>
       <c r="K58" s="12"/>
     </row>
-    <row r="59" spans="1:11" s="51" customFormat="1" ht="24" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" s="50" customFormat="1" ht="24" x14ac:dyDescent="0.25">
       <c r="A59" s="15">
         <f t="shared" si="4"/>
         <v>14</v>
@@ -4457,7 +4451,7 @@
         <v>174</v>
       </c>
       <c r="G59" s="10" t="s">
-        <v>290</v>
+        <v>282</v>
       </c>
       <c r="H59" s="14">
         <v>0.38</v>
@@ -4471,7 +4465,7 @@
       </c>
       <c r="K59" s="12"/>
     </row>
-    <row r="60" spans="1:11" s="51" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" s="50" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A60" s="15">
         <f t="shared" si="4"/>
         <v>15</v>
@@ -4492,7 +4486,7 @@
         <v>173</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>289</v>
+        <v>281</v>
       </c>
       <c r="H60" s="14">
         <v>0.56999999999999995</v>
@@ -4506,7 +4500,7 @@
       </c>
       <c r="K60" s="12"/>
     </row>
-    <row r="61" spans="1:11" s="51" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:11" s="50" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="18">
         <f>1+A60</f>
         <v>16</v>
@@ -4515,19 +4509,19 @@
         <v>201</v>
       </c>
       <c r="C61" s="19" t="s">
-        <v>240</v>
+        <v>232</v>
       </c>
       <c r="D61" s="19" t="s">
-        <v>238</v>
+        <v>230</v>
       </c>
       <c r="E61" s="19" t="s">
         <v>18</v>
       </c>
       <c r="F61" s="19" t="s">
-        <v>239</v>
+        <v>231</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>259</v>
+        <v>251</v>
       </c>
       <c r="H61" s="20">
         <v>0.49</v>
@@ -4541,7 +4535,7 @@
       </c>
       <c r="K61" s="23"/>
     </row>
-    <row r="62" spans="1:11" s="51" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:11" s="50" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A62" s="18">
         <f>1+A61</f>
         <v>17</v>
@@ -4562,7 +4556,7 @@
         <v>177</v>
       </c>
       <c r="G62" s="10" t="s">
-        <v>293</v>
+        <v>285</v>
       </c>
       <c r="H62" s="14">
         <v>0.3</v>
@@ -4576,7 +4570,7 @@
       </c>
       <c r="K62" s="12"/>
     </row>
-    <row r="63" spans="1:11" s="51" customFormat="1" ht="36" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:11" s="50" customFormat="1" ht="36" x14ac:dyDescent="0.25">
       <c r="A63" s="15">
         <f t="shared" si="4"/>
         <v>18</v>
@@ -4597,7 +4591,7 @@
         <v>178</v>
       </c>
       <c r="G63" s="10" t="s">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="H63" s="14">
         <v>0.34</v>
@@ -4611,95 +4605,91 @@
       </c>
       <c r="K63" s="12"/>
     </row>
-    <row r="64" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="38">
+    <row r="64" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="18">
         <f>1+A63</f>
         <v>19</v>
       </c>
-      <c r="B64" s="39" t="s">
-        <v>223</v>
-      </c>
-      <c r="C64" s="39" t="s">
-        <v>224</v>
-      </c>
-      <c r="D64" s="39" t="s">
-        <v>225</v>
-      </c>
-      <c r="E64" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F64" s="39" t="s">
-        <v>222</v>
-      </c>
-      <c r="G64" s="39"/>
-      <c r="H64" s="40">
-        <v>0.48</v>
-      </c>
-      <c r="I64" s="41">
-        <v>0</v>
-      </c>
-      <c r="J64" s="40">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
-      </c>
-      <c r="K64" s="42" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="65" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="38">
+      <c r="B64" s="19" t="s">
+        <v>219</v>
+      </c>
+      <c r="C64" s="19" t="s">
+        <v>363</v>
+      </c>
+      <c r="D64" s="19" t="s">
+        <v>364</v>
+      </c>
+      <c r="E64" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="19" t="s">
+        <v>365</v>
+      </c>
+      <c r="G64" s="19"/>
+      <c r="H64" s="20">
+        <v>4.41</v>
+      </c>
+      <c r="I64" s="27">
+        <v>2</v>
+      </c>
+      <c r="J64" s="20">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>8.82</v>
+      </c>
+      <c r="K64" s="23"/>
+    </row>
+    <row r="65" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="18">
         <f>1+A64</f>
         <v>20</v>
       </c>
-      <c r="B65" s="39" t="s">
-        <v>223</v>
-      </c>
-      <c r="C65" s="39" t="s">
-        <v>228</v>
-      </c>
-      <c r="D65" s="39" t="s">
-        <v>227</v>
-      </c>
-      <c r="E65" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="F65" s="39" t="s">
-        <v>226</v>
-      </c>
-      <c r="G65" s="39"/>
-      <c r="H65" s="40">
-        <v>4</v>
-      </c>
-      <c r="I65" s="41">
-        <v>0</v>
-      </c>
-      <c r="J65" s="40">
-        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
-        <v>0</v>
-      </c>
-      <c r="K65" s="42" t="s">
-        <v>295</v>
-      </c>
-    </row>
-    <row r="66" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="19" t="s">
+        <v>367</v>
+      </c>
+      <c r="C65" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="D65" s="19" t="s">
+        <v>366</v>
+      </c>
+      <c r="E65" s="19" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" s="19" t="s">
+        <v>369</v>
+      </c>
+      <c r="G65" s="19"/>
+      <c r="H65" s="20">
+        <v>3.08</v>
+      </c>
+      <c r="I65" s="27">
+        <v>2</v>
+      </c>
+      <c r="J65" s="20">
+        <f>Table2[[#This Row],[Price]]*Table2[[#This Row],[Qty]]</f>
+        <v>6.16</v>
+      </c>
+      <c r="K65" s="23"/>
+    </row>
+    <row r="66" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="18">
         <f>1+A65</f>
         <v>21</v>
       </c>
       <c r="B66" s="19" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="C66" s="19" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>234</v>
+        <v>226</v>
       </c>
       <c r="E66" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F66" s="19" t="s">
-        <v>235</v>
+        <v>227</v>
       </c>
       <c r="G66" s="19"/>
       <c r="H66" s="20">
@@ -4713,28 +4703,28 @@
         <v>11.7</v>
       </c>
       <c r="K66" s="12" t="s">
-        <v>318</v>
-      </c>
-    </row>
-    <row r="67" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="67" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="15">
         <f>1+A66</f>
         <v>22</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>236</v>
+        <v>228</v>
       </c>
       <c r="E67" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F67" s="10" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="G67" s="10"/>
       <c r="H67" s="14">
@@ -4783,7 +4773,7 @@
       </c>
       <c r="K69" s="26"/>
     </row>
-    <row r="70" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="38">
         <f>1</f>
         <v>1</v>
@@ -4795,7 +4785,7 @@
         <v>155</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="E70" s="31" t="s">
         <v>68</v>
@@ -4815,10 +4805,10 @@
         <v>0</v>
       </c>
       <c r="K70" s="34" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="71" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="18">
         <f t="shared" ref="A71:A81" si="5">1+A70</f>
         <v>2</v>
@@ -4850,10 +4840,10 @@
         <v>6.24</v>
       </c>
       <c r="K71" s="12" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="72" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="18">
         <f t="shared" si="5"/>
         <v>3</v>
@@ -4886,7 +4876,7 @@
       </c>
       <c r="K72" s="23"/>
     </row>
-    <row r="73" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="18">
         <f t="shared" si="5"/>
         <v>4</v>
@@ -4895,7 +4885,7 @@
         <v>219</v>
       </c>
       <c r="C73" s="19" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="D73" s="19" t="s">
         <v>72</v>
@@ -4904,7 +4894,7 @@
         <v>18</v>
       </c>
       <c r="F73" s="19" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="G73" s="19"/>
       <c r="H73" s="20">
@@ -4919,7 +4909,7 @@
       </c>
       <c r="K73" s="23"/>
     </row>
-    <row r="74" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="15">
         <f t="shared" ref="A74:A79" si="6">1+A73</f>
         <v>5</v>
@@ -4928,16 +4918,16 @@
         <v>146</v>
       </c>
       <c r="C74" s="10" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="D74" s="10" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="E74" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F74" s="10" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="G74" s="10"/>
       <c r="H74" s="14">
@@ -4952,7 +4942,7 @@
       </c>
       <c r="K74" s="12"/>
     </row>
-    <row r="75" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A75" s="15">
         <f t="shared" si="6"/>
         <v>6</v>
@@ -4961,16 +4951,16 @@
         <v>146</v>
       </c>
       <c r="C75" s="10" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="D75" s="10" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="E75" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="G75" s="10"/>
       <c r="H75" s="14">
@@ -4985,25 +4975,25 @@
       </c>
       <c r="K75" s="12"/>
     </row>
-    <row r="76" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A76" s="18">
         <f t="shared" si="6"/>
         <v>7</v>
       </c>
       <c r="B76" s="19" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C76" s="19" t="s">
-        <v>361</v>
+        <v>353</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="E76" s="10" t="s">
         <v>68</v>
       </c>
       <c r="F76" s="19" t="s">
-        <v>368</v>
+        <v>360</v>
       </c>
       <c r="G76" s="19"/>
       <c r="H76" s="20">
@@ -5018,25 +5008,25 @@
       </c>
       <c r="K76" s="23"/>
     </row>
-    <row r="77" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A77" s="18">
         <f t="shared" si="6"/>
         <v>8</v>
       </c>
       <c r="B77" s="19" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C77" s="19" t="s">
-        <v>363</v>
+        <v>355</v>
       </c>
       <c r="D77" s="19" t="s">
-        <v>366</v>
+        <v>358</v>
       </c>
       <c r="E77" s="19" t="s">
         <v>68</v>
       </c>
       <c r="F77" s="19" t="s">
-        <v>369</v>
+        <v>361</v>
       </c>
       <c r="G77" s="19"/>
       <c r="H77" s="20">
@@ -5050,28 +5040,28 @@
         <v>13.54</v>
       </c>
       <c r="K77" s="23" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="78" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="78" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="18">
         <f t="shared" si="6"/>
         <v>9</v>
       </c>
       <c r="B78" s="19" t="s">
-        <v>360</v>
+        <v>352</v>
       </c>
       <c r="C78" s="19" t="s">
-        <v>362</v>
+        <v>354</v>
       </c>
       <c r="D78" s="19" t="s">
-        <v>367</v>
+        <v>359</v>
       </c>
       <c r="E78" s="19" t="s">
         <v>68</v>
       </c>
       <c r="F78" s="19" t="s">
-        <v>370</v>
+        <v>362</v>
       </c>
       <c r="G78" s="19"/>
       <c r="H78" s="20">
@@ -5085,10 +5075,10 @@
         <v>4.42</v>
       </c>
       <c r="K78" s="23" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="79" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="79" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="18">
         <f t="shared" si="6"/>
         <v>10</v>
@@ -5121,7 +5111,7 @@
       </c>
       <c r="K79" s="23"/>
     </row>
-    <row r="80" spans="1:11" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:11" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A80" s="18">
         <f t="shared" si="5"/>
         <v>11</v>
@@ -5154,7 +5144,7 @@
       </c>
       <c r="K80" s="23"/>
     </row>
-    <row r="81" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="38">
         <f t="shared" si="5"/>
         <v>12</v>
@@ -5186,10 +5176,10 @@
         <v>0</v>
       </c>
       <c r="K81" s="34" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="82" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="18">
         <f t="shared" ref="A82:A86" si="7">1+A81</f>
         <v>13</v>
@@ -5221,10 +5211,10 @@
         <v>2.35</v>
       </c>
       <c r="K82" s="12" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="38">
         <f t="shared" si="7"/>
         <v>14</v>
@@ -5256,19 +5246,19 @@
         <v>0</v>
       </c>
       <c r="K83" s="34" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="18">
         <f t="shared" si="7"/>
         <v>15</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="C84" s="19" t="s">
-        <v>232</v>
+        <v>224</v>
       </c>
       <c r="D84" s="19" t="s">
         <v>88</v>
@@ -5277,10 +5267,10 @@
         <v>68</v>
       </c>
       <c r="F84" s="19" t="s">
-        <v>233</v>
+        <v>225</v>
       </c>
       <c r="G84" s="19" t="s">
-        <v>297</v>
+        <v>289</v>
       </c>
       <c r="H84" s="20">
         <v>0.12</v>
@@ -5294,7 +5284,7 @@
       </c>
       <c r="K84" s="23"/>
     </row>
-    <row r="85" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="15">
         <f t="shared" si="7"/>
         <v>16</v>
@@ -5326,9 +5316,9 @@
         <v>4.72</v>
       </c>
       <c r="K85" s="12"/>
-      <c r="M85" s="52"/>
-    </row>
-    <row r="86" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M85" s="51"/>
+    </row>
+    <row r="86" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="15">
         <f t="shared" si="7"/>
         <v>17</v>
@@ -5360,31 +5350,31 @@
         <v>2.13</v>
       </c>
       <c r="K86" s="12" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="18">
         <f t="shared" ref="A87:A94" si="8">1+A86</f>
         <v>18</v>
       </c>
       <c r="B87" s="19" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="C87" s="19">
         <v>1935187</v>
       </c>
       <c r="D87" s="10" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="E87" s="10" t="s">
         <v>18</v>
       </c>
       <c r="F87" s="19" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="G87" s="10" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="H87" s="20">
         <v>0.64</v>
@@ -5398,25 +5388,25 @@
       </c>
       <c r="K87" s="23"/>
     </row>
-    <row r="88" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="18">
         <f>1+A87</f>
         <v>19</v>
       </c>
       <c r="B88" s="19" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="C88" s="19">
         <v>7200</v>
       </c>
       <c r="D88" s="19" t="s">
-        <v>358</v>
+        <v>350</v>
       </c>
       <c r="E88" s="19" t="s">
         <v>18</v>
       </c>
       <c r="F88" s="19" t="s">
-        <v>359</v>
+        <v>351</v>
       </c>
       <c r="G88" s="19"/>
       <c r="H88" s="20">
@@ -5431,25 +5421,25 @@
       </c>
       <c r="K88" s="23"/>
     </row>
-    <row r="89" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A89" s="15">
         <f>1+A88</f>
         <v>20</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="E89" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="G89" s="1"/>
       <c r="H89" s="2">
@@ -5464,25 +5454,25 @@
       </c>
       <c r="K89" s="12"/>
     </row>
-    <row r="90" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="15">
         <f t="shared" si="8"/>
         <v>21</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>352</v>
+        <v>344</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="E90" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>347</v>
+        <v>339</v>
       </c>
       <c r="G90" s="1"/>
       <c r="H90" s="2">
@@ -5497,25 +5487,25 @@
       </c>
       <c r="K90" s="12"/>
     </row>
-    <row r="91" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="15">
         <f t="shared" si="8"/>
         <v>22</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>353</v>
+        <v>345</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="E91" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="G91" s="1"/>
       <c r="H91" s="2">
@@ -5530,25 +5520,25 @@
       </c>
       <c r="K91" s="12"/>
     </row>
-    <row r="92" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A92" s="15">
         <f t="shared" si="8"/>
         <v>23</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="E92" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>349</v>
+        <v>341</v>
       </c>
       <c r="G92" s="1"/>
       <c r="H92" s="2">
@@ -5563,25 +5553,25 @@
       </c>
       <c r="K92" s="12"/>
     </row>
-    <row r="93" spans="1:13" s="51" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:13" s="50" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A93" s="15">
         <f t="shared" si="8"/>
         <v>24</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>345</v>
+        <v>337</v>
       </c>
       <c r="E93" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>350</v>
+        <v>342</v>
       </c>
       <c r="G93" s="1"/>
       <c r="H93" s="2">
@@ -5602,19 +5592,19 @@
         <v>25</v>
       </c>
       <c r="B94" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="D94" s="1" t="s">
         <v>338</v>
       </c>
-      <c r="C94" s="1" t="s">
-        <v>356</v>
-      </c>
-      <c r="D94" s="1" t="s">
-        <v>346</v>
-      </c>
       <c r="E94" s="1" t="s">
         <v>18</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>351</v>
+        <v>343</v>
       </c>
       <c r="G94" s="1"/>
       <c r="H94" s="2">
@@ -5630,13 +5620,10 @@
       <c r="K94" s="4"/>
     </row>
     <row r="95" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C95" s="53"/>
+      <c r="C95" s="52"/>
     </row>
     <row r="96" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A96" s="53"/>
-      <c r="D96" s="43" t="s">
-        <v>221</v>
-      </c>
+      <c r="A96" s="52"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>